<commit_message>
Fixed checks for "key lengths". Added the CHECK_ONLY_FIRST condition that makes it possible to improve BSI "key lengths" compliance checks by having checks for 3000+ lengths.
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -688,7 +688,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="547">
   <si>
     <t>NIST</t>
   </si>
@@ -1935,7 +1935,7 @@
     <t>YEAR 2023</t>
   </si>
   <si>
-    <t>2028+</t>
+    <t>YEAR 2028+</t>
   </si>
   <si>
     <t>rsa_pkcs1_sha384</t>
@@ -2157,13 +2157,16 @@
     <t>YEAR 2031+</t>
   </si>
   <si>
-    <t>YEAR 2029+</t>
+    <t>YEAR 2029+ and CHECK_ONLY_FIRST 2</t>
   </si>
   <si>
     <t>DSS</t>
   </si>
   <si>
-    <t>YEAR 2022</t>
+    <t>YEAR 2022 and CHECK_ONLY_FIRST 1</t>
+  </si>
+  <si>
+    <t>YEAR 2029+ and CHECK_ONLY_FIRST 1</t>
   </si>
   <si>
     <t>Static and ephemeral Diffie-Hellman keys</t>
@@ -2654,7 +2657,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="161">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2911,6 +2914,9 @@
     <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2997,8 +3003,14 @@
     <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
@@ -4809,14 +4821,14 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="133"/>
-      <c r="B1" s="134" t="s">
+      <c r="A1" s="136"/>
+      <c r="B1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="134" t="s">
+      <c r="C1" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="156" t="s">
+      <c r="D1" s="159" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
@@ -4825,16 +4837,16 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
+        <v>543</v>
+      </c>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
       <c r="E2" s="9"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="78" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>14</v>
@@ -4849,13 +4861,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="78" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -16906,10 +16918,10 @@
       <c r="G3" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I3" s="98" t="s">
+      <c r="I3" s="99" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="61" t="s">
@@ -16944,10 +16956,10 @@
       <c r="G4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="I4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="61" t="s">
@@ -16982,10 +16994,10 @@
       <c r="G5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I5" s="98" t="s">
+      <c r="I5" s="99" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="61" t="s">
@@ -17008,20 +17020,20 @@
       <c r="C6" s="28">
         <v>1.3</v>
       </c>
-      <c r="D6" s="99" t="s">
+      <c r="D6" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="99"/>
+      <c r="E6" s="100"/>
       <c r="F6" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="I6" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="61" t="s">
@@ -17044,20 +17056,20 @@
       <c r="C7" s="28">
         <v>1.3</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="99"/>
+      <c r="E7" s="100"/>
       <c r="F7" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I7" s="98" t="s">
+      <c r="I7" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="61" t="s">
@@ -17080,20 +17092,20 @@
       <c r="C8" s="28">
         <v>1.3</v>
       </c>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="99"/>
+      <c r="E8" s="100"/>
       <c r="F8" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I8" s="98" t="s">
+      <c r="I8" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="61" t="s">
@@ -17116,20 +17128,20 @@
       <c r="C9" s="28">
         <v>1.3</v>
       </c>
-      <c r="D9" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="99"/>
+      <c r="D9" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="100"/>
       <c r="F9" s="31" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I9" s="98" t="s">
+      <c r="I9" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="61" t="s">
@@ -17152,20 +17164,20 @@
       <c r="C10" s="28">
         <v>1.3</v>
       </c>
-      <c r="D10" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="99"/>
+      <c r="D10" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="100"/>
       <c r="F10" s="31" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I10" s="98" t="s">
+      <c r="I10" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="61" t="s">
@@ -17188,20 +17200,20 @@
       <c r="C11" s="28">
         <v>1.3</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="99"/>
+      <c r="E11" s="100"/>
       <c r="F11" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I11" s="98" t="s">
+      <c r="I11" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="61" t="s">
@@ -17224,20 +17236,20 @@
       <c r="C12" s="28">
         <v>1.3</v>
       </c>
-      <c r="D12" s="99" t="s">
+      <c r="D12" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="99"/>
+      <c r="E12" s="100"/>
       <c r="F12" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I12" s="98" t="s">
+      <c r="I12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="61" t="s">
@@ -17260,20 +17272,20 @@
       <c r="C13" s="28">
         <v>1.3</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="99"/>
+      <c r="E13" s="100"/>
       <c r="F13" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I13" s="98" t="s">
+      <c r="I13" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="61" t="s">
@@ -17296,20 +17308,20 @@
       <c r="C14" s="28">
         <v>1.3</v>
       </c>
-      <c r="D14" s="99" t="s">
+      <c r="D14" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="99"/>
+      <c r="E14" s="100"/>
       <c r="F14" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I14" s="98" t="s">
+      <c r="I14" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="61" t="s">
@@ -17332,20 +17344,20 @@
       <c r="C15" s="28">
         <v>1.3</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="99"/>
+      <c r="E15" s="100"/>
       <c r="F15" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I15" s="98" t="s">
+      <c r="I15" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="61" t="s">
@@ -17368,20 +17380,20 @@
       <c r="C16" s="28">
         <v>1.3</v>
       </c>
-      <c r="D16" s="99" t="s">
+      <c r="D16" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="99"/>
+      <c r="E16" s="100"/>
       <c r="F16" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I16" s="98" t="s">
+      <c r="I16" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J16" s="61" t="s">
@@ -17404,20 +17416,20 @@
       <c r="C17" s="28">
         <v>1.3</v>
       </c>
-      <c r="D17" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="99"/>
+      <c r="D17" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="100"/>
       <c r="F17" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I17" s="98" t="s">
+      <c r="I17" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="61" t="s">
@@ -17440,20 +17452,20 @@
       <c r="C18" s="28">
         <v>1.3</v>
       </c>
-      <c r="D18" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="99"/>
+      <c r="D18" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="100"/>
       <c r="F18" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I18" s="98" t="s">
+      <c r="I18" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J18" s="61" t="s">
@@ -17476,20 +17488,20 @@
       <c r="C19" s="28">
         <v>1.3</v>
       </c>
-      <c r="D19" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="99"/>
+      <c r="D19" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="100"/>
       <c r="F19" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="I19" s="98" t="s">
+      <c r="I19" s="99" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="61" t="s">
@@ -21510,7 +21522,7 @@
       <c r="C1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="101" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="73"/>
@@ -21533,7 +21545,7 @@
       <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="101"/>
+      <c r="H2" s="102"/>
       <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
@@ -21545,16 +21557,16 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="103" t="s">
         <v>450</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="103" t="s">
         <v>451</v>
       </c>
       <c r="C3" s="47">
         <v>112.0</v>
       </c>
-      <c r="D3" s="103" t="s">
+      <c r="D3" s="104" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="79"/>
@@ -21564,16 +21576,16 @@
       <c r="G3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="104" t="s">
+      <c r="H3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="105" t="s">
+      <c r="I3" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="106" t="s">
+      <c r="J3" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="106" t="s">
+      <c r="K3" s="107" t="s">
         <v>15</v>
       </c>
     </row>
@@ -21587,10 +21599,10 @@
       <c r="C4" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="109" t="s">
         <v>454</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -21599,7 +21611,7 @@
       <c r="G4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="109" t="s">
+      <c r="H4" s="110" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -21622,10 +21634,10 @@
       <c r="C5" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="108" t="s">
+      <c r="E5" s="109" t="s">
         <v>457</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -21634,7 +21646,7 @@
       <c r="G5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="109" t="s">
+      <c r="H5" s="110" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -21657,17 +21669,17 @@
       <c r="C6" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="D6" s="107" t="s">
+      <c r="D6" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="110"/>
+      <c r="E6" s="111"/>
       <c r="F6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="110" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -21690,17 +21702,17 @@
       <c r="C7" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="D7" s="107" t="s">
+      <c r="D7" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="110"/>
+      <c r="E7" s="111"/>
       <c r="F7" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -21723,17 +21735,17 @@
       <c r="C8" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="110"/>
+      <c r="E8" s="111"/>
       <c r="F8" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="109" t="s">
+      <c r="H8" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -21756,17 +21768,17 @@
       <c r="C9" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="D9" s="107" t="s">
+      <c r="D9" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="110"/>
+      <c r="E9" s="111"/>
       <c r="F9" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="H9" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -21789,17 +21801,17 @@
       <c r="C10" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="110"/>
+      <c r="E10" s="111"/>
       <c r="F10" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="109" t="s">
+      <c r="H10" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -21822,17 +21834,17 @@
       <c r="C11" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="D11" s="107" t="s">
+      <c r="D11" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="110"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="109" t="s">
+      <c r="H11" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -21855,17 +21867,17 @@
       <c r="C12" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="D12" s="107" t="s">
+      <c r="D12" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="110"/>
+      <c r="E12" s="111"/>
       <c r="F12" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="109" t="s">
+      <c r="H12" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="5" t="s">
@@ -21888,17 +21900,17 @@
       <c r="C13" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="110"/>
+      <c r="E13" s="111"/>
       <c r="F13" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="109" t="s">
+      <c r="H13" s="110" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -21921,34 +21933,34 @@
       <c r="C14" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="D14" s="111" t="s">
+      <c r="D14" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="112"/>
+      <c r="E14" s="113"/>
       <c r="F14" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="109" t="s">
+      <c r="H14" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="113" t="s">
+      <c r="I14" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="114" t="s">
+      <c r="J14" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="114" t="s">
+      <c r="K14" s="115" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="102" t="s">
+      <c r="A15" s="103" t="s">
         <v>468</v>
       </c>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="103" t="s">
         <v>451</v>
       </c>
       <c r="C15" s="47" t="s">
@@ -21957,14 +21969,14 @@
       <c r="D15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="110"/>
+      <c r="E15" s="111"/>
       <c r="F15" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="104" t="s">
+      <c r="H15" s="105" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -21990,14 +22002,14 @@
       <c r="D16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="110"/>
+      <c r="E16" s="111"/>
       <c r="F16" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="109" t="s">
+      <c r="H16" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="5" t="s">
@@ -22023,14 +22035,14 @@
       <c r="D17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="110"/>
+      <c r="E17" s="111"/>
       <c r="F17" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="109" t="s">
+      <c r="H17" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I17" s="5" t="s">
@@ -22056,14 +22068,14 @@
       <c r="D18" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="110"/>
+      <c r="E18" s="111"/>
       <c r="F18" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="109" t="s">
+      <c r="H18" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -22089,14 +22101,14 @@
       <c r="D19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="110"/>
+      <c r="E19" s="111"/>
       <c r="F19" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="109" t="s">
+      <c r="H19" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I19" s="5" t="s">
@@ -22122,14 +22134,14 @@
       <c r="D20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="110"/>
+      <c r="E20" s="111"/>
       <c r="F20" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="109" t="s">
+      <c r="H20" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -22153,14 +22165,14 @@
       <c r="D21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="110"/>
+      <c r="E21" s="111"/>
       <c r="F21" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="109" t="s">
+      <c r="H21" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I21" s="5" t="s">
@@ -22184,14 +22196,14 @@
       <c r="D22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="110"/>
+      <c r="E22" s="111"/>
       <c r="F22" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="109" t="s">
+      <c r="H22" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I22" s="5" t="s">
@@ -22215,14 +22227,14 @@
       <c r="D23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="110"/>
+      <c r="E23" s="111"/>
       <c r="F23" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="109" t="s">
+      <c r="H23" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I23" s="5" t="s">
@@ -22246,14 +22258,14 @@
       <c r="D24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="110"/>
+      <c r="E24" s="111"/>
       <c r="F24" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="109" t="s">
+      <c r="H24" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="5" t="s">
@@ -22267,7 +22279,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="115" t="s">
+      <c r="A25" s="116" t="s">
         <v>481</v>
       </c>
       <c r="B25" s="78">
@@ -22277,14 +22289,14 @@
       <c r="D25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="110"/>
+      <c r="E25" s="111"/>
       <c r="F25" s="48" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="109" t="s">
+      <c r="H25" s="110" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="5" t="s">
@@ -23353,26 +23365,26 @@
       <c r="B1" s="71" t="s">
         <v>483</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="117" t="s">
         <v>484</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="119" t="s">
+      <c r="E1" s="119"/>
+      <c r="F1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="120"/>
-      <c r="H1" s="121" t="s">
+      <c r="G1" s="121"/>
+      <c r="H1" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122" t="s">
+      <c r="I1" s="123"/>
+      <c r="J1" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="74"/>
@@ -23399,7 +23411,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="125" t="s">
         <v>486</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -23408,16 +23420,16 @@
       <c r="C3" s="78">
         <v>224.0</v>
       </c>
-      <c r="D3" s="125" t="s">
+      <c r="D3" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="126" t="s">
+      <c r="E3" s="127" t="s">
         <v>487</v>
       </c>
-      <c r="F3" s="127" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="128"/>
+      <c r="F3" s="128" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="129"/>
       <c r="H3" s="32" t="s">
         <v>16</v>
       </c>
@@ -23436,22 +23448,22 @@
       <c r="C4" s="78">
         <v>256.0</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="126" t="s">
+      <c r="E4" s="127" t="s">
         <v>488</v>
       </c>
-      <c r="F4" s="129" t="s">
+      <c r="F4" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="126" t="s">
+      <c r="G4" s="131" t="s">
         <v>489</v>
       </c>
-      <c r="H4" s="130" t="s">
+      <c r="H4" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="130" t="s">
+      <c r="I4" s="132" t="s">
         <v>487</v>
       </c>
       <c r="J4" s="36" t="s">
@@ -23471,16 +23483,16 @@
       <c r="C5" s="78">
         <v>2048.0</v>
       </c>
-      <c r="D5" s="125" t="s">
+      <c r="D5" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="127" t="s">
         <v>487</v>
       </c>
-      <c r="F5" s="129" t="s">
+      <c r="F5" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="128" t="s">
+      <c r="G5" s="133" t="s">
         <v>491</v>
       </c>
       <c r="H5" s="32" t="s">
@@ -23501,17 +23513,17 @@
       <c r="C6" s="78">
         <v>3076.0</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="126" t="s">
+      <c r="E6" s="127" t="s">
         <v>488</v>
       </c>
-      <c r="F6" s="129" t="s">
+      <c r="F6" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="128" t="s">
-        <v>489</v>
+      <c r="G6" s="133" t="s">
+        <v>492</v>
       </c>
       <c r="H6" s="32" t="s">
         <v>16</v>
@@ -23534,22 +23546,22 @@
       <c r="C7" s="78">
         <v>2048.0</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="127" t="s">
         <v>487</v>
       </c>
-      <c r="F7" s="129" t="s">
+      <c r="F7" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="126" t="s">
+      <c r="G7" s="131" t="s">
         <v>491</v>
       </c>
-      <c r="H7" s="130" t="s">
+      <c r="H7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="131" t="s">
+      <c r="I7" s="134" t="s">
         <v>487</v>
       </c>
       <c r="J7" s="36" t="s">
@@ -23566,17 +23578,17 @@
       <c r="C8" s="78">
         <v>3076.0</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="126" t="s">
+      <c r="E8" s="127" t="s">
         <v>488</v>
       </c>
-      <c r="F8" s="129" t="s">
+      <c r="F8" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="128" t="s">
-        <v>489</v>
+      <c r="G8" s="133" t="s">
+        <v>492</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>16</v>
@@ -23596,14 +23608,14 @@
       <c r="C9" s="78">
         <v>1024.0</v>
       </c>
-      <c r="D9" s="128" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="126"/>
-      <c r="F9" s="132" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="128"/>
+      <c r="D9" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="127"/>
+      <c r="F9" s="135" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="129"/>
       <c r="H9" s="32" t="s">
         <v>16</v>
       </c>
@@ -23619,23 +23631,23 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="124" t="s">
-        <v>492</v>
+      <c r="A10" s="125" t="s">
+        <v>493</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C10" s="78">
         <v>224.0</v>
       </c>
-      <c r="D10" s="128" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="126"/>
-      <c r="F10" s="127" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="128"/>
+      <c r="D10" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="127"/>
+      <c r="F10" s="128" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="129"/>
       <c r="H10" s="32" t="s">
         <v>16</v>
       </c>
@@ -23654,14 +23666,14 @@
       <c r="C11" s="78">
         <v>256.0</v>
       </c>
-      <c r="D11" s="128" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="126"/>
-      <c r="F11" s="129" t="s">
+      <c r="D11" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="127"/>
+      <c r="F11" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="128" t="s">
+      <c r="G11" s="133" t="s">
         <v>489</v>
       </c>
       <c r="H11" s="32" t="s">
@@ -23680,19 +23692,19 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="B12" s="4" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C12" s="78">
         <v>2048.0</v>
       </c>
-      <c r="D12" s="128" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="126"/>
-      <c r="F12" s="129" t="s">
+      <c r="D12" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="127"/>
+      <c r="F12" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="128" t="s">
+      <c r="G12" s="133" t="s">
         <v>491</v>
       </c>
       <c r="H12" s="32" t="s">
@@ -23713,15 +23725,15 @@
       <c r="C13" s="78">
         <v>3076.0</v>
       </c>
-      <c r="D13" s="128" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="126"/>
-      <c r="F13" s="129" t="s">
+      <c r="D13" s="129" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="127"/>
+      <c r="F13" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="128" t="s">
-        <v>489</v>
+      <c r="G13" s="133" t="s">
+        <v>492</v>
       </c>
       <c r="H13" s="32" t="s">
         <v>16</v>
@@ -24799,53 +24811,53 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="133"/>
-      <c r="B1" s="134" t="s">
+      <c r="A1" s="136"/>
+      <c r="B1" s="137" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="74"/>
       <c r="D1" s="74"/>
-      <c r="E1" s="134" t="s">
+      <c r="E1" s="137" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="74"/>
       <c r="G1" s="74"/>
-      <c r="H1" s="134" t="s">
+      <c r="H1" s="137" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="78"/>
-      <c r="B2" s="135"/>
+      <c r="B2" s="138"/>
       <c r="C2" s="78" t="s">
-        <v>496</v>
-      </c>
-      <c r="D2" s="136" t="s">
         <v>497</v>
       </c>
-      <c r="E2" s="135"/>
+      <c r="D2" s="139" t="s">
+        <v>498</v>
+      </c>
+      <c r="E2" s="138"/>
       <c r="F2" s="78" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="G2" s="78" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="48"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="78" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="78"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137" t="s">
+      <c r="D3" s="139"/>
+      <c r="E3" s="140" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="78"/>
@@ -24859,14 +24871,14 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="78" t="s">
-        <v>499</v>
-      </c>
-      <c r="B4" s="135"/>
+        <v>500</v>
+      </c>
+      <c r="B4" s="138"/>
       <c r="C4" s="78"/>
-      <c r="D4" s="138" t="s">
-        <v>500</v>
-      </c>
-      <c r="E4" s="135"/>
+      <c r="D4" s="141" t="s">
+        <v>501</v>
+      </c>
+      <c r="E4" s="138"/>
       <c r="F4" s="78"/>
       <c r="G4" s="78"/>
       <c r="H4" s="10" t="s">
@@ -24878,12 +24890,12 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="78"/>
-      <c r="B5" s="135"/>
+      <c r="B5" s="138"/>
       <c r="C5" s="78"/>
-      <c r="D5" s="139" t="s">
-        <v>501</v>
-      </c>
-      <c r="E5" s="135"/>
+      <c r="D5" s="142" t="s">
+        <v>502</v>
+      </c>
+      <c r="E5" s="138"/>
       <c r="F5" s="78"/>
       <c r="G5" s="78"/>
       <c r="H5" s="10"/>
@@ -24893,12 +24905,12 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="78"/>
-      <c r="B6" s="135"/>
+      <c r="B6" s="138"/>
       <c r="C6" s="78"/>
-      <c r="D6" s="139" t="s">
-        <v>502</v>
-      </c>
-      <c r="E6" s="135"/>
+      <c r="D6" s="142" t="s">
+        <v>503</v>
+      </c>
+      <c r="E6" s="138"/>
       <c r="F6" s="78"/>
       <c r="G6" s="78"/>
       <c r="H6" s="10"/>
@@ -24908,12 +24920,12 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="78"/>
-      <c r="B7" s="135"/>
+      <c r="B7" s="138"/>
       <c r="C7" s="78"/>
-      <c r="D7" s="139" t="s">
-        <v>503</v>
-      </c>
-      <c r="E7" s="135"/>
+      <c r="D7" s="142" t="s">
+        <v>504</v>
+      </c>
+      <c r="E7" s="138"/>
       <c r="F7" s="78"/>
       <c r="G7" s="78"/>
       <c r="H7" s="10"/>
@@ -24923,14 +24935,14 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="78" t="s">
-        <v>504</v>
-      </c>
-      <c r="B8" s="135"/>
+        <v>505</v>
+      </c>
+      <c r="B8" s="138"/>
       <c r="C8" s="78"/>
-      <c r="D8" s="136" t="s">
-        <v>505</v>
-      </c>
-      <c r="E8" s="135"/>
+      <c r="D8" s="139" t="s">
+        <v>506</v>
+      </c>
+      <c r="E8" s="138"/>
       <c r="F8" s="78"/>
       <c r="G8" s="78"/>
       <c r="H8" s="10" t="s">
@@ -24942,19 +24954,19 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="78" t="s">
-        <v>506</v>
-      </c>
-      <c r="B9" s="135"/>
+        <v>507</v>
+      </c>
+      <c r="B9" s="138"/>
       <c r="C9" s="78"/>
-      <c r="D9" s="136" t="s">
-        <v>507</v>
-      </c>
-      <c r="E9" s="140" t="s">
+      <c r="D9" s="139" t="s">
         <v>508</v>
+      </c>
+      <c r="E9" s="143" t="s">
+        <v>509</v>
       </c>
       <c r="F9" s="78"/>
       <c r="G9" s="78" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>16</v>
@@ -24965,14 +24977,14 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="78" t="s">
-        <v>509</v>
-      </c>
-      <c r="B10" s="135"/>
+        <v>510</v>
+      </c>
+      <c r="B10" s="138"/>
       <c r="C10" s="78"/>
-      <c r="D10" s="136" t="s">
-        <v>510</v>
-      </c>
-      <c r="E10" s="135"/>
+      <c r="D10" s="139" t="s">
+        <v>511</v>
+      </c>
+      <c r="E10" s="138"/>
       <c r="F10" s="78"/>
       <c r="G10" s="78"/>
       <c r="H10" s="10" t="s">
@@ -24984,16 +24996,16 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="78" t="s">
-        <v>511</v>
-      </c>
-      <c r="B11" s="140" t="s">
-        <v>508</v>
+        <v>512</v>
+      </c>
+      <c r="B11" s="143" t="s">
+        <v>509</v>
       </c>
       <c r="C11" s="78"/>
-      <c r="D11" s="139" t="s">
-        <v>500</v>
-      </c>
-      <c r="E11" s="135"/>
+      <c r="D11" s="142" t="s">
+        <v>501</v>
+      </c>
+      <c r="E11" s="138"/>
       <c r="F11" s="78"/>
       <c r="G11" s="78"/>
       <c r="H11" s="10" t="s">
@@ -25005,14 +25017,14 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="78"/>
-      <c r="B12" s="140" t="s">
-        <v>508</v>
+      <c r="B12" s="143" t="s">
+        <v>509</v>
       </c>
       <c r="C12" s="78"/>
-      <c r="D12" s="139" t="s">
-        <v>501</v>
-      </c>
-      <c r="E12" s="135"/>
+      <c r="D12" s="142" t="s">
+        <v>502</v>
+      </c>
+      <c r="E12" s="138"/>
       <c r="F12" s="78"/>
       <c r="G12" s="78"/>
       <c r="H12" s="10"/>
@@ -25022,14 +25034,14 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="78"/>
-      <c r="B13" s="140" t="s">
-        <v>508</v>
+      <c r="B13" s="143" t="s">
+        <v>509</v>
       </c>
       <c r="C13" s="78"/>
-      <c r="D13" s="139" t="s">
-        <v>502</v>
-      </c>
-      <c r="E13" s="135"/>
+      <c r="D13" s="142" t="s">
+        <v>503</v>
+      </c>
+      <c r="E13" s="138"/>
       <c r="F13" s="78"/>
       <c r="G13" s="78"/>
       <c r="H13" s="10"/>
@@ -25039,14 +25051,14 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="78"/>
-      <c r="B14" s="135" t="s">
-        <v>512</v>
+      <c r="B14" s="138" t="s">
+        <v>513</v>
       </c>
       <c r="C14" s="78"/>
-      <c r="D14" s="139" t="s">
-        <v>503</v>
-      </c>
-      <c r="E14" s="135"/>
+      <c r="D14" s="142" t="s">
+        <v>504</v>
+      </c>
+      <c r="E14" s="138"/>
       <c r="F14" s="78"/>
       <c r="G14" s="78"/>
       <c r="H14" s="10"/>
@@ -25055,341 +25067,341 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="141" t="s">
-        <v>513</v>
-      </c>
-      <c r="B15" s="142"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="141"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="143"/>
+      <c r="A15" s="144" t="s">
+        <v>514</v>
+      </c>
+      <c r="B15" s="145"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="146"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="144" t="s">
-        <v>514</v>
-      </c>
-      <c r="B16" s="145"/>
+      <c r="A16" s="147" t="s">
+        <v>515</v>
+      </c>
+      <c r="B16" s="148"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="144" t="s">
-        <v>515</v>
+      <c r="D16" s="147" t="s">
+        <v>516</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="146" t="s">
+      <c r="G16" s="147"/>
+      <c r="H16" s="149" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="144" t="s">
-        <v>517</v>
-      </c>
-      <c r="B17" s="145"/>
+      <c r="A17" s="147" t="s">
+        <v>518</v>
+      </c>
+      <c r="B17" s="148"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="144" t="s">
-        <v>518</v>
+      <c r="D17" s="147" t="s">
+        <v>519</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
+      <c r="G17" s="147"/>
+      <c r="H17" s="147"/>
       <c r="I17" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="144" t="s">
-        <v>519</v>
-      </c>
-      <c r="B18" s="145"/>
-      <c r="C18" s="147" t="s">
+      <c r="A18" s="147" t="s">
         <v>520</v>
       </c>
-      <c r="D18" s="144" t="s">
+      <c r="B18" s="148"/>
+      <c r="C18" s="150" t="s">
         <v>521</v>
       </c>
-      <c r="E18" s="148" t="s">
-        <v>508</v>
-      </c>
-      <c r="F18" s="147" t="s">
-        <v>520</v>
-      </c>
-      <c r="G18" s="144"/>
-      <c r="H18" s="146" t="s">
+      <c r="D18" s="147" t="s">
+        <v>522</v>
+      </c>
+      <c r="E18" s="151" t="s">
+        <v>509</v>
+      </c>
+      <c r="F18" s="150" t="s">
+        <v>521</v>
+      </c>
+      <c r="G18" s="147"/>
+      <c r="H18" s="149" t="s">
         <v>22</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="144" t="s">
-        <v>522</v>
-      </c>
-      <c r="B19" s="147" t="s">
-        <v>508</v>
+      <c r="A19" s="147" t="s">
+        <v>523</v>
+      </c>
+      <c r="B19" s="150" t="s">
+        <v>509</v>
       </c>
       <c r="C19" s="24"/>
-      <c r="D19" s="149" t="s">
-        <v>523</v>
-      </c>
-      <c r="E19" s="150" t="s">
+      <c r="D19" s="152" t="s">
         <v>524</v>
       </c>
+      <c r="E19" s="153" t="s">
+        <v>525</v>
+      </c>
       <c r="F19" s="24"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="146" t="s">
+      <c r="G19" s="147"/>
+      <c r="H19" s="149" t="s">
         <v>22</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="144"/>
-      <c r="B20" s="151" t="s">
-        <v>512</v>
+      <c r="A20" s="147"/>
+      <c r="B20" s="154" t="s">
+        <v>513</v>
       </c>
       <c r="C20" s="24"/>
-      <c r="D20" s="149" t="s">
-        <v>525</v>
+      <c r="D20" s="152" t="s">
+        <v>526</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="144"/>
+      <c r="G20" s="147"/>
+      <c r="H20" s="147"/>
       <c r="I20" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="144"/>
-      <c r="B21" s="152" t="s">
-        <v>526</v>
+      <c r="A21" s="147"/>
+      <c r="B21" s="155" t="s">
+        <v>527</v>
       </c>
       <c r="C21" s="24"/>
-      <c r="D21" s="144" t="s">
-        <v>527</v>
+      <c r="D21" s="147" t="s">
+        <v>528</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
+      <c r="G21" s="147"/>
+      <c r="H21" s="147"/>
       <c r="I21" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="144" t="s">
-        <v>528</v>
-      </c>
-      <c r="B22" s="151" t="s">
-        <v>512</v>
+      <c r="A22" s="147" t="s">
+        <v>529</v>
+      </c>
+      <c r="B22" s="154" t="s">
+        <v>513</v>
       </c>
       <c r="C22" s="24"/>
-      <c r="D22" s="144"/>
+      <c r="D22" s="147"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
-      <c r="G22" s="144"/>
-      <c r="H22" s="153" t="s">
-        <v>516</v>
+      <c r="G22" s="147"/>
+      <c r="H22" s="156" t="s">
+        <v>517</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="144" t="s">
-        <v>529</v>
-      </c>
-      <c r="B23" s="147" t="s">
-        <v>508</v>
+      <c r="A23" s="147" t="s">
+        <v>530</v>
+      </c>
+      <c r="B23" s="150" t="s">
+        <v>509</v>
       </c>
       <c r="C23" s="24"/>
-      <c r="D23" s="144" t="s">
-        <v>530</v>
+      <c r="D23" s="147" t="s">
+        <v>531</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="146" t="s">
+      <c r="G23" s="147"/>
+      <c r="H23" s="149" t="s">
         <v>22</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="144" t="s">
-        <v>531</v>
-      </c>
-      <c r="B24" s="147" t="s">
-        <v>508</v>
+      <c r="A24" s="147" t="s">
+        <v>532</v>
+      </c>
+      <c r="B24" s="150" t="s">
+        <v>509</v>
       </c>
       <c r="C24" s="24"/>
-      <c r="D24" s="154" t="s">
-        <v>532</v>
-      </c>
-      <c r="E24" s="147" t="s">
-        <v>508</v>
+      <c r="D24" s="157" t="s">
+        <v>533</v>
+      </c>
+      <c r="E24" s="150" t="s">
+        <v>509</v>
       </c>
       <c r="F24" s="24"/>
-      <c r="G24" s="144"/>
-      <c r="H24" s="146" t="s">
+      <c r="G24" s="147"/>
+      <c r="H24" s="149" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="144"/>
-      <c r="B25" s="147" t="s">
-        <v>508</v>
+      <c r="A25" s="147"/>
+      <c r="B25" s="150" t="s">
+        <v>509</v>
       </c>
       <c r="C25" s="24"/>
-      <c r="D25" s="144" t="s">
-        <v>533</v>
+      <c r="D25" s="147" t="s">
+        <v>534</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="144"/>
-      <c r="H25" s="144"/>
+      <c r="G25" s="147"/>
+      <c r="H25" s="147"/>
       <c r="I25" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="144" t="s">
-        <v>534</v>
-      </c>
-      <c r="B26" s="151" t="s">
-        <v>512</v>
+      <c r="A26" s="147" t="s">
+        <v>535</v>
+      </c>
+      <c r="B26" s="154" t="s">
+        <v>513</v>
       </c>
       <c r="C26" s="24"/>
-      <c r="D26" s="144" t="s">
-        <v>535</v>
-      </c>
-      <c r="E26" s="147" t="s">
-        <v>508</v>
+      <c r="D26" s="147" t="s">
+        <v>536</v>
+      </c>
+      <c r="E26" s="150" t="s">
+        <v>509</v>
       </c>
       <c r="F26" s="24"/>
-      <c r="G26" s="144"/>
-      <c r="H26" s="146" t="s">
+      <c r="G26" s="147"/>
+      <c r="H26" s="149" t="s">
         <v>22</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="144"/>
-      <c r="B27" s="152" t="s">
-        <v>526</v>
+      <c r="A27" s="147"/>
+      <c r="B27" s="155" t="s">
+        <v>527</v>
       </c>
       <c r="C27" s="24"/>
-      <c r="D27" s="144" t="s">
-        <v>536</v>
+      <c r="D27" s="147" t="s">
+        <v>537</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="144"/>
-      <c r="H27" s="144"/>
+      <c r="G27" s="147"/>
+      <c r="H27" s="147"/>
       <c r="I27" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="144" t="s">
-        <v>537</v>
-      </c>
-      <c r="B28" s="151" t="s">
-        <v>512</v>
+      <c r="A28" s="147" t="s">
+        <v>538</v>
+      </c>
+      <c r="B28" s="154" t="s">
+        <v>513</v>
       </c>
       <c r="C28" s="24"/>
-      <c r="D28" s="144"/>
+      <c r="D28" s="147"/>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="144"/>
-      <c r="H28" s="153" t="s">
-        <v>516</v>
+      <c r="G28" s="147"/>
+      <c r="H28" s="156" t="s">
+        <v>517</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="144" t="s">
-        <v>538</v>
-      </c>
-      <c r="B29" s="151" t="s">
-        <v>512</v>
+      <c r="A29" s="147" t="s">
+        <v>539</v>
+      </c>
+      <c r="B29" s="154" t="s">
+        <v>513</v>
       </c>
       <c r="C29" s="24"/>
-      <c r="D29" s="144" t="s">
-        <v>539</v>
-      </c>
-      <c r="E29" s="151"/>
+      <c r="D29" s="147" t="s">
+        <v>540</v>
+      </c>
+      <c r="E29" s="154"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="144"/>
-      <c r="H29" s="153" t="s">
-        <v>516</v>
+      <c r="G29" s="147"/>
+      <c r="H29" s="156" t="s">
+        <v>517</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="144"/>
+      <c r="A30" s="147"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
-      <c r="D30" s="144"/>
+      <c r="D30" s="147"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
-      <c r="G30" s="144"/>
-      <c r="H30" s="144"/>
+      <c r="G30" s="147"/>
+      <c r="H30" s="147"/>
       <c r="I30" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="144" t="s">
-        <v>540</v>
-      </c>
-      <c r="B31" s="155" t="s">
+      <c r="A31" s="147" t="s">
+        <v>541</v>
+      </c>
+      <c r="B31" s="158" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="24"/>
-      <c r="D31" s="144"/>
+      <c r="D31" s="147"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
-      <c r="G31" s="144"/>
-      <c r="H31" s="144"/>
+      <c r="G31" s="147"/>
+      <c r="H31" s="147"/>
       <c r="I31" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="144" t="s">
-        <v>541</v>
+      <c r="A32" s="147" t="s">
+        <v>542</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="24"/>
-      <c r="D32" s="144"/>
+      <c r="D32" s="147"/>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
-      <c r="G32" s="144"/>
-      <c r="H32" s="144"/>
+      <c r="G32" s="147"/>
+      <c r="H32" s="147"/>
       <c r="I32" s="22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved prepare_testssl_output function readability and performances. Added new sheets to default_versions.json. Updated database.
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -76,6 +76,14 @@
         <t xml:space="preserve">R32</t>
       </text>
     </comment>
+    <comment authorId="0" ref="D4">
+      <text>
+        <t xml:space="preserve">Same as in Public-Key Cryptography Standards (PKCS) 10 request or calculated by the issuing CA
+----
+non ricordo se avevamo deciso di lasciare solo la nota o come gestire questo caso
+	-Riccardo Germenia</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="D5">
       <text>
         <t xml:space="preserve">RSA, ECDSA, or DSA signature certificate: digital signature;
@@ -102,6 +110,16 @@
     <comment authorId="0" ref="B9">
       <text>
         <t xml:space="preserve">Required. Multiple SANs are permitted, e.g., for load balanced environments.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D9">
+      <text>
+        <t xml:space="preserve">DNS host name, or IP address if there is no DNS name assigned. Other name forms may be included, if appropriate.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G9">
+      <text>
+        <t xml:space="preserve">use wildcards</t>
       </text>
     </comment>
     <comment authorId="0" ref="H9">
@@ -849,12 +867,37 @@
         <t xml:space="preserve">value: 2, version: 3</t>
       </text>
     </comment>
+    <comment authorId="0" ref="A4">
+      <text>
+        <t xml:space="preserve"> Also known as DN</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C4">
+      <text>
+        <t xml:space="preserve">A single value should be encoded in each Relative Distinguished Name (RDN) (the single values that compose the DN). All attributes that are of DirectoryString type should be encoded as a PrintableString.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E4">
+      <text>
+        <t xml:space="preserve">use wildcards in CN</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C6">
+      <text>
+        <t xml:space="preserve">A single value should be encoded in each Relative Distinguished Name (RDN) (the single values that compose the DN). All attributes that are of DirectoryString type should be encoded as a PrintableString.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E6">
+      <text>
+        <t xml:space="preserve">use wildcards in CN</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2549" uniqueCount="594">
   <si>
     <t>NIST</t>
   </si>
@@ -2368,16 +2411,16 @@
     <t>X.509 version</t>
   </si>
   <si>
-    <t>value: 2, version: 3</t>
-  </si>
-  <si>
-    <t>Issuer Distinguished Name (DN)</t>
-  </si>
-  <si>
-    <t>A single value should be encoded in each Relative Distinguished Name (RDN) (the single values that compose the DN). All attributes that are of DirectoryString type should be encoded as a PrintableString.</t>
-  </si>
-  <si>
-    <t>use wildcards in CN, S</t>
+    <t>VALUE Certificate X.509 version == 2</t>
+  </si>
+  <si>
+    <t>Issuer Distinguished Name</t>
+  </si>
+  <si>
+    <t>VALUE Certificate , not in [Issuer Distinguished Name][CN,O,OU,L,S]</t>
+  </si>
+  <si>
+    <t>VALUE Certificate * not in [Issuer Distinguished Name][CN]</t>
   </si>
   <si>
     <t>validity</t>
@@ -2389,12 +2432,6 @@
     <t>Subject Distinguished Name</t>
   </si>
   <si>
-    <t>A single value should be encoded in each RDN (the single values that compose the DN). All attributes that are of DirectoryString type should be encoded as a PrintableString. If present, the CN attribute should be of the form: CN={host IP address | host DNS name}</t>
-  </si>
-  <si>
-    <t>use wildcards</t>
-  </si>
-  <si>
     <t>Extension</t>
   </si>
   <si>
@@ -2410,9 +2447,6 @@
     <t>Subject Key Identifier (SKI)</t>
   </si>
   <si>
-    <t>Same as in Public-Key Cryptography Standards (PKCS) 10 request or calculated by the issuing CA</t>
-  </si>
-  <si>
     <t>Key Usage</t>
   </si>
   <si>
@@ -2437,7 +2471,10 @@
     <t>Subject Alternative Name (SAN)</t>
   </si>
   <si>
-    <t>DNS host name, or IP address if there is no DNS name assigned. Other name forms may be included, if appropriate.</t>
+    <t>CONTAINS DNS OR CONTAINS IP Address</t>
+  </si>
+  <si>
+    <t>CONTAINS NOT *</t>
   </si>
   <si>
     <t>Authority Information Access</t>
@@ -3343,9 +3380,6 @@
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -3355,14 +3389,11 @@
     <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -3377,12 +3408,18 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -4193,7 +4230,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="139" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B1" s="140" t="s">
         <v>0</v>
@@ -4217,14 +4254,14 @@
       <c r="A2" s="141"/>
       <c r="B2" s="27"/>
       <c r="C2" s="142" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D2" s="142" t="s">
         <v>502</v>
       </c>
       <c r="E2" s="143"/>
       <c r="F2" s="142" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G2" s="142" t="s">
         <v>502</v>
@@ -4237,98 +4274,96 @@
     </row>
     <row r="3">
       <c r="A3" s="142" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="149" t="s">
-        <v>516</v>
+      <c r="C3" s="149"/>
+      <c r="D3" s="148" t="s">
+        <v>514</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="151"/>
+      <c r="F3" s="150"/>
       <c r="G3" s="141"/>
       <c r="H3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="153"/>
+      <c r="I3" s="151"/>
       <c r="J3" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="142" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="149" t="s">
-        <v>518</v>
-      </c>
+      <c r="C4" s="150"/>
+      <c r="D4" s="148"/>
       <c r="E4" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="151"/>
+      <c r="F4" s="150"/>
       <c r="G4" s="141"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="155"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="153"/>
       <c r="J4" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="142" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="142" t="s">
-        <v>520</v>
-      </c>
-      <c r="D5" s="149" t="s">
-        <v>521</v>
+        <v>517</v>
+      </c>
+      <c r="D5" s="148" t="s">
+        <v>518</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="142" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="G5" s="141"/>
       <c r="H5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="153"/>
+      <c r="I5" s="151"/>
       <c r="J5" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="142" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="156" t="s">
-        <v>523</v>
+      <c r="C6" s="150"/>
+      <c r="D6" s="154" t="s">
+        <v>520</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="151"/>
+      <c r="F6" s="150"/>
       <c r="G6" s="141"/>
       <c r="H6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="153"/>
+      <c r="I6" s="151"/>
       <c r="J6" s="11" t="s">
         <v>50</v>
       </c>
@@ -4338,90 +4373,92 @@
       <c r="B7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="151"/>
-      <c r="D7" s="149" t="s">
-        <v>524</v>
+      <c r="C7" s="150"/>
+      <c r="D7" s="148" t="s">
+        <v>521</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="151"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="141"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="155"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="153"/>
       <c r="J7" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="142" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="152"/>
-      <c r="D8" s="152"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="151"/>
+      <c r="F8" s="150"/>
       <c r="G8" s="141"/>
       <c r="H8" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="153"/>
+      <c r="I8" s="151"/>
       <c r="J8" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="142" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="157" t="s">
-        <v>527</v>
+      <c r="C9" s="149"/>
+      <c r="D9" s="155" t="s">
+        <v>524</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="151"/>
-      <c r="G9" s="141"/>
+        <v>13</v>
+      </c>
+      <c r="F9" s="150"/>
+      <c r="G9" s="148" t="s">
+        <v>525</v>
+      </c>
       <c r="H9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="153"/>
+      <c r="I9" s="151"/>
       <c r="J9" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="142" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="152"/>
+      <c r="C10" s="149"/>
       <c r="D10" s="142" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="151"/>
+      <c r="F10" s="150"/>
       <c r="G10" s="142" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="H10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="158" t="s">
-        <v>530</v>
+      <c r="I10" s="156" t="s">
+        <v>528</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>50</v>
@@ -4432,42 +4469,42 @@
       <c r="B11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="149" t="s">
-        <v>531</v>
-      </c>
-      <c r="E11" s="146"/>
-      <c r="F11" s="151"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="148" t="s">
+        <v>529</v>
+      </c>
+      <c r="E11" s="157"/>
+      <c r="F11" s="150"/>
       <c r="G11" s="141"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="159"/>
+      <c r="H11" s="152"/>
+      <c r="I11" s="158"/>
       <c r="J11" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="142" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="151"/>
-      <c r="D12" s="149" t="s">
-        <v>533</v>
+      <c r="C12" s="150"/>
+      <c r="D12" s="148" t="s">
+        <v>531</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="151"/>
+      <c r="F12" s="150"/>
       <c r="G12" s="142" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="158" t="s">
-        <v>534</v>
+      <c r="I12" s="156" t="s">
+        <v>532</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>50</v>
@@ -4478,13 +4515,13 @@
       <c r="B13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="151"/>
-      <c r="D13" s="149" t="s">
-        <v>535</v>
-      </c>
-      <c r="E13" s="150"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="151"/>
+      <c r="C13" s="150"/>
+      <c r="D13" s="148" t="s">
+        <v>533</v>
+      </c>
+      <c r="E13" s="159"/>
+      <c r="F13" s="150"/>
+      <c r="G13" s="150"/>
       <c r="H13" s="160"/>
       <c r="I13" s="161"/>
       <c r="J13" s="11" t="s">
@@ -4493,40 +4530,40 @@
     </row>
     <row r="14">
       <c r="A14" s="142" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="151"/>
-      <c r="D14" s="151"/>
-      <c r="E14" s="150"/>
-      <c r="F14" s="151"/>
-      <c r="G14" s="151"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="159"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="150"/>
       <c r="H14" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="147"/>
+      <c r="I14" s="146"/>
       <c r="J14" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="142" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="151"/>
+      <c r="C15" s="150"/>
       <c r="D15" s="142"/>
       <c r="E15" s="162"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="152"/>
+      <c r="F15" s="149"/>
+      <c r="G15" s="149"/>
       <c r="H15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="147"/>
+      <c r="I15" s="146"/>
       <c r="J15" s="11" t="s">
         <v>50</v>
       </c>
@@ -4536,7 +4573,7 @@
       <c r="B16" s="27"/>
       <c r="C16" s="141"/>
       <c r="D16" s="163"/>
-      <c r="E16" s="146"/>
+      <c r="E16" s="157"/>
       <c r="F16" s="141"/>
       <c r="G16" s="141"/>
       <c r="H16" s="160"/>
@@ -4547,14 +4584,14 @@
     </row>
     <row r="17">
       <c r="A17" s="142" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="141"/>
       <c r="D17" s="163"/>
-      <c r="E17" s="146"/>
+      <c r="E17" s="157"/>
       <c r="F17" s="141"/>
       <c r="G17" s="141"/>
       <c r="H17" s="160"/>
@@ -4565,14 +4602,14 @@
     </row>
     <row r="18">
       <c r="A18" s="142" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="141"/>
       <c r="D18" s="163"/>
-      <c r="E18" s="146"/>
+      <c r="E18" s="157"/>
       <c r="F18" s="141"/>
       <c r="G18" s="141"/>
       <c r="H18" s="160"/>
@@ -4657,7 +4694,7 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B2" s="119"/>
       <c r="C2" s="119"/>
@@ -4665,7 +4702,7 @@
     </row>
     <row r="3">
       <c r="A3" s="142" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>13</v>
@@ -4680,7 +4717,7 @@
     </row>
     <row r="4">
       <c r="A4" s="142" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="160"/>
@@ -4770,7 +4807,7 @@
       </c>
       <c r="G1" s="167"/>
       <c r="H1" s="167" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="2">
@@ -4795,21 +4832,21 @@
     </row>
     <row r="4">
       <c r="A4" s="167" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B4" s="169" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C4" s="168"/>
       <c r="D4" s="169" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E4" s="168"/>
       <c r="F4" s="169" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G4" s="169" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H4" s="170"/>
     </row>
@@ -4826,20 +4863,20 @@
     <row r="6">
       <c r="A6" s="167"/>
       <c r="B6" s="171" t="s">
+        <v>547</v>
+      </c>
+      <c r="C6" s="169" t="s">
+        <v>548</v>
+      </c>
+      <c r="D6" s="169" t="s">
         <v>549</v>
-      </c>
-      <c r="C6" s="169" t="s">
-        <v>550</v>
-      </c>
-      <c r="D6" s="169" t="s">
-        <v>551</v>
       </c>
       <c r="E6" s="168"/>
       <c r="F6" s="171" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G6" s="169" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H6" s="170"/>
     </row>
@@ -4848,7 +4885,7 @@
       <c r="B7" s="167"/>
       <c r="C7" s="167"/>
       <c r="D7" s="169" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E7" s="168"/>
       <c r="F7" s="168"/>
@@ -4859,13 +4896,13 @@
       <c r="A8" s="167"/>
       <c r="B8" s="167"/>
       <c r="C8" s="167" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D8" s="168"/>
       <c r="E8" s="168"/>
       <c r="F8" s="168"/>
       <c r="G8" s="167" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H8" s="167" t="s">
         <v>414</v>
@@ -4875,7 +4912,7 @@
       <c r="A9" s="167"/>
       <c r="B9" s="167"/>
       <c r="C9" s="172" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D9" s="168"/>
       <c r="E9" s="168"/>
@@ -4886,18 +4923,18 @@
     <row r="10">
       <c r="A10" s="167"/>
       <c r="B10" s="169" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C10" s="169" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D10" s="168"/>
       <c r="E10" s="169" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F10" s="168"/>
       <c r="G10" s="169" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H10" s="170"/>
     </row>
@@ -4907,7 +4944,7 @@
       <c r="C11" s="167"/>
       <c r="D11" s="168"/>
       <c r="E11" s="169" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F11" s="168"/>
       <c r="G11" s="167"/>
@@ -4919,7 +4956,7 @@
       <c r="C12" s="167"/>
       <c r="D12" s="168"/>
       <c r="E12" s="169" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F12" s="168"/>
       <c r="G12" s="167"/>
@@ -4930,7 +4967,7 @@
       <c r="B13" s="167"/>
       <c r="C13" s="167"/>
       <c r="D13" s="169" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E13" s="167"/>
       <c r="F13" s="168"/>
@@ -4941,11 +4978,11 @@
       <c r="A14" s="167"/>
       <c r="B14" s="167"/>
       <c r="C14" s="169" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D14" s="168"/>
       <c r="E14" s="169" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F14" s="168"/>
       <c r="G14" s="168"/>
@@ -4957,7 +4994,7 @@
       <c r="C15" s="167"/>
       <c r="D15" s="168"/>
       <c r="E15" s="169" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F15" s="168"/>
       <c r="G15" s="168"/>
@@ -4967,31 +5004,31 @@
       <c r="A16" s="167"/>
       <c r="B16" s="167"/>
       <c r="C16" s="171" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D16" s="168"/>
       <c r="E16" s="167"/>
       <c r="F16" s="168"/>
       <c r="G16" s="171" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H16" s="174"/>
     </row>
     <row r="17">
       <c r="A17" s="167"/>
       <c r="B17" s="169" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C17" s="169" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D17" s="168"/>
       <c r="E17" s="169" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F17" s="168"/>
       <c r="G17" s="169" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="H17" s="170"/>
     </row>
@@ -5001,7 +5038,7 @@
       <c r="C18" s="167"/>
       <c r="D18" s="168"/>
       <c r="E18" s="169" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F18" s="168"/>
       <c r="G18" s="167"/>
@@ -5013,7 +5050,7 @@
       <c r="C19" s="167"/>
       <c r="D19" s="168"/>
       <c r="E19" s="169" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F19" s="168"/>
       <c r="G19" s="168"/>
@@ -5023,11 +5060,11 @@
       <c r="A20" s="167"/>
       <c r="B20" s="167"/>
       <c r="C20" s="169" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D20" s="168"/>
       <c r="E20" s="169" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F20" s="167"/>
       <c r="G20" s="167"/>
@@ -5037,11 +5074,11 @@
       <c r="A21" s="167"/>
       <c r="B21" s="167"/>
       <c r="C21" s="169" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D21" s="168"/>
       <c r="E21" s="169" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F21" s="168"/>
       <c r="G21" s="168"/>
@@ -5050,14 +5087,14 @@
     <row r="22">
       <c r="A22" s="167"/>
       <c r="B22" s="172" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C22" s="172" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D22" s="168"/>
       <c r="E22" s="172" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F22" s="168"/>
       <c r="G22" s="168"/>
@@ -5067,7 +5104,7 @@
       <c r="A23" s="167"/>
       <c r="B23" s="167"/>
       <c r="C23" s="172" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D23" s="168"/>
       <c r="E23" s="167"/>
@@ -5079,7 +5116,7 @@
       <c r="A24" s="167"/>
       <c r="B24" s="167"/>
       <c r="C24" s="172" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D24" s="168"/>
       <c r="E24" s="168"/>
@@ -5091,7 +5128,7 @@
       <c r="A25" s="167"/>
       <c r="B25" s="167"/>
       <c r="C25" s="172" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D25" s="168"/>
       <c r="E25" s="168"/>
@@ -5102,16 +5139,16 @@
     <row r="26">
       <c r="A26" s="167"/>
       <c r="B26" s="167" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C26" s="168"/>
       <c r="D26" s="168"/>
       <c r="E26" s="167" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F26" s="168"/>
       <c r="G26" s="167" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H26" s="167" t="s">
         <v>414</v>
@@ -5120,25 +5157,25 @@
     <row r="27">
       <c r="A27" s="167"/>
       <c r="B27" s="169" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C27" s="168"/>
       <c r="D27" s="168"/>
       <c r="E27" s="168"/>
       <c r="F27" s="168"/>
       <c r="G27" s="171" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H27" s="170"/>
     </row>
     <row r="28">
       <c r="A28" s="167"/>
       <c r="B28" s="172" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C28" s="168"/>
       <c r="D28" s="167" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E28" s="168"/>
       <c r="F28" s="168"/>
@@ -5157,7 +5194,7 @@
     </row>
     <row r="30">
       <c r="A30" s="167" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B30" s="167"/>
       <c r="C30" s="168"/>
@@ -5222,7 +5259,7 @@
     </row>
     <row r="5">
       <c r="A5" s="179" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B5" s="177"/>
       <c r="C5" s="177"/>
@@ -5274,13 +5311,13 @@
     </row>
     <row r="12">
       <c r="A12" s="180" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D12" s="177"/>
     </row>
     <row r="13">
       <c r="A13" s="180" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B13" s="177"/>
       <c r="C13" s="177"/>
@@ -5288,13 +5325,13 @@
     </row>
     <row r="14">
       <c r="A14" s="180" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D14" s="177"/>
     </row>
     <row r="15">
       <c r="A15" s="180" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B15" s="177"/>
     </row>
@@ -27215,125 +27252,117 @@
       <c r="C3" s="142" t="s">
         <v>504</v>
       </c>
-      <c r="D3" s="146"/>
+      <c r="D3" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="E3" s="141"/>
       <c r="F3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="147"/>
+      <c r="G3" s="146"/>
       <c r="H3" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="147" t="s">
         <v>505</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="148" t="s">
         <v>506</v>
       </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="151"/>
+      <c r="D4" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="148" t="s">
+        <v>507</v>
+      </c>
       <c r="F4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="147"/>
+      <c r="G4" s="146"/>
       <c r="H4" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="27"/>
-      <c r="C5" s="149"/>
+      <c r="A5" s="142" t="s">
+        <v>508</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="148" t="s">
+        <v>509</v>
+      </c>
       <c r="D5" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="152" t="s">
-        <v>507</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="147"/>
-      <c r="H5" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="E5" s="148" t="s">
+        <v>509</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="146"/>
+      <c r="H5" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="142" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="149" t="s">
-        <v>509</v>
+      <c r="C6" s="148" t="s">
+        <v>506</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="149" t="s">
-        <v>509</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="148" t="s">
+        <v>507</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="147"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="142" t="s">
-        <v>510</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="149" t="s">
-        <v>511</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="149" t="s">
-        <v>512</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="147"/>
-      <c r="H7" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B7 F2:F7 H2:H7 G3:G7 D5:D7">
+  <conditionalFormatting sqref="B2:B6 F2:F6 H2:H6 D3:D6 G3:G6">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"must not"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7 F2:F7 H2:H7 G3:G7 D5:D7">
+  <conditionalFormatting sqref="B2:B6 F2:F6 H2:H6 D3:D6 G3:G6">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"recommended"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7 F2:F7 H2:H7 G3:G7 D5:D7">
+  <conditionalFormatting sqref="B2:B6 F2:F6 H2:H6 D3:D6 G3:G6">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"not recommended"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7 F2:F7 H2:H7 G3:G7 D5:D7">
+  <conditionalFormatting sqref="B2:B6 F2:F6 H2:H6 D3:D6 G3:G6">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"must"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7 F2:F7 H2:H7 G3:G7 D5:D7">
+  <conditionalFormatting sqref="B2:B6 F2:F6 H2:H6 D3:D6 G3:G6">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"not recommended*"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added conditional notes and fixed small issues with analysis
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -516,6 +516,12 @@
         <t xml:space="preserve">the server supports TLS 1.3</t>
       </text>
     </comment>
+    <comment authorId="0" ref="J16">
+      <text>
+        <t xml:space="preserve">ha senso mettere la seconda nota solo se è abilitata?
+	-Riccardo Germenia</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="G41">
       <text>
         <t xml:space="preserve">le lasciamo così?
@@ -779,15 +785,20 @@
         <t xml:space="preserve">BSI-TR-02102-2, 3.3.3 + 3.4.3</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G1">
+    <comment authorId="0" ref="H1">
       <text>
         <t xml:space="preserve">R8</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H1">
+    <comment authorId="0" ref="I1">
       <text>
         <t xml:space="preserve">Being a list of recommendations:
 not mentioned --&gt; not recommended</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G2">
+      <text>
+        <t xml:space="preserve">Not explicitally mentioned but required to match the mechanical check of the conditions with the NIST case</t>
       </text>
     </comment>
     <comment authorId="0" ref="D3">
@@ -795,7 +806,7 @@
         <t xml:space="preserve">TLS servers conforming to this specification shall be configured with an RSA signature certificate or an ECDSA signature certificate</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G3">
+    <comment authorId="0" ref="H3">
       <text>
         <t xml:space="preserve">R8+R5</t>
       </text>
@@ -818,12 +829,6 @@
     <comment authorId="0" ref="E6">
       <text>
         <t xml:space="preserve">At a minimum, TLS servers conforming to this specification shall be configured with an RSA signature certificate or an ECDSA signature certificate. </t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="F4">
-      <text>
-        <t xml:space="preserve">essendo tutti e 3 validi andrebbe messa la condizione con i this or
-	-Riccardo Germenia</t>
       </text>
     </comment>
   </commentList>
@@ -1010,7 +1015,10 @@
     </comment>
     <comment authorId="0" ref="E6">
       <text>
-        <t xml:space="preserve">use wildcards in CN</t>
+        <t xml:space="preserve">use wildcards in CN
+----
+dato che NON DEVE avere le wildcards nel campo nella condizione va verificato sele contiene. Se le contiene risulta il livello must not
+	-Riccardo Germenia</t>
       </text>
     </comment>
   </commentList>
@@ -1018,7 +1026,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="598">
   <si>
     <t>NIST</t>
   </si>
@@ -2103,10 +2111,10 @@
     <t>signature_algorithms</t>
   </si>
   <si>
-    <t>NOTE if this condition results as an ERROR "must be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported</t>
-  </si>
-  <si>
-    <t>NOTE if this condition results as an ERROR "must be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported. and NOTE in order for the web-server to be compliant with BSI guidelines you should enabled all the signature algorithms reccommended by BSI</t>
+    <t>NOTE_DISABLED if this condition results as an ERROR "must be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported</t>
+  </si>
+  <si>
+    <t>NOTE_DISABLED if this condition results as an ERROR "must be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported. and NOTE_ENABLED in order for the web-server to be compliant with BSI guidelines you should enabled all the signature algorithms reccommended by BSI</t>
   </si>
   <si>
     <t>use_srtp</t>
@@ -2184,13 +2192,13 @@
     <t>signature_algorithms_cert</t>
   </si>
   <si>
-    <t>TLS 1.3 and NOTE if this condition results as an ERROR "must be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported</t>
-  </si>
-  <si>
-    <t>NOTE This field's level is not explicitly mentioned in the guidelines. If you want to use it in order for the web-server to be compliant with BSI guidelines you should enabled all the signature algorithms reccommended by BSI and also enable the rsa_pkcs1_sha256, rsa_pkcs1_sha384 and rsa_pkcs1_sha512 signature algorithms</t>
-  </si>
-  <si>
-    <t>TLS 1.2 and NOTE if this condition results as an ALERT "should be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported</t>
+    <t>TLS 1.3 and NOTE_DISABLED if this condition results as an ERROR "must be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported</t>
+  </si>
+  <si>
+    <t>NOTE_ENABLED This field's level is not explicitly mentioned in the guidelines. If you want to use it in order for the web-server to be compliant with BSI guidelines you should enabled all the signature algorithms reccommended by BSI and also enable the rsa_pkcs1_sha256, rsa_pkcs1_sha384 and rsa_pkcs1_sha512 signature algorithms</t>
+  </si>
+  <si>
+    <t>TLS 1.2 and NOTE_DISABLED if this condition results as an ALERT "should be enabled" it may be a false positive. It is caused by the web-server not asking the certificate to the client not allowing the tool to verify whether the extension is supported</t>
   </si>
   <si>
     <t>key_share</t>
@@ -2469,18 +2477,27 @@
     <t>THIS or CertificateSignature ecdsa and CHECK_KEY_TYPE rsa</t>
   </si>
   <si>
+    <t>THIS or CertificateSignature dsa;ecdsa</t>
+  </si>
+  <si>
     <t>dsa</t>
   </si>
   <si>
     <t>CHECK_KEY_TYPE dsa</t>
   </si>
   <si>
+    <t>THIS or CertificateSignature rsa;ecdsa</t>
+  </si>
+  <si>
     <t>ecdsa</t>
   </si>
   <si>
     <t>THIS or CertificateSignature rsa and CHECK_KEY_TYPE ecddsa</t>
   </si>
   <si>
+    <t>THIS or CertificateSignature rsa;dsa</t>
+  </si>
+  <si>
     <t>Use</t>
   </si>
   <si>
@@ -2532,7 +2549,7 @@
     <t>X.509 version</t>
   </si>
   <si>
-    <t>VALUE Certificate X.509 version == 2</t>
+    <t>NOTE_FALSE {reason} and VALUE Certificate X.509 version == 2</t>
   </si>
   <si>
     <t>Issuer Distinguished Name</t>
@@ -2541,7 +2558,7 @@
     <t>VALUE Certificate , not in [Issuer Distinguished Name][CN,O,OU,L,S]</t>
   </si>
   <si>
-    <t>VALUE Certificate * not in [Issuer Distinguished Name][CN] NOTE BSI guidelines prohibit the usage of * inside the CN field of the Issuer Distinguished Name</t>
+    <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason}, remember that BSI guidelines prohibit the usage of * in this field and VALUE Certificate * in [Issuer Distinguished Name][CN]</t>
   </si>
   <si>
     <t>validity</t>
@@ -2553,7 +2570,7 @@
     <t>Subject Distinguished Name</t>
   </si>
   <si>
-    <t>VALUE Certificate * not in [Subject Distinguished Name][CN] and NOTE BSI guidelines prohibit the usage of * inside the CN field of the Subject Distinguished Name</t>
+    <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason}, remember that BSI guidelines prohibit the usage of * in this field and VALUE Certificate * in [Subject Distinguished Name][CN]</t>
   </si>
   <si>
     <t>Extension</t>
@@ -2595,7 +2612,7 @@
     <t>VALUE CertificateExtensions DNS in subjectAltName OR VALUE CertificateExtensions IP Address in subjectAltName</t>
   </si>
   <si>
-    <t>VALUE CertificateExtensions * not in subjectAltName and NOTE BSI guidelines prohibit the usage of * inside the subjectAltName field</t>
+    <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason} and VALUE CertificateExtensions * in subjectAltName</t>
   </si>
   <si>
     <t>authorityInfoAccess</t>
@@ -2809,7 +2826,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2901,6 +2918,11 @@
     <font>
       <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -3086,7 +3108,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="186">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3444,10 +3466,16 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="3" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3472,13 +3500,13 @@
     <xf borderId="7" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3508,20 +3536,17 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -3529,16 +3554,16 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3548,7 +3573,7 @@
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3557,13 +3582,16 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3602,17 +3630,17 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -4312,389 +4340,389 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="138" t="s">
-        <v>512</v>
-      </c>
-      <c r="B1" s="139" t="s">
+      <c r="A1" s="140" t="s">
+        <v>515</v>
+      </c>
+      <c r="B1" s="141" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="108"/>
       <c r="D1" s="108"/>
-      <c r="E1" s="139" t="s">
+      <c r="E1" s="141" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="108"/>
       <c r="G1" s="108"/>
-      <c r="H1" s="139" t="s">
+      <c r="H1" s="141" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="108"/>
       <c r="J1" s="9" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="140"/>
+      <c r="A2" s="142"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="141" t="s">
-        <v>513</v>
-      </c>
-      <c r="D2" s="143" t="s">
-        <v>502</v>
-      </c>
-      <c r="E2" s="142"/>
-      <c r="F2" s="141" t="s">
-        <v>513</v>
-      </c>
-      <c r="G2" s="141" t="s">
-        <v>502</v>
+      <c r="C2" s="143" t="s">
+        <v>516</v>
+      </c>
+      <c r="D2" s="145" t="s">
+        <v>505</v>
+      </c>
+      <c r="E2" s="144"/>
+      <c r="F2" s="143" t="s">
+        <v>516</v>
+      </c>
+      <c r="G2" s="143" t="s">
+        <v>505</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="143" t="s">
-        <v>502</v>
-      </c>
-      <c r="J2" s="144"/>
+      <c r="I2" s="145" t="s">
+        <v>505</v>
+      </c>
+      <c r="J2" s="146"/>
     </row>
     <row r="3">
-      <c r="A3" s="141" t="s">
-        <v>514</v>
+      <c r="A3" s="143" t="s">
+        <v>517</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="150"/>
-      <c r="G3" s="140"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="142"/>
       <c r="H3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="151"/>
+      <c r="I3" s="126"/>
       <c r="J3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="141" t="s">
-        <v>515</v>
+      <c r="A4" s="143" t="s">
+        <v>518</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="149"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="151"/>
       <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="150"/>
-      <c r="G4" s="140"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="153"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="154"/>
       <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="141" t="s">
-        <v>516</v>
+      <c r="A5" s="143" t="s">
+        <v>519</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="141" t="s">
-        <v>517</v>
-      </c>
-      <c r="D5" s="149" t="s">
-        <v>518</v>
+      <c r="C5" s="143" t="s">
+        <v>520</v>
+      </c>
+      <c r="D5" s="151" t="s">
+        <v>521</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="141" t="s">
-        <v>517</v>
-      </c>
-      <c r="G5" s="140"/>
+      <c r="F5" s="143" t="s">
+        <v>520</v>
+      </c>
+      <c r="G5" s="142"/>
       <c r="H5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="151"/>
+      <c r="I5" s="126"/>
       <c r="J5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="141" t="s">
-        <v>519</v>
+      <c r="A6" s="143" t="s">
+        <v>522</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="154" t="s">
-        <v>520</v>
+      <c r="C6" s="152"/>
+      <c r="D6" s="155" t="s">
+        <v>523</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="150"/>
-      <c r="G6" s="140"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="142"/>
       <c r="H6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="151"/>
+      <c r="I6" s="126"/>
       <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="140"/>
+      <c r="A7" s="142"/>
       <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="150"/>
-      <c r="D7" s="149" t="s">
-        <v>521</v>
+      <c r="C7" s="152"/>
+      <c r="D7" s="151" t="s">
+        <v>524</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="150"/>
-      <c r="G7" s="140"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="153"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="154"/>
       <c r="J7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="141" t="s">
-        <v>522</v>
+      <c r="A8" s="143" t="s">
+        <v>525</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="148"/>
-      <c r="D8" s="155"/>
+      <c r="C8" s="150"/>
+      <c r="D8" s="156"/>
       <c r="E8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="150"/>
-      <c r="G8" s="140"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="142"/>
       <c r="H8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="151"/>
+      <c r="I8" s="126"/>
       <c r="J8" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="141" t="s">
-        <v>523</v>
+      <c r="A9" s="143" t="s">
+        <v>526</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="148"/>
-      <c r="D9" s="156" t="s">
-        <v>524</v>
+      <c r="C9" s="150"/>
+      <c r="D9" s="157" t="s">
+        <v>527</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="150"/>
-      <c r="G9" s="147" t="s">
-        <v>525</v>
+      <c r="F9" s="152"/>
+      <c r="G9" s="149" t="s">
+        <v>528</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="151"/>
+      <c r="I9" s="126"/>
       <c r="J9" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="141" t="s">
-        <v>526</v>
+      <c r="A10" s="143" t="s">
+        <v>529</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="157" t="s">
-        <v>527</v>
+      <c r="C10" s="150"/>
+      <c r="D10" s="158" t="s">
+        <v>530</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="150"/>
-      <c r="G10" s="141" t="s">
-        <v>528</v>
+      <c r="F10" s="152"/>
+      <c r="G10" s="143" t="s">
+        <v>531</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="158" t="s">
-        <v>528</v>
+      <c r="I10" s="159" t="s">
+        <v>531</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="141"/>
+      <c r="A11" s="143"/>
       <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="150"/>
-      <c r="D11" s="157" t="s">
-        <v>529</v>
-      </c>
-      <c r="E11" s="159"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="152"/>
-      <c r="I11" s="160"/>
+      <c r="C11" s="152"/>
+      <c r="D11" s="158" t="s">
+        <v>532</v>
+      </c>
+      <c r="E11" s="160"/>
+      <c r="F11" s="152"/>
+      <c r="G11" s="142"/>
+      <c r="H11" s="153"/>
+      <c r="I11" s="161"/>
       <c r="J11" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="141" t="s">
-        <v>530</v>
+      <c r="A12" s="143" t="s">
+        <v>533</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="150"/>
-      <c r="D12" s="149" t="s">
-        <v>531</v>
+      <c r="C12" s="152"/>
+      <c r="D12" s="151" t="s">
+        <v>534</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="150"/>
-      <c r="G12" s="141" t="s">
-        <v>532</v>
+      <c r="F12" s="152"/>
+      <c r="G12" s="143" t="s">
+        <v>535</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="158" t="s">
-        <v>532</v>
+      <c r="I12" s="159" t="s">
+        <v>535</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="141"/>
+      <c r="A13" s="143"/>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="150"/>
-      <c r="D13" s="149" t="s">
-        <v>533</v>
-      </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="162"/>
-      <c r="I13" s="163"/>
+      <c r="C13" s="152"/>
+      <c r="D13" s="151" t="s">
+        <v>536</v>
+      </c>
+      <c r="E13" s="162"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="164"/>
       <c r="J13" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="141" t="s">
-        <v>534</v>
+      <c r="A14" s="143" t="s">
+        <v>537</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="150"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="161"/>
-      <c r="F14" s="150"/>
-      <c r="G14" s="150"/>
+      <c r="C14" s="152"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
       <c r="H14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="145"/>
+      <c r="I14" s="147"/>
       <c r="J14" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="141" t="s">
-        <v>535</v>
+      <c r="A15" s="143" t="s">
+        <v>538</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="150"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="165"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
       <c r="H15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="145"/>
+      <c r="I15" s="147"/>
       <c r="J15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="140"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="166"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="162"/>
-      <c r="I16" s="163"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="142"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="164"/>
       <c r="J16" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="141" t="s">
-        <v>536</v>
+      <c r="A17" s="143" t="s">
+        <v>539</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="140"/>
-      <c r="D17" s="166"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="162"/>
-      <c r="I17" s="163"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="168"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="142"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="164"/>
       <c r="J17" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="141" t="s">
-        <v>537</v>
+      <c r="A18" s="143" t="s">
+        <v>540</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="140"/>
-      <c r="D18" s="166"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="162"/>
-      <c r="I18" s="163"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="168"/>
+      <c r="E18" s="160"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="142"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="164"/>
       <c r="J18" s="12" t="s">
         <v>15</v>
       </c>
@@ -4756,51 +4784,51 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="167"/>
+      <c r="A1" s="169"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="168" t="s">
+      <c r="D1" s="170" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B2" s="118"/>
       <c r="C2" s="118"/>
       <c r="D2" s="111"/>
     </row>
     <row r="3">
-      <c r="A3" s="141" t="s">
-        <v>540</v>
+      <c r="A3" s="143" t="s">
+        <v>543</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="169" t="s">
+      <c r="C3" s="171" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="169" t="s">
+      <c r="E3" s="171" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="141" t="s">
-        <v>541</v>
+      <c r="A4" s="143" t="s">
+        <v>544</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="162"/>
+      <c r="C4" s="163"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="169" t="s">
+      <c r="E4" s="171" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4873,414 +4901,414 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="170" t="s">
+      <c r="D1" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170" t="s">
+      <c r="E1" s="172"/>
+      <c r="F1" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170" t="s">
-        <v>542</v>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="170"/>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
+      <c r="A2" s="172"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
     </row>
     <row r="3">
-      <c r="A3" s="170"/>
-      <c r="B3" s="170"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
+      <c r="A3" s="172"/>
+      <c r="B3" s="172"/>
+      <c r="C3" s="173"/>
+      <c r="D3" s="173"/>
+      <c r="E3" s="173"/>
+      <c r="F3" s="173"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="173"/>
     </row>
     <row r="4">
-      <c r="A4" s="170" t="s">
-        <v>543</v>
-      </c>
-      <c r="B4" s="172" t="s">
-        <v>544</v>
-      </c>
-      <c r="C4" s="171"/>
-      <c r="D4" s="172" t="s">
-        <v>545</v>
-      </c>
-      <c r="E4" s="171"/>
-      <c r="F4" s="172" t="s">
+      <c r="A4" s="172" t="s">
         <v>546</v>
       </c>
-      <c r="G4" s="172" t="s">
+      <c r="B4" s="174" t="s">
         <v>547</v>
       </c>
-      <c r="H4" s="173"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="174" t="s">
+        <v>548</v>
+      </c>
+      <c r="E4" s="173"/>
+      <c r="F4" s="174" t="s">
+        <v>549</v>
+      </c>
+      <c r="G4" s="174" t="s">
+        <v>550</v>
+      </c>
+      <c r="H4" s="175"/>
     </row>
     <row r="5">
-      <c r="A5" s="170"/>
-      <c r="B5" s="170"/>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="171"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="173"/>
+      <c r="A5" s="172"/>
+      <c r="B5" s="172"/>
+      <c r="C5" s="173"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="173"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="175"/>
     </row>
     <row r="6">
-      <c r="A6" s="170"/>
-      <c r="B6" s="174" t="s">
-        <v>548</v>
-      </c>
-      <c r="C6" s="172" t="s">
-        <v>549</v>
-      </c>
-      <c r="D6" s="172" t="s">
-        <v>550</v>
-      </c>
-      <c r="E6" s="171"/>
-      <c r="F6" s="174" t="s">
+      <c r="A6" s="172"/>
+      <c r="B6" s="176" t="s">
         <v>551</v>
       </c>
-      <c r="G6" s="172" t="s">
+      <c r="C6" s="174" t="s">
         <v>552</v>
       </c>
-      <c r="H6" s="173"/>
+      <c r="D6" s="174" t="s">
+        <v>553</v>
+      </c>
+      <c r="E6" s="173"/>
+      <c r="F6" s="176" t="s">
+        <v>554</v>
+      </c>
+      <c r="G6" s="174" t="s">
+        <v>555</v>
+      </c>
+      <c r="H6" s="175"/>
     </row>
     <row r="7">
-      <c r="A7" s="170"/>
-      <c r="B7" s="170"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="172" t="s">
-        <v>553</v>
-      </c>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
+      <c r="A7" s="172"/>
+      <c r="B7" s="172"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="174" t="s">
+        <v>556</v>
+      </c>
+      <c r="E7" s="173"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="172"/>
+      <c r="H7" s="172"/>
     </row>
     <row r="8">
-      <c r="A8" s="170"/>
-      <c r="B8" s="170"/>
-      <c r="C8" s="170" t="s">
-        <v>554</v>
-      </c>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="170" t="s">
-        <v>555</v>
-      </c>
-      <c r="H8" s="170" t="s">
+      <c r="A8" s="172"/>
+      <c r="B8" s="172"/>
+      <c r="C8" s="172" t="s">
+        <v>557</v>
+      </c>
+      <c r="D8" s="173"/>
+      <c r="E8" s="173"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="172" t="s">
+        <v>558</v>
+      </c>
+      <c r="H8" s="172" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="170"/>
-      <c r="B9" s="170"/>
-      <c r="C9" s="175" t="s">
+      <c r="A9" s="172"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="177" t="s">
+        <v>559</v>
+      </c>
+      <c r="D9" s="173"/>
+      <c r="E9" s="173"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="173"/>
+      <c r="H9" s="178"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="172"/>
+      <c r="B10" s="174" t="s">
+        <v>560</v>
+      </c>
+      <c r="C10" s="174" t="s">
+        <v>561</v>
+      </c>
+      <c r="D10" s="173"/>
+      <c r="E10" s="174" t="s">
+        <v>562</v>
+      </c>
+      <c r="F10" s="173"/>
+      <c r="G10" s="174" t="s">
+        <v>563</v>
+      </c>
+      <c r="H10" s="175"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="172"/>
+      <c r="B11" s="172"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="173"/>
+      <c r="E11" s="174" t="s">
+        <v>564</v>
+      </c>
+      <c r="F11" s="173"/>
+      <c r="G11" s="172"/>
+      <c r="H11" s="175"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="172"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="174" t="s">
+        <v>565</v>
+      </c>
+      <c r="F12" s="173"/>
+      <c r="G12" s="172"/>
+      <c r="H12" s="175"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="172"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="172"/>
+      <c r="D13" s="174" t="s">
         <v>556</v>
       </c>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="176"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="170"/>
-      <c r="B10" s="172" t="s">
-        <v>557</v>
-      </c>
-      <c r="C10" s="172" t="s">
-        <v>558</v>
-      </c>
-      <c r="D10" s="171"/>
-      <c r="E10" s="172" t="s">
-        <v>559</v>
-      </c>
-      <c r="F10" s="171"/>
-      <c r="G10" s="172" t="s">
-        <v>560</v>
-      </c>
-      <c r="H10" s="173"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="170"/>
-      <c r="B11" s="170"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="172" t="s">
-        <v>561</v>
-      </c>
-      <c r="F11" s="171"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="173"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="170"/>
-      <c r="B12" s="170"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="172" t="s">
-        <v>562</v>
-      </c>
-      <c r="F12" s="171"/>
-      <c r="G12" s="170"/>
-      <c r="H12" s="173"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="170"/>
-      <c r="B13" s="170"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="172" t="s">
-        <v>553</v>
-      </c>
-      <c r="E13" s="170"/>
-      <c r="F13" s="171"/>
-      <c r="G13" s="170"/>
-      <c r="H13" s="173"/>
+      <c r="E13" s="172"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="172"/>
+      <c r="H13" s="175"/>
     </row>
     <row r="14">
-      <c r="A14" s="170"/>
-      <c r="B14" s="170"/>
-      <c r="C14" s="172" t="s">
-        <v>563</v>
-      </c>
-      <c r="D14" s="171"/>
-      <c r="E14" s="172" t="s">
-        <v>564</v>
-      </c>
-      <c r="F14" s="171"/>
-      <c r="G14" s="171"/>
-      <c r="H14" s="173"/>
+      <c r="A14" s="172"/>
+      <c r="B14" s="172"/>
+      <c r="C14" s="174" t="s">
+        <v>566</v>
+      </c>
+      <c r="D14" s="173"/>
+      <c r="E14" s="174" t="s">
+        <v>567</v>
+      </c>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="175"/>
     </row>
     <row r="15">
-      <c r="A15" s="170"/>
-      <c r="B15" s="170"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172" t="s">
-        <v>565</v>
-      </c>
-      <c r="F15" s="171"/>
-      <c r="G15" s="171"/>
-      <c r="H15" s="173"/>
+      <c r="A15" s="172"/>
+      <c r="B15" s="172"/>
+      <c r="C15" s="172"/>
+      <c r="D15" s="173"/>
+      <c r="E15" s="174" t="s">
+        <v>568</v>
+      </c>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="175"/>
     </row>
     <row r="16">
-      <c r="A16" s="170"/>
-      <c r="B16" s="170"/>
-      <c r="C16" s="174" t="s">
-        <v>566</v>
-      </c>
-      <c r="D16" s="171"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="171"/>
-      <c r="G16" s="174" t="s">
-        <v>567</v>
-      </c>
-      <c r="H16" s="177"/>
+      <c r="A16" s="172"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="176" t="s">
+        <v>569</v>
+      </c>
+      <c r="D16" s="173"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="176" t="s">
+        <v>570</v>
+      </c>
+      <c r="H16" s="179"/>
     </row>
     <row r="17">
-      <c r="A17" s="170"/>
-      <c r="B17" s="172" t="s">
-        <v>568</v>
-      </c>
-      <c r="C17" s="172" t="s">
-        <v>569</v>
-      </c>
-      <c r="D17" s="171"/>
-      <c r="E17" s="172" t="s">
+      <c r="A17" s="172"/>
+      <c r="B17" s="174" t="s">
+        <v>571</v>
+      </c>
+      <c r="C17" s="174" t="s">
+        <v>572</v>
+      </c>
+      <c r="D17" s="173"/>
+      <c r="E17" s="174" t="s">
+        <v>573</v>
+      </c>
+      <c r="F17" s="173"/>
+      <c r="G17" s="174" t="s">
+        <v>574</v>
+      </c>
+      <c r="H17" s="175"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="172"/>
+      <c r="B18" s="172"/>
+      <c r="C18" s="172"/>
+      <c r="D18" s="173"/>
+      <c r="E18" s="174" t="s">
+        <v>575</v>
+      </c>
+      <c r="F18" s="173"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="175"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="172"/>
+      <c r="B19" s="172"/>
+      <c r="C19" s="172"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="174" t="s">
+        <v>576</v>
+      </c>
+      <c r="F19" s="173"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="175"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="172"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="174" t="s">
+        <v>577</v>
+      </c>
+      <c r="D20" s="173"/>
+      <c r="E20" s="174" t="s">
+        <v>578</v>
+      </c>
+      <c r="F20" s="172"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="175"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="172"/>
+      <c r="B21" s="172"/>
+      <c r="C21" s="174" t="s">
+        <v>579</v>
+      </c>
+      <c r="D21" s="173"/>
+      <c r="E21" s="174" t="s">
+        <v>580</v>
+      </c>
+      <c r="F21" s="173"/>
+      <c r="G21" s="173"/>
+      <c r="H21" s="175"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="172"/>
+      <c r="B22" s="177" t="s">
+        <v>581</v>
+      </c>
+      <c r="C22" s="177" t="s">
+        <v>582</v>
+      </c>
+      <c r="D22" s="173"/>
+      <c r="E22" s="177" t="s">
+        <v>583</v>
+      </c>
+      <c r="F22" s="173"/>
+      <c r="G22" s="173"/>
+      <c r="H22" s="178"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="172"/>
+      <c r="B23" s="172"/>
+      <c r="C23" s="177" t="s">
+        <v>584</v>
+      </c>
+      <c r="D23" s="173"/>
+      <c r="E23" s="172"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="173"/>
+      <c r="H23" s="178"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="172"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="177" t="s">
+        <v>585</v>
+      </c>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="178"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="172"/>
+      <c r="B25" s="172"/>
+      <c r="C25" s="177" t="s">
+        <v>586</v>
+      </c>
+      <c r="D25" s="173"/>
+      <c r="E25" s="173"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="173"/>
+      <c r="H25" s="178"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="172"/>
+      <c r="B26" s="172" t="s">
+        <v>587</v>
+      </c>
+      <c r="C26" s="173"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="172" t="s">
+        <v>588</v>
+      </c>
+      <c r="F26" s="173"/>
+      <c r="G26" s="172" t="s">
         <v>570</v>
       </c>
-      <c r="F17" s="171"/>
-      <c r="G17" s="172" t="s">
-        <v>571</v>
-      </c>
-      <c r="H17" s="173"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="170"/>
-      <c r="B18" s="170"/>
-      <c r="C18" s="170"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172" t="s">
-        <v>572</v>
-      </c>
-      <c r="F18" s="171"/>
-      <c r="G18" s="170"/>
-      <c r="H18" s="173"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="170"/>
-      <c r="B19" s="170"/>
-      <c r="C19" s="170"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172" t="s">
-        <v>573</v>
-      </c>
-      <c r="F19" s="171"/>
-      <c r="G19" s="171"/>
-      <c r="H19" s="173"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="170"/>
-      <c r="B20" s="170"/>
-      <c r="C20" s="172" t="s">
-        <v>574</v>
-      </c>
-      <c r="D20" s="171"/>
-      <c r="E20" s="172" t="s">
-        <v>575</v>
-      </c>
-      <c r="F20" s="170"/>
-      <c r="G20" s="170"/>
-      <c r="H20" s="173"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="170"/>
-      <c r="B21" s="170"/>
-      <c r="C21" s="172" t="s">
-        <v>576</v>
-      </c>
-      <c r="D21" s="171"/>
-      <c r="E21" s="172" t="s">
-        <v>577</v>
-      </c>
-      <c r="F21" s="171"/>
-      <c r="G21" s="171"/>
-      <c r="H21" s="173"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="170"/>
-      <c r="B22" s="175" t="s">
-        <v>578</v>
-      </c>
-      <c r="C22" s="175" t="s">
-        <v>579</v>
-      </c>
-      <c r="D22" s="171"/>
-      <c r="E22" s="175" t="s">
-        <v>580</v>
-      </c>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="176"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="170"/>
-      <c r="B23" s="170"/>
-      <c r="C23" s="175" t="s">
-        <v>581</v>
-      </c>
-      <c r="D23" s="171"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="171"/>
-      <c r="G23" s="171"/>
-      <c r="H23" s="176"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="170"/>
-      <c r="B24" s="170"/>
-      <c r="C24" s="175" t="s">
-        <v>582</v>
-      </c>
-      <c r="D24" s="171"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="171"/>
-      <c r="G24" s="171"/>
-      <c r="H24" s="176"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="170"/>
-      <c r="B25" s="170"/>
-      <c r="C25" s="175" t="s">
-        <v>583</v>
-      </c>
-      <c r="D25" s="171"/>
-      <c r="E25" s="171"/>
-      <c r="F25" s="171"/>
-      <c r="G25" s="171"/>
-      <c r="H25" s="176"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="170"/>
-      <c r="B26" s="170" t="s">
-        <v>584</v>
-      </c>
-      <c r="C26" s="171"/>
-      <c r="D26" s="171"/>
-      <c r="E26" s="170" t="s">
-        <v>585</v>
-      </c>
-      <c r="F26" s="171"/>
-      <c r="G26" s="170" t="s">
-        <v>567</v>
-      </c>
-      <c r="H26" s="170" t="s">
+      <c r="H26" s="172" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="170"/>
-      <c r="B27" s="172" t="s">
-        <v>586</v>
-      </c>
-      <c r="C27" s="171"/>
-      <c r="D27" s="171"/>
-      <c r="E27" s="171"/>
-      <c r="F27" s="171"/>
-      <c r="G27" s="174" t="s">
-        <v>567</v>
-      </c>
-      <c r="H27" s="173"/>
+      <c r="A27" s="172"/>
+      <c r="B27" s="174" t="s">
+        <v>589</v>
+      </c>
+      <c r="C27" s="173"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="173"/>
+      <c r="F27" s="173"/>
+      <c r="G27" s="176" t="s">
+        <v>570</v>
+      </c>
+      <c r="H27" s="175"/>
     </row>
     <row r="28">
-      <c r="A28" s="170"/>
-      <c r="B28" s="175" t="s">
-        <v>587</v>
-      </c>
-      <c r="C28" s="171"/>
-      <c r="D28" s="170" t="s">
-        <v>588</v>
-      </c>
-      <c r="E28" s="171"/>
-      <c r="F28" s="171"/>
-      <c r="G28" s="178"/>
-      <c r="H28" s="176"/>
+      <c r="A28" s="172"/>
+      <c r="B28" s="177" t="s">
+        <v>590</v>
+      </c>
+      <c r="C28" s="173"/>
+      <c r="D28" s="172" t="s">
+        <v>591</v>
+      </c>
+      <c r="E28" s="173"/>
+      <c r="F28" s="173"/>
+      <c r="G28" s="180"/>
+      <c r="H28" s="178"/>
     </row>
     <row r="29">
-      <c r="A29" s="170"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="170"/>
-      <c r="E29" s="171"/>
-      <c r="F29" s="171"/>
-      <c r="G29" s="178"/>
-      <c r="H29" s="176"/>
+      <c r="A29" s="172"/>
+      <c r="B29" s="172"/>
+      <c r="C29" s="172"/>
+      <c r="D29" s="172"/>
+      <c r="E29" s="173"/>
+      <c r="F29" s="173"/>
+      <c r="G29" s="180"/>
+      <c r="H29" s="178"/>
     </row>
     <row r="30">
-      <c r="A30" s="170" t="s">
-        <v>589</v>
-      </c>
-      <c r="B30" s="170"/>
-      <c r="C30" s="171"/>
-      <c r="D30" s="171"/>
-      <c r="E30" s="171"/>
-      <c r="F30" s="171"/>
-      <c r="G30" s="171"/>
-      <c r="H30" s="176"/>
+      <c r="A30" s="172" t="s">
+        <v>592</v>
+      </c>
+      <c r="B30" s="172"/>
+      <c r="C30" s="173"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="173"/>
+      <c r="F30" s="173"/>
+      <c r="G30" s="173"/>
+      <c r="H30" s="178"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5313,105 +5341,105 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="179" t="str">
+      <c r="A2" s="181" t="str">
         <f>HYPERLINK("http://www.isg.rhul.ac.uk/tls/Lucky13.html","Lucky 13")</f>
         <v>Lucky 13</v>
       </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
     </row>
     <row r="3">
-      <c r="A3" s="181" t="str">
+      <c r="A3" s="183" t="str">
         <f>HYPERLINK("https://nerdoholic.org/uploads/dergln/beast_part2/ssl_jun21.pdf","BEAST")</f>
         <v>BEAST</v>
       </c>
-      <c r="B3" s="180"/>
+      <c r="B3" s="182"/>
     </row>
     <row r="4">
-      <c r="A4" s="179" t="str">
+      <c r="A4" s="181" t="str">
         <f>HYPERLINK("https://sweet32.info/","Sweet32")</f>
         <v>Sweet32</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="182"/>
     </row>
     <row r="5">
-      <c r="A5" s="182" t="s">
-        <v>590</v>
-      </c>
-      <c r="B5" s="180"/>
-      <c r="C5" s="180"/>
-      <c r="D5" s="180"/>
+      <c r="A5" s="184" t="s">
+        <v>593</v>
+      </c>
+      <c r="B5" s="182"/>
+      <c r="C5" s="182"/>
+      <c r="D5" s="182"/>
     </row>
     <row r="6">
-      <c r="A6" s="179" t="str">
+      <c r="A6" s="181" t="str">
         <f>HYPERLINK("http://breachattack.com/","BREACH")</f>
         <v>BREACH</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="179" t="str">
+      <c r="A7" s="181" t="str">
         <f>HYPERLINK("https://security.googleblog.com/2014/10/this-poodle-bites-exploiting-ssl-30.html","POODLE")</f>
         <v>POODLE</v>
       </c>
-      <c r="B7" s="180"/>
-      <c r="D7" s="180"/>
+      <c r="B7" s="182"/>
+      <c r="D7" s="182"/>
     </row>
     <row r="8">
-      <c r="A8" s="179" t="str">
+      <c r="A8" s="181" t="str">
         <f>HYPERLINK("https://mitls.org/pages/attacks/3SHAKE","3SHAKE")</f>
         <v>3SHAKE</v>
       </c>
-      <c r="B8" s="180"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
+      <c r="B8" s="182"/>
+      <c r="C8" s="182"/>
+      <c r="D8" s="182"/>
     </row>
     <row r="9">
-      <c r="A9" s="179" t="str">
+      <c r="A9" s="181" t="str">
         <f>HYPERLINK("https://drownattack.com/","DROWN")</f>
         <v>DROWN</v>
       </c>
-      <c r="D9" s="180"/>
+      <c r="D9" s="182"/>
     </row>
     <row r="10">
-      <c r="A10" s="179" t="str">
+      <c r="A10" s="181" t="str">
         <f>HYPERLINK("https://robotattack.org/","ROBOT ")</f>
         <v>ROBOT </v>
       </c>
-      <c r="B10" s="180"/>
-      <c r="D10" s="180"/>
+      <c r="B10" s="182"/>
+      <c r="D10" s="182"/>
     </row>
     <row r="11">
-      <c r="A11" s="179" t="str">
+      <c r="A11" s="181" t="str">
         <f>HYPERLINK("https://www.kb.cert.org/vuls/id/120541/","Renegotiation attack")</f>
         <v>Renegotiation attack</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="183" t="s">
-        <v>591</v>
-      </c>
-      <c r="D12" s="180"/>
+      <c r="A12" s="185" t="s">
+        <v>594</v>
+      </c>
+      <c r="D12" s="182"/>
     </row>
     <row r="13">
-      <c r="A13" s="183" t="s">
-        <v>592</v>
-      </c>
-      <c r="B13" s="180"/>
-      <c r="C13" s="180"/>
-      <c r="D13" s="180"/>
+      <c r="A13" s="185" t="s">
+        <v>595</v>
+      </c>
+      <c r="B13" s="182"/>
+      <c r="C13" s="182"/>
+      <c r="D13" s="182"/>
     </row>
     <row r="14">
-      <c r="A14" s="183" t="s">
-        <v>593</v>
-      </c>
-      <c r="D14" s="180"/>
+      <c r="A14" s="185" t="s">
+        <v>596</v>
+      </c>
+      <c r="D14" s="182"/>
     </row>
     <row r="15">
-      <c r="A15" s="183" t="s">
-        <v>594</v>
-      </c>
-      <c r="B15" s="180"/>
+      <c r="A15" s="185" t="s">
+        <v>597</v>
+      </c>
+      <c r="B15" s="182"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12059,7 +12087,9 @@
       <c r="I38" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J38" s="21"/>
+      <c r="J38" s="79" t="s">
+        <v>389</v>
+      </c>
       <c r="K38" s="21" t="s">
         <v>23</v>
       </c>
@@ -25490,9 +25520,9 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3 K3:L994 G5:G8 I7:J7 G13:G14 I13:J13 G16 I16 I18:J18 G20:G21 G25:G26 I25:J26 G29:G33 G36:G994 I40:J994">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -27500,9 +27530,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.75"/>
+    <col customWidth="1" min="3" max="3" width="10.5"/>
     <col customWidth="1" min="4" max="4" width="13.75"/>
-    <col customWidth="1" min="5" max="5" width="25.5"/>
+    <col customWidth="1" min="5" max="5" width="49.5"/>
     <col customWidth="1" min="6" max="6" width="13.75"/>
+    <col customWidth="1" min="7" max="7" width="55.63"/>
+    <col customWidth="1" min="8" max="8" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
@@ -27521,10 +27554,11 @@
       <c r="F1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="117" t="s">
+      <c r="I1" s="117" t="s">
         <v>30</v>
       </c>
     </row>
@@ -27536,15 +27570,18 @@
       <c r="E2" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="119" t="s">
+      <c r="F2" s="123"/>
+      <c r="G2" s="125" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="108"/>
+      <c r="I2" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="119" t="s">
+      <c r="J2" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="119" t="s">
+      <c r="K2" s="119" t="s">
         <v>11</v>
       </c>
     </row>
@@ -27561,20 +27598,21 @@
       <c r="D3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="126"/>
+      <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27591,28 +27629,31 @@
       <c r="D4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>482</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="126" t="s">
+        <v>483</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="93" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B5" s="93">
         <v>2.0</v>
@@ -27620,17 +27661,17 @@
       <c r="C5" s="93">
         <v>1.2</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>484</v>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>15</v>
+      <c r="G5" s="126" t="s">
+        <v>486</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>15</v>
@@ -27639,12 +27680,15 @@
         <v>15</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="93" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B6" s="93">
         <v>3.0</v>
@@ -27655,22 +27699,25 @@
       <c r="D6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>486</v>
+      <c r="E6" s="7" t="s">
+        <v>488</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="126" t="s">
+        <v>489</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="I6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27680,26 +27727,26 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:J6">
+  <conditionalFormatting sqref="D3:K6">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"must not"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:J6">
+  <conditionalFormatting sqref="D3:K6">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"recommended"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:J6">
+  <conditionalFormatting sqref="D3:K6">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"not recommended"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:J6">
+  <conditionalFormatting sqref="D3:K6">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"must"</formula>
     </cfRule>
@@ -27734,70 +27781,70 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="125" t="s">
-        <v>487</v>
-      </c>
-      <c r="B1" s="125" t="s">
-        <v>488</v>
+      <c r="A1" s="127" t="s">
+        <v>490</v>
+      </c>
+      <c r="B1" s="127" t="s">
+        <v>491</v>
       </c>
       <c r="C1" s="83" t="s">
-        <v>489</v>
-      </c>
-      <c r="D1" s="126" t="s">
+        <v>492</v>
+      </c>
+      <c r="D1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="127"/>
-      <c r="F1" s="128" t="s">
+      <c r="E1" s="129"/>
+      <c r="F1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="127"/>
-      <c r="H1" s="128" t="s">
-        <v>490</v>
-      </c>
-      <c r="I1" s="127"/>
-      <c r="J1" s="128" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="130" t="s">
+        <v>493</v>
+      </c>
+      <c r="I1" s="129"/>
+      <c r="J1" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="129"/>
-      <c r="L1" s="130" t="s">
+      <c r="K1" s="131"/>
+      <c r="L1" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
     </row>
     <row r="2">
       <c r="A2" s="108"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
       <c r="D2" s="111"/>
-      <c r="E2" s="127" t="s">
-        <v>491</v>
+      <c r="E2" s="129" t="s">
+        <v>494</v>
       </c>
       <c r="F2" s="111"/>
-      <c r="G2" s="127" t="s">
-        <v>491</v>
+      <c r="G2" s="129" t="s">
+        <v>494</v>
       </c>
       <c r="H2" s="111"/>
-      <c r="I2" s="127" t="s">
-        <v>491</v>
+      <c r="I2" s="129" t="s">
+        <v>494</v>
       </c>
       <c r="J2" s="111"/>
-      <c r="K2" s="127" t="s">
-        <v>491</v>
-      </c>
-      <c r="L2" s="132" t="s">
+      <c r="K2" s="129" t="s">
+        <v>494</v>
+      </c>
+      <c r="L2" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="132" t="s">
+      <c r="M2" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="132" t="s">
+      <c r="N2" s="134" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="133" t="s">
-        <v>492</v>
+      <c r="A3" s="135" t="s">
+        <v>495</v>
       </c>
       <c r="B3" s="98" t="s">
         <v>39</v>
@@ -27808,17 +27855,17 @@
       <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="134" t="s">
-        <v>493</v>
-      </c>
-      <c r="F3" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="136"/>
-      <c r="H3" s="137" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="136"/>
+      <c r="E3" s="136" t="s">
+        <v>496</v>
+      </c>
+      <c r="F3" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="138"/>
+      <c r="H3" s="139" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="138"/>
       <c r="J3" s="22" t="s">
         <v>15</v>
       </c>
@@ -27840,26 +27887,26 @@
       <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="134" t="s">
-        <v>494</v>
+      <c r="E4" s="136" t="s">
+        <v>497</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="136" t="s">
-        <v>495</v>
+      <c r="G4" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="136" t="s">
-        <v>495</v>
+      <c r="I4" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="79" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="L4" s="30" t="s">
         <v>15</v>
@@ -27873,34 +27920,34 @@
     </row>
     <row r="5">
       <c r="B5" s="98" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C5" s="93">
         <v>-1.0</v>
       </c>
-      <c r="D5" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="134"/>
-      <c r="F5" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="136"/>
-      <c r="H5" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="136"/>
-      <c r="J5" s="135" t="s">
+      <c r="D5" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="136"/>
+      <c r="F5" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="138"/>
+      <c r="H5" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="138"/>
+      <c r="J5" s="137" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="79"/>
-      <c r="L5" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="135" t="s">
+      <c r="L5" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="137" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27914,17 +27961,17 @@
       <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="134" t="s">
-        <v>493</v>
+      <c r="E6" s="136" t="s">
+        <v>496</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="136"/>
+      <c r="G6" s="138"/>
       <c r="H6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="136"/>
+      <c r="I6" s="138"/>
       <c r="J6" s="22" t="s">
         <v>15</v>
       </c>
@@ -27946,20 +27993,20 @@
       <c r="D7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="134" t="s">
-        <v>494</v>
+      <c r="E7" s="136" t="s">
+        <v>497</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="136" t="s">
-        <v>495</v>
+      <c r="G7" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="136" t="s">
-        <v>495</v>
+      <c r="I7" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>15</v>
@@ -27985,24 +28032,24 @@
       <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="134" t="s">
-        <v>493</v>
+      <c r="E8" s="136" t="s">
+        <v>496</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="136" t="s">
+      <c r="G8" s="138" t="s">
         <v>436</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="136"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="11" t="s">
         <v>18</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="L8" s="30" t="s">
         <v>15</v>
@@ -28021,20 +28068,20 @@
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="134" t="s">
-        <v>494</v>
+      <c r="E9" s="136" t="s">
+        <v>497</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="136" t="s">
-        <v>495</v>
+      <c r="G9" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="136" t="s">
-        <v>495</v>
+      <c r="I9" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="J9" s="22" t="s">
         <v>15</v>
@@ -28054,18 +28101,18 @@
       <c r="C10" s="93">
         <v>1024.0</v>
       </c>
-      <c r="D10" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="136"/>
-      <c r="F10" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="136"/>
-      <c r="H10" s="137" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="136"/>
+      <c r="D10" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="138"/>
+      <c r="F10" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="138"/>
+      <c r="H10" s="139" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="138"/>
       <c r="J10" s="22" t="s">
         <v>15</v>
       </c>
@@ -28081,27 +28128,27 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="133" t="s">
-        <v>497</v>
+      <c r="A11" s="135" t="s">
+        <v>500</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="C11" s="93">
         <v>224.0</v>
       </c>
-      <c r="D11" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="136"/>
-      <c r="F11" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="136"/>
-      <c r="H11" s="137" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="136"/>
+      <c r="D11" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="138"/>
+      <c r="F11" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="138"/>
+      <c r="H11" s="139" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="138"/>
       <c r="J11" s="22" t="s">
         <v>15</v>
       </c>
@@ -28120,21 +28167,21 @@
       <c r="C12" s="93">
         <v>256.0</v>
       </c>
-      <c r="D12" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="136"/>
+      <c r="D12" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="138"/>
       <c r="F12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="136" t="s">
-        <v>495</v>
+      <c r="G12" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="136" t="s">
-        <v>495</v>
+      <c r="I12" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="J12" s="22" t="s">
         <v>15</v>
@@ -28152,31 +28199,31 @@
     </row>
     <row r="13">
       <c r="B13" s="98" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C13" s="93">
         <v>1024.0</v>
       </c>
-      <c r="D13" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="136"/>
-      <c r="F13" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="136"/>
-      <c r="H13" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="136"/>
-      <c r="J13" s="135" t="s">
+      <c r="D13" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="138"/>
+      <c r="F13" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="138"/>
+      <c r="H13" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="138"/>
+      <c r="J13" s="137" t="s">
         <v>15</v>
       </c>
       <c r="K13" s="22"/>
-      <c r="L13" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" s="135" t="s">
+      <c r="L13" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="137" t="s">
         <v>15</v>
       </c>
       <c r="N13" s="7" t="s">
@@ -28187,18 +28234,18 @@
       <c r="C14" s="93">
         <v>2048.0</v>
       </c>
-      <c r="D14" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="136"/>
+      <c r="D14" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="138"/>
       <c r="F14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="136"/>
+      <c r="G14" s="138"/>
       <c r="H14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="136"/>
+      <c r="I14" s="138"/>
       <c r="J14" s="22" t="s">
         <v>15</v>
       </c>
@@ -28217,21 +28264,21 @@
       <c r="C15" s="93">
         <v>3076.0</v>
       </c>
-      <c r="D15" s="135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="136"/>
+      <c r="D15" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="138"/>
       <c r="F15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="136" t="s">
-        <v>495</v>
+      <c r="G15" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="136" t="s">
-        <v>495</v>
+      <c r="I15" s="138" t="s">
+        <v>498</v>
       </c>
       <c r="J15" s="22" t="s">
         <v>15</v>
@@ -28319,131 +28366,131 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="138" t="s">
-        <v>500</v>
-      </c>
-      <c r="B1" s="139" t="s">
+      <c r="A1" s="140" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" s="141" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="108"/>
-      <c r="D1" s="139" t="s">
+      <c r="D1" s="141" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="108"/>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="141" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="108"/>
       <c r="H1" s="9" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="140"/>
+      <c r="A2" s="142"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="141" t="s">
-        <v>502</v>
-      </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="141" t="s">
-        <v>502</v>
+      <c r="C2" s="143" t="s">
+        <v>505</v>
+      </c>
+      <c r="D2" s="144"/>
+      <c r="E2" s="143" t="s">
+        <v>505</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="143" t="s">
-        <v>502</v>
-      </c>
-      <c r="H2" s="144"/>
+      <c r="G2" s="145" t="s">
+        <v>505</v>
+      </c>
+      <c r="H2" s="146"/>
     </row>
     <row r="3">
-      <c r="A3" s="141" t="s">
-        <v>503</v>
+      <c r="A3" s="143" t="s">
+        <v>506</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="141" t="s">
-        <v>504</v>
+      <c r="C3" s="143" t="s">
+        <v>507</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="140"/>
+      <c r="E3" s="142"/>
       <c r="F3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="145"/>
+      <c r="G3" s="147"/>
       <c r="H3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="146" t="s">
-        <v>505</v>
+      <c r="A4" s="148" t="s">
+        <v>508</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="147" t="s">
-        <v>506</v>
+      <c r="C4" s="149" t="s">
+        <v>509</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="147" t="s">
-        <v>507</v>
+      <c r="E4" s="149" t="s">
+        <v>510</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="145"/>
+      <c r="G4" s="147"/>
       <c r="H4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="141" t="s">
-        <v>508</v>
+      <c r="A5" s="143" t="s">
+        <v>511</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="147" t="s">
-        <v>509</v>
+      <c r="C5" s="149" t="s">
+        <v>512</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="147" t="s">
-        <v>509</v>
+      <c r="E5" s="149" t="s">
+        <v>512</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="145"/>
+      <c r="G5" s="147"/>
       <c r="H5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="141" t="s">
-        <v>510</v>
+      <c r="A6" s="143" t="s">
+        <v>513</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="147" t="s">
-        <v>506</v>
+      <c r="C6" s="149" t="s">
+        <v>509</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="147" t="s">
-        <v>511</v>
+      <c r="E6" s="149" t="s">
+        <v>514</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="145"/>
+      <c r="G6" s="147"/>
       <c r="H6" s="12" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added post_actions to configuration_generator and fixed issues with generated confs
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -1005,7 +1005,11 @@
     </comment>
     <comment authorId="0" ref="E4">
       <text>
-        <t xml:space="preserve">use wildcards in CN</t>
+        <t xml:space="preserve">use wildcards in CN
+----
+questo sistema è in fase di test
+L'idea è fornire delle keyword tipo {cert} che possono essere inserite nelle note condizionali per mostrare il problema incontrato. Per applicare questa cosa la nota va prima del controllo
+	-Riccardo Germenia</t>
       </text>
     </comment>
     <comment authorId="0" ref="C6">
@@ -1015,10 +1019,7 @@
     </comment>
     <comment authorId="0" ref="E6">
       <text>
-        <t xml:space="preserve">use wildcards in CN
-----
-dato che NON DEVE avere le wildcards nel campo nella condizione va verificato sele contiene. Se le contiene risulta il livello must not
-	-Riccardo Germenia</t>
+        <t xml:space="preserve">use wildcards in CN</t>
       </text>
     </comment>
   </commentList>
@@ -1325,7 +1326,7 @@
     <t>0x00,0x39</t>
   </si>
   <si>
-    <t>TLS_DHE_DSS_WITH_AES_128_GCM_SHA256 (0x00, 0xA2)</t>
+    <t>TLS_DHE_DSS_WITH_AES_128_GCM_SHA256</t>
   </si>
   <si>
     <t>0x00,0xA2</t>
@@ -1334,7 +1335,7 @@
     <t>DSA</t>
   </si>
   <si>
-    <t>TLS_DHE_DSS_WITH_AES_256_GCM_SHA384 (0x00, 0xA3)</t>
+    <t>TLS_DHE_DSS_WITH_AES_256_GCM_SHA384</t>
   </si>
   <si>
     <t>0x00,0xA3</t>
@@ -2075,7 +2076,7 @@
     <t>truncated_hmac</t>
   </si>
   <si>
-    <t>CIPHER CBC and VLP false and NOTE should only be used if the server communicates with constrained-device clients</t>
+    <t>CIPHER CBC and VLP false and NOTE_ENABLED should only be used if the server communicates with constrained-device clients</t>
   </si>
   <si>
     <t>status_request</t>
@@ -2549,7 +2550,7 @@
     <t>X.509 version</t>
   </si>
   <si>
-    <t>NOTE_FALSE {reason} and VALUE Certificate X.509 version == 2</t>
+    <t>VALUE Certificate X.509 version == 2</t>
   </si>
   <si>
     <t>Issuer Distinguished Name</t>
@@ -11157,7 +11158,7 @@
       <c r="G7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="77" t="s">
         <v>349</v>
       </c>
       <c r="I7" s="21" t="s">

</xml_diff>

<commit_message>
Added groups support to configuration generator
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -590,6 +590,12 @@
         <t xml:space="preserve">Use up to year 2022</t>
       </text>
     </comment>
+    <comment authorId="0" ref="A24">
+      <text>
+        <t xml:space="preserve">la x qui era minuscola, nello standard è maiuscola
+	-Riccardo Germenia</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -2310,10 +2316,10 @@
     <t>brainpoolP512r1</t>
   </si>
   <si>
-    <t>x25519 / Curve25519</t>
-  </si>
-  <si>
-    <t>x448 / Curve448</t>
+    <t>X25519 / Curve25519</t>
+  </si>
+  <si>
+    <t>X448 / Curve448</t>
   </si>
   <si>
     <t>SignatureScheme</t>
@@ -3408,10 +3414,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>

</xml_diff>

<commit_message>
Fixed conditions for CertificateExtensions
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -90,10 +90,7 @@
     </comment>
     <comment authorId="0" ref="D3">
       <text>
-        <t xml:space="preserve">Same as subject key identifier in issuing CA certificate; Prohibited: Issuer DN, Serial Number tuple
-----
-todo fix this condition. Will create a new function
-	-Riccardo Germenia</t>
+        <t xml:space="preserve">Same as subject key identifier in issuing CA certificate; Prohibited: Issuer DN, Serial Number tuple</t>
       </text>
     </comment>
     <comment authorId="0" ref="H3">
@@ -108,7 +105,10 @@
     </comment>
     <comment authorId="0" ref="D4">
       <text>
-        <t xml:space="preserve">Same as in Public-Key Cryptography Standards (PKCS) 10 request or calculated by the issuing CA</t>
+        <t xml:space="preserve">Same as in Public-Key Cryptography Standards (PKCS) 10 request or calculated by the issuing CA
+----
+le parentesi nelle note danno problemi
+	-Riccardo Germenia</t>
       </text>
     </comment>
     <comment authorId="0" ref="A5">
@@ -141,18 +141,23 @@
     <comment authorId="0" ref="D6">
       <text>
         <t xml:space="preserve">id-kp-serverAuth {1 3 6 1 5 5 7 3 1}
-http://oid-info.com/get/1.3.6.1.5.5.7.3.1
-----
-si può compattare anche la riga sotto con la condiziona contains_not ma devo verificare che escano due note separate per le condizioni
-	-Riccardo Germenia
-http://oid-info.com/get/1.3.6.1.5.5.7.3.1
-	-Riccardo Germenia</t>
+http://oid-info.com/get/1.3.6.1.5.5.7.3.1</t>
       </text>
     </comment>
     <comment authorId="0" ref="H6">
       <text>
         <t xml:space="preserve">R28
 </t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A7">
+      <text>
+        <t xml:space="preserve">Extended Key Usage</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D7">
+      <text>
+        <t xml:space="preserve">the keyAgreement and keyEncipherments are considered mutually exclusive as show in section 5.4.3 of https://www.etsi.org/deliver/etsi_ts/102200_102299/102280/01.01.01_60/ts_102280v010101p.pdf</t>
       </text>
     </comment>
     <comment authorId="0" ref="A9">
@@ -212,11 +217,15 @@
     </comment>
     <comment authorId="0" ref="D13">
       <text>
-        <t xml:space="preserve">A CRL can be indicated in two ways:
-- DistributionPoint ::= SEQUENCE
-- DistributionPointName ::= CHOICE
-The certificate can only employ the DistributionPoint "SEQUENCE" type, using the "distributionPoint" field.
-The use of the two other fields ("reasons" and "cRLIssuer") or the other method "CHOICE" are forbidded</t>
+        <t xml:space="preserve">A CRL is indicated by a DistributionPoint ::= SEQUENCE.
+This SEQUENCE can contain three items:
+    distributionPoint: DistributionPointName
+    reasons: ReasonFlags
+    cRLIssuer: GeneralNames.
+The DistributionPointName type is a CHOICE with two options:
+    fullName
+    nameRelativeToCRLIssuer
+A valid distributionPoint must not have the "reasons" and "cRLIssuer" fields and the distributionPoint can not be of type nameRelativeToCRLIssuer</t>
       </text>
     </comment>
     <comment authorId="0" ref="A14">
@@ -233,10 +242,7 @@
     </comment>
     <comment authorId="0" ref="A15">
       <text>
-        <t xml:space="preserve">TLS Certificate Status Request
-----
-update: si deve usare OCSP_stapling e vedere se è offered o not offered
-	-Riccardo Germenia</t>
+        <t xml:space="preserve">TLS Certificate Status Request</t>
       </text>
     </comment>
     <comment authorId="0" ref="B15">
@@ -244,21 +250,25 @@
         <t xml:space="preserve">Optional. This extension (sometimes referred to as the “must staple” extension) may be present to indicate to clients that the server supports OCSP stapling and will provide a stapled OCSP response when one is requested.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B13">
+    <comment authorId="0" ref="D12">
       <text>
-        <t xml:space="preserve">CRL Distribution Points cercarlo dentro RFC per capire cosa si intende nel commento
+        <t xml:space="preserve">Possibilità:
+1) verificare se url è valido
+2) vedere se url risponde con 200
+3) verificare se è parte di una lista di crl "valide"
+	-Riccardo Germenia
+cert_crlDistributionPoints del dump di testssl contiene le informazioni. Se non contiene "http" allora non rispetta il criterio.
+	-Riccardo Germenia
+per ora controllo se contine i valori IP o URI che sono entrambi validi in teoria
 	-Riccardo Germenia</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A17">
+    <comment authorId="0" ref="A1">
       <text>
         <t xml:space="preserve">'authorityInfoAccess' contiene anche l'url dell'OCSP
-	-Riccardo Germenia</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A18">
-      <text>
-        <t xml:space="preserve">'crlDistributionPoints' se c'è questo campo in teoria c'è anche la CRL per la revoca
+	-Riccardo Germenia
+----
+'crlDistributionPoints' se c'è questo campo in teoria c'è anche la CRL per la revoca
 	-Riccardo Germenia</t>
       </text>
     </comment>
@@ -588,12 +598,6 @@
     <comment authorId="0" ref="H16">
       <text>
         <t xml:space="preserve">Use up to year 2022</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A24">
-      <text>
-        <t xml:space="preserve">la x qui era minuscola, nello standard è maiuscola
-	-Riccardo Germenia</t>
       </text>
     </comment>
   </commentList>
@@ -1011,11 +1015,7 @@
     </comment>
     <comment authorId="0" ref="E4">
       <text>
-        <t xml:space="preserve">use wildcards in CN
-----
-questo sistema è in fase di test
-L'idea è fornire delle keyword tipo {cert} che possono essere inserite nelle note condizionali per mostrare il problema incontrato. Per applicare questa cosa la nota va prima del controllo
-	-Riccardo Germenia</t>
+        <t xml:space="preserve">use wildcards in CN</t>
       </text>
     </comment>
     <comment authorId="0" ref="C6">
@@ -1033,7 +1033,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="598">
   <si>
     <t>NIST</t>
   </si>
@@ -2589,9 +2589,15 @@
     <t>authorityKeyIdentifier</t>
   </si>
   <si>
+    <t>CHECK_AKI</t>
+  </si>
+  <si>
     <t>subjectKeyIdentifier</t>
   </si>
   <si>
+    <t>NOTE_ALWAYS The guidelines state `Same as in Public-Key Cryptography Standards PKCS 10 request or calculated by the issuing CA`. The tool can not verify this condition since this specific check can only be performed by monitoring the endpoint during the certificate issuing phase</t>
+  </si>
+  <si>
     <t>keyUsage</t>
   </si>
   <si>
@@ -2604,10 +2610,10 @@
     <t>extendedKeyUsage</t>
   </si>
   <si>
-    <t>VALUE CertificateExtensions TLS Web Server Authentication in extendedKeyUsage AND VALUE CertificateExtensions anyExtendedKeyUsage not in extendedKeyUsage</t>
-  </si>
-  <si>
-    <t>anyExtendedKeyUsage</t>
+    <t>NOTE_FALSE the check failed in certificate {cert} for reason {reason} AND VALUE CertificateExtensions TLS Web Server Authentication in extendedKeyUsage</t>
+  </si>
+  <si>
+    <t>(NOTE_TRUE the check failed in certificate {cert} for reason {reason} AND VALUE CertificateExtensions Any Extended Key Usage in extendedKeyUsage) OR CHECK_SAME_KEYUSAGE</t>
   </si>
   <si>
     <t>Certificate Policies</t>
@@ -2637,25 +2643,19 @@
     <t>crlDistributionPoints</t>
   </si>
   <si>
-    <t>HTTP value in distributionPoint field pointing to a full and complete CRL.</t>
+    <t>VALUE CertificateExtensions IP in crlDistributionPoints OR VALUE CertificateExtensions URI in crlDistributionPoints</t>
   </si>
   <si>
     <t>THIS or CertificateExtensions Authority Information Access</t>
   </si>
   <si>
-    <t>reasons and cRLIssuer fields, and nameRelativetoCRLIssuer CHOICE</t>
+    <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason} AND (VALUE CertificateExtensions Relative Name in crlDistributionPoints OR VALUE CertificateExtensions CRL Issuer in crlDistributionPoints OR VALUE CertificateExtensions Reasons in crlDistributionPoints) AND DISABLE_IF False</t>
   </si>
   <si>
     <t>ct_precert_scts</t>
   </si>
   <si>
     <t>OCSP must staple extension</t>
-  </si>
-  <si>
-    <t>revocation with OCSP</t>
-  </si>
-  <si>
-    <t>revocation with CRL</t>
   </si>
   <si>
     <t>AgID</t>
@@ -2833,7 +2833,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2950,12 +2950,6 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -3115,7 +3109,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="184">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3595,12 +3589,6 @@
     <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -3637,17 +3625,17 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -4398,7 +4386,9 @@
         <v>18</v>
       </c>
       <c r="C3" s="150"/>
-      <c r="D3" s="151"/>
+      <c r="D3" s="151" t="s">
+        <v>518</v>
+      </c>
       <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
@@ -4414,13 +4404,15 @@
     </row>
     <row r="4">
       <c r="A4" s="143" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="152"/>
-      <c r="D4" s="151"/>
+      <c r="D4" s="151" t="s">
+        <v>520</v>
+      </c>
       <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
@@ -4434,22 +4426,22 @@
     </row>
     <row r="5">
       <c r="A5" s="143" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="143" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D5" s="151" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="143" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="G5" s="142"/>
       <c r="H5" s="11" t="s">
@@ -4462,14 +4454,14 @@
     </row>
     <row r="6">
       <c r="A6" s="143" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="152"/>
       <c r="D6" s="155" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>18</v>
@@ -4485,13 +4477,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="142"/>
+      <c r="A7" s="143" t="s">
+        <v>524</v>
+      </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="152"/>
       <c r="D7" s="151" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>15</v>
@@ -4506,7 +4500,7 @@
     </row>
     <row r="8">
       <c r="A8" s="143" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>23</v>
@@ -4528,21 +4522,21 @@
     </row>
     <row r="9">
       <c r="A9" s="143" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="150"/>
       <c r="D9" s="157" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="152"/>
       <c r="G9" s="149" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
@@ -4554,40 +4548,42 @@
     </row>
     <row r="10">
       <c r="A10" s="143" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="150"/>
       <c r="D10" s="158" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="152"/>
       <c r="G10" s="143" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="159" t="s">
+        <v>533</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="143" t="s">
         <v>531</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="143"/>
       <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="152"/>
       <c r="D11" s="158" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E11" s="160"/>
       <c r="F11" s="152"/>
@@ -4600,40 +4596,42 @@
     </row>
     <row r="12">
       <c r="A12" s="143" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="152"/>
       <c r="D12" s="151" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="152"/>
       <c r="G12" s="143" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="159" t="s">
+        <v>537</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="143" t="s">
         <v>535</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="143"/>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="152"/>
       <c r="D13" s="151" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E13" s="162"/>
       <c r="F13" s="152"/>
@@ -4646,7 +4644,7 @@
     </row>
     <row r="14">
       <c r="A14" s="143" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>23</v>
@@ -4666,7 +4664,7 @@
     </row>
     <row r="15">
       <c r="A15" s="143" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>23</v>
@@ -4684,83 +4682,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="142"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="167"/>
-      <c r="E16" s="160"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="164"/>
-      <c r="J16" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="143" t="s">
-        <v>539</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="142"/>
-      <c r="D17" s="168"/>
-      <c r="E17" s="160"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="164"/>
-      <c r="J17" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="143" t="s">
-        <v>540</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="142"/>
-      <c r="D18" s="168"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="142"/>
-      <c r="H18" s="163"/>
-      <c r="I18" s="164"/>
-      <c r="J18" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B18 H2:H18 J2:J18 E3:E10 I3:I18 E12">
+  <conditionalFormatting sqref="B2:B15 H2:H15 J2:J15 E3:E10 I3:I15 E12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"must not"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B18 H2:H18 J2:J18 E3:E10 I3:I18 E12">
+  <conditionalFormatting sqref="B2:B15 H2:H15 J2:J15 E3:E10 I3:I15 E12">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"recommended"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B18 H2:H18 J2:J18 E3:E10 I3:I18 E12">
+  <conditionalFormatting sqref="B2:B15 H2:H15 J2:J15 E3:E10 I3:I15 E12">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"not recommended"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B18 H2:H18 J2:J18 E3:E10 I3:I18 E12">
+  <conditionalFormatting sqref="B2:B15 H2:H15 J2:J15 E3:E10 I3:I15 E12">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"must"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B18 H2:H18 J2:J18 E3:E10 I3:I18 E12">
+  <conditionalFormatting sqref="B2:B15 H2:H15 J2:J15 E3:E10 I3:I15 E12">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"not recommended*"</formula>
     </cfRule>
@@ -4791,14 +4739,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="169"/>
+      <c r="A1" s="167"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="170" t="s">
+      <c r="D1" s="168" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -4820,11 +4768,11 @@
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="169" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="169" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4835,7 +4783,7 @@
       <c r="B4" s="11"/>
       <c r="C4" s="163"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="171" t="s">
+      <c r="E4" s="169" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4908,414 +4856,414 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="172" t="s">
+      <c r="D1" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172" t="s">
+      <c r="E1" s="170"/>
+      <c r="F1" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172" t="s">
+      <c r="G1" s="170"/>
+      <c r="H1" s="170" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="172"/>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
+      <c r="A2" s="170"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
     </row>
     <row r="3">
-      <c r="A3" s="172"/>
-      <c r="B3" s="172"/>
-      <c r="C3" s="173"/>
-      <c r="D3" s="173"/>
-      <c r="E3" s="173"/>
-      <c r="F3" s="173"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="173"/>
+      <c r="A3" s="170"/>
+      <c r="B3" s="170"/>
+      <c r="C3" s="171"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
     </row>
     <row r="4">
-      <c r="A4" s="172" t="s">
+      <c r="A4" s="170" t="s">
         <v>546</v>
       </c>
-      <c r="B4" s="174" t="s">
+      <c r="B4" s="172" t="s">
         <v>547</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="174" t="s">
+      <c r="C4" s="171"/>
+      <c r="D4" s="172" t="s">
         <v>548</v>
       </c>
-      <c r="E4" s="173"/>
-      <c r="F4" s="174" t="s">
+      <c r="E4" s="171"/>
+      <c r="F4" s="172" t="s">
         <v>549</v>
       </c>
-      <c r="G4" s="174" t="s">
+      <c r="G4" s="172" t="s">
         <v>550</v>
       </c>
-      <c r="H4" s="175"/>
+      <c r="H4" s="173"/>
     </row>
     <row r="5">
-      <c r="A5" s="172"/>
-      <c r="B5" s="172"/>
-      <c r="C5" s="173"/>
-      <c r="D5" s="173"/>
-      <c r="E5" s="173"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="172"/>
-      <c r="H5" s="175"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="170"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="170"/>
+      <c r="H5" s="173"/>
     </row>
     <row r="6">
-      <c r="A6" s="172"/>
-      <c r="B6" s="176" t="s">
+      <c r="A6" s="170"/>
+      <c r="B6" s="174" t="s">
         <v>551</v>
       </c>
-      <c r="C6" s="174" t="s">
+      <c r="C6" s="172" t="s">
         <v>552</v>
       </c>
-      <c r="D6" s="174" t="s">
+      <c r="D6" s="172" t="s">
         <v>553</v>
       </c>
-      <c r="E6" s="173"/>
-      <c r="F6" s="176" t="s">
+      <c r="E6" s="171"/>
+      <c r="F6" s="174" t="s">
         <v>554</v>
       </c>
-      <c r="G6" s="174" t="s">
+      <c r="G6" s="172" t="s">
         <v>555</v>
       </c>
-      <c r="H6" s="175"/>
+      <c r="H6" s="173"/>
     </row>
     <row r="7">
-      <c r="A7" s="172"/>
-      <c r="B7" s="172"/>
-      <c r="C7" s="172"/>
-      <c r="D7" s="174" t="s">
+      <c r="A7" s="170"/>
+      <c r="B7" s="170"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="172" t="s">
         <v>556</v>
       </c>
-      <c r="E7" s="173"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="172"/>
-      <c r="H7" s="172"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="170"/>
     </row>
     <row r="8">
-      <c r="A8" s="172"/>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172" t="s">
+      <c r="A8" s="170"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="170" t="s">
         <v>557</v>
       </c>
-      <c r="D8" s="173"/>
-      <c r="E8" s="173"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="172" t="s">
+      <c r="D8" s="171"/>
+      <c r="E8" s="171"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="170" t="s">
         <v>558</v>
       </c>
-      <c r="H8" s="172" t="s">
+      <c r="H8" s="170" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="172"/>
-      <c r="B9" s="172"/>
-      <c r="C9" s="177" t="s">
+      <c r="A9" s="170"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="175" t="s">
         <v>559</v>
       </c>
-      <c r="D9" s="173"/>
-      <c r="E9" s="173"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="173"/>
-      <c r="H9" s="178"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
+      <c r="H9" s="176"/>
     </row>
     <row r="10">
-      <c r="A10" s="172"/>
-      <c r="B10" s="174" t="s">
+      <c r="A10" s="170"/>
+      <c r="B10" s="172" t="s">
         <v>560</v>
       </c>
-      <c r="C10" s="174" t="s">
+      <c r="C10" s="172" t="s">
         <v>561</v>
       </c>
-      <c r="D10" s="173"/>
-      <c r="E10" s="174" t="s">
+      <c r="D10" s="171"/>
+      <c r="E10" s="172" t="s">
         <v>562</v>
       </c>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174" t="s">
+      <c r="F10" s="171"/>
+      <c r="G10" s="172" t="s">
         <v>563</v>
       </c>
-      <c r="H10" s="175"/>
+      <c r="H10" s="173"/>
     </row>
     <row r="11">
-      <c r="A11" s="172"/>
-      <c r="B11" s="172"/>
-      <c r="C11" s="172"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="174" t="s">
+      <c r="A11" s="170"/>
+      <c r="B11" s="170"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="172" t="s">
         <v>564</v>
       </c>
-      <c r="F11" s="173"/>
-      <c r="G11" s="172"/>
-      <c r="H11" s="175"/>
+      <c r="F11" s="171"/>
+      <c r="G11" s="170"/>
+      <c r="H11" s="173"/>
     </row>
     <row r="12">
-      <c r="A12" s="172"/>
-      <c r="B12" s="172"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="174" t="s">
+      <c r="A12" s="170"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="172" t="s">
         <v>565</v>
       </c>
-      <c r="F12" s="173"/>
-      <c r="G12" s="172"/>
-      <c r="H12" s="175"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="170"/>
+      <c r="H12" s="173"/>
     </row>
     <row r="13">
-      <c r="A13" s="172"/>
-      <c r="B13" s="172"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="174" t="s">
+      <c r="A13" s="170"/>
+      <c r="B13" s="170"/>
+      <c r="C13" s="170"/>
+      <c r="D13" s="172" t="s">
         <v>556</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="172"/>
-      <c r="H13" s="175"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="171"/>
+      <c r="G13" s="170"/>
+      <c r="H13" s="173"/>
     </row>
     <row r="14">
-      <c r="A14" s="172"/>
-      <c r="B14" s="172"/>
-      <c r="C14" s="174" t="s">
+      <c r="A14" s="170"/>
+      <c r="B14" s="170"/>
+      <c r="C14" s="172" t="s">
         <v>566</v>
       </c>
-      <c r="D14" s="173"/>
-      <c r="E14" s="174" t="s">
+      <c r="D14" s="171"/>
+      <c r="E14" s="172" t="s">
         <v>567</v>
       </c>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="175"/>
+      <c r="F14" s="171"/>
+      <c r="G14" s="171"/>
+      <c r="H14" s="173"/>
     </row>
     <row r="15">
-      <c r="A15" s="172"/>
-      <c r="B15" s="172"/>
-      <c r="C15" s="172"/>
-      <c r="D15" s="173"/>
-      <c r="E15" s="174" t="s">
+      <c r="A15" s="170"/>
+      <c r="B15" s="170"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172" t="s">
         <v>568</v>
       </c>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="175"/>
+      <c r="F15" s="171"/>
+      <c r="G15" s="171"/>
+      <c r="H15" s="173"/>
     </row>
     <row r="16">
-      <c r="A16" s="172"/>
-      <c r="B16" s="172"/>
-      <c r="C16" s="176" t="s">
+      <c r="A16" s="170"/>
+      <c r="B16" s="170"/>
+      <c r="C16" s="174" t="s">
         <v>569</v>
       </c>
-      <c r="D16" s="173"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="176" t="s">
+      <c r="D16" s="171"/>
+      <c r="E16" s="170"/>
+      <c r="F16" s="171"/>
+      <c r="G16" s="174" t="s">
         <v>570</v>
       </c>
-      <c r="H16" s="179"/>
+      <c r="H16" s="177"/>
     </row>
     <row r="17">
-      <c r="A17" s="172"/>
-      <c r="B17" s="174" t="s">
+      <c r="A17" s="170"/>
+      <c r="B17" s="172" t="s">
         <v>571</v>
       </c>
-      <c r="C17" s="174" t="s">
+      <c r="C17" s="172" t="s">
         <v>572</v>
       </c>
-      <c r="D17" s="173"/>
-      <c r="E17" s="174" t="s">
+      <c r="D17" s="171"/>
+      <c r="E17" s="172" t="s">
         <v>573</v>
       </c>
-      <c r="F17" s="173"/>
-      <c r="G17" s="174" t="s">
+      <c r="F17" s="171"/>
+      <c r="G17" s="172" t="s">
         <v>574</v>
       </c>
-      <c r="H17" s="175"/>
+      <c r="H17" s="173"/>
     </row>
     <row r="18">
-      <c r="A18" s="172"/>
-      <c r="B18" s="172"/>
-      <c r="C18" s="172"/>
-      <c r="D18" s="173"/>
-      <c r="E18" s="174" t="s">
+      <c r="A18" s="170"/>
+      <c r="B18" s="170"/>
+      <c r="C18" s="170"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172" t="s">
         <v>575</v>
       </c>
-      <c r="F18" s="173"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="175"/>
+      <c r="F18" s="171"/>
+      <c r="G18" s="170"/>
+      <c r="H18" s="173"/>
     </row>
     <row r="19">
-      <c r="A19" s="172"/>
-      <c r="B19" s="172"/>
-      <c r="C19" s="172"/>
-      <c r="D19" s="173"/>
-      <c r="E19" s="174" t="s">
+      <c r="A19" s="170"/>
+      <c r="B19" s="170"/>
+      <c r="C19" s="170"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172" t="s">
         <v>576</v>
       </c>
-      <c r="F19" s="173"/>
-      <c r="G19" s="173"/>
-      <c r="H19" s="175"/>
+      <c r="F19" s="171"/>
+      <c r="G19" s="171"/>
+      <c r="H19" s="173"/>
     </row>
     <row r="20">
-      <c r="A20" s="172"/>
-      <c r="B20" s="172"/>
-      <c r="C20" s="174" t="s">
+      <c r="A20" s="170"/>
+      <c r="B20" s="170"/>
+      <c r="C20" s="172" t="s">
         <v>577</v>
       </c>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174" t="s">
+      <c r="D20" s="171"/>
+      <c r="E20" s="172" t="s">
         <v>578</v>
       </c>
-      <c r="F20" s="172"/>
-      <c r="G20" s="172"/>
-      <c r="H20" s="175"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="173"/>
     </row>
     <row r="21">
-      <c r="A21" s="172"/>
-      <c r="B21" s="172"/>
-      <c r="C21" s="174" t="s">
+      <c r="A21" s="170"/>
+      <c r="B21" s="170"/>
+      <c r="C21" s="172" t="s">
         <v>579</v>
       </c>
-      <c r="D21" s="173"/>
-      <c r="E21" s="174" t="s">
+      <c r="D21" s="171"/>
+      <c r="E21" s="172" t="s">
         <v>580</v>
       </c>
-      <c r="F21" s="173"/>
-      <c r="G21" s="173"/>
-      <c r="H21" s="175"/>
+      <c r="F21" s="171"/>
+      <c r="G21" s="171"/>
+      <c r="H21" s="173"/>
     </row>
     <row r="22">
-      <c r="A22" s="172"/>
-      <c r="B22" s="177" t="s">
+      <c r="A22" s="170"/>
+      <c r="B22" s="175" t="s">
         <v>581</v>
       </c>
-      <c r="C22" s="177" t="s">
+      <c r="C22" s="175" t="s">
         <v>582</v>
       </c>
-      <c r="D22" s="173"/>
-      <c r="E22" s="177" t="s">
+      <c r="D22" s="171"/>
+      <c r="E22" s="175" t="s">
         <v>583</v>
       </c>
-      <c r="F22" s="173"/>
-      <c r="G22" s="173"/>
-      <c r="H22" s="178"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="171"/>
+      <c r="H22" s="176"/>
     </row>
     <row r="23">
-      <c r="A23" s="172"/>
-      <c r="B23" s="172"/>
-      <c r="C23" s="177" t="s">
+      <c r="A23" s="170"/>
+      <c r="B23" s="170"/>
+      <c r="C23" s="175" t="s">
         <v>584</v>
       </c>
-      <c r="D23" s="173"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="173"/>
-      <c r="H23" s="178"/>
+      <c r="D23" s="171"/>
+      <c r="E23" s="170"/>
+      <c r="F23" s="171"/>
+      <c r="G23" s="171"/>
+      <c r="H23" s="176"/>
     </row>
     <row r="24">
-      <c r="A24" s="172"/>
-      <c r="B24" s="172"/>
-      <c r="C24" s="177" t="s">
+      <c r="A24" s="170"/>
+      <c r="B24" s="170"/>
+      <c r="C24" s="175" t="s">
         <v>585</v>
       </c>
-      <c r="D24" s="173"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="178"/>
+      <c r="D24" s="171"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="171"/>
+      <c r="H24" s="176"/>
     </row>
     <row r="25">
-      <c r="A25" s="172"/>
-      <c r="B25" s="172"/>
-      <c r="C25" s="177" t="s">
+      <c r="A25" s="170"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="175" t="s">
         <v>586</v>
       </c>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="173"/>
-      <c r="H25" s="178"/>
+      <c r="D25" s="171"/>
+      <c r="E25" s="171"/>
+      <c r="F25" s="171"/>
+      <c r="G25" s="171"/>
+      <c r="H25" s="176"/>
     </row>
     <row r="26">
-      <c r="A26" s="172"/>
-      <c r="B26" s="172" t="s">
+      <c r="A26" s="170"/>
+      <c r="B26" s="170" t="s">
         <v>587</v>
       </c>
-      <c r="C26" s="173"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="172" t="s">
+      <c r="C26" s="171"/>
+      <c r="D26" s="171"/>
+      <c r="E26" s="170" t="s">
         <v>588</v>
       </c>
-      <c r="F26" s="173"/>
-      <c r="G26" s="172" t="s">
+      <c r="F26" s="171"/>
+      <c r="G26" s="170" t="s">
         <v>570</v>
       </c>
-      <c r="H26" s="172" t="s">
+      <c r="H26" s="170" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="172"/>
-      <c r="B27" s="174" t="s">
+      <c r="A27" s="170"/>
+      <c r="B27" s="172" t="s">
         <v>589</v>
       </c>
-      <c r="C27" s="173"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="176" t="s">
+      <c r="C27" s="171"/>
+      <c r="D27" s="171"/>
+      <c r="E27" s="171"/>
+      <c r="F27" s="171"/>
+      <c r="G27" s="174" t="s">
         <v>570</v>
       </c>
-      <c r="H27" s="175"/>
+      <c r="H27" s="173"/>
     </row>
     <row r="28">
-      <c r="A28" s="172"/>
-      <c r="B28" s="177" t="s">
+      <c r="A28" s="170"/>
+      <c r="B28" s="175" t="s">
         <v>590</v>
       </c>
-      <c r="C28" s="173"/>
-      <c r="D28" s="172" t="s">
+      <c r="C28" s="171"/>
+      <c r="D28" s="170" t="s">
         <v>591</v>
       </c>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="180"/>
-      <c r="H28" s="178"/>
+      <c r="E28" s="171"/>
+      <c r="F28" s="171"/>
+      <c r="G28" s="178"/>
+      <c r="H28" s="176"/>
     </row>
     <row r="29">
-      <c r="A29" s="172"/>
-      <c r="B29" s="172"/>
-      <c r="C29" s="172"/>
-      <c r="D29" s="172"/>
-      <c r="E29" s="173"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="180"/>
-      <c r="H29" s="178"/>
+      <c r="A29" s="170"/>
+      <c r="B29" s="170"/>
+      <c r="C29" s="170"/>
+      <c r="D29" s="170"/>
+      <c r="E29" s="171"/>
+      <c r="F29" s="171"/>
+      <c r="G29" s="178"/>
+      <c r="H29" s="176"/>
     </row>
     <row r="30">
-      <c r="A30" s="172" t="s">
+      <c r="A30" s="170" t="s">
         <v>592</v>
       </c>
-      <c r="B30" s="172"/>
-      <c r="C30" s="173"/>
-      <c r="D30" s="173"/>
-      <c r="E30" s="173"/>
-      <c r="F30" s="173"/>
-      <c r="G30" s="173"/>
-      <c r="H30" s="178"/>
+      <c r="B30" s="170"/>
+      <c r="C30" s="171"/>
+      <c r="D30" s="171"/>
+      <c r="E30" s="171"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="171"/>
+      <c r="H30" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5348,105 +5296,105 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="181" t="str">
+      <c r="A2" s="179" t="str">
         <f>HYPERLINK("http://www.isg.rhul.ac.uk/tls/Lucky13.html","Lucky 13")</f>
         <v>Lucky 13</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
     </row>
     <row r="3">
-      <c r="A3" s="183" t="str">
+      <c r="A3" s="181" t="str">
         <f>HYPERLINK("https://nerdoholic.org/uploads/dergln/beast_part2/ssl_jun21.pdf","BEAST")</f>
         <v>BEAST</v>
       </c>
-      <c r="B3" s="182"/>
+      <c r="B3" s="180"/>
     </row>
     <row r="4">
-      <c r="A4" s="181" t="str">
+      <c r="A4" s="179" t="str">
         <f>HYPERLINK("https://sweet32.info/","Sweet32")</f>
         <v>Sweet32</v>
       </c>
-      <c r="D4" s="182"/>
+      <c r="D4" s="180"/>
     </row>
     <row r="5">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="182" t="s">
         <v>593</v>
       </c>
-      <c r="B5" s="182"/>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
+      <c r="B5" s="180"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="180"/>
     </row>
     <row r="6">
-      <c r="A6" s="181" t="str">
+      <c r="A6" s="179" t="str">
         <f>HYPERLINK("http://breachattack.com/","BREACH")</f>
         <v>BREACH</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="181" t="str">
+      <c r="A7" s="179" t="str">
         <f>HYPERLINK("https://security.googleblog.com/2014/10/this-poodle-bites-exploiting-ssl-30.html","POODLE")</f>
         <v>POODLE</v>
       </c>
-      <c r="B7" s="182"/>
-      <c r="D7" s="182"/>
+      <c r="B7" s="180"/>
+      <c r="D7" s="180"/>
     </row>
     <row r="8">
-      <c r="A8" s="181" t="str">
+      <c r="A8" s="179" t="str">
         <f>HYPERLINK("https://mitls.org/pages/attacks/3SHAKE","3SHAKE")</f>
         <v>3SHAKE</v>
       </c>
-      <c r="B8" s="182"/>
-      <c r="C8" s="182"/>
-      <c r="D8" s="182"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
     </row>
     <row r="9">
-      <c r="A9" s="181" t="str">
+      <c r="A9" s="179" t="str">
         <f>HYPERLINK("https://drownattack.com/","DROWN")</f>
         <v>DROWN</v>
       </c>
-      <c r="D9" s="182"/>
+      <c r="D9" s="180"/>
     </row>
     <row r="10">
-      <c r="A10" s="181" t="str">
+      <c r="A10" s="179" t="str">
         <f>HYPERLINK("https://robotattack.org/","ROBOT ")</f>
         <v>ROBOT </v>
       </c>
-      <c r="B10" s="182"/>
-      <c r="D10" s="182"/>
+      <c r="B10" s="180"/>
+      <c r="D10" s="180"/>
     </row>
     <row r="11">
-      <c r="A11" s="181" t="str">
+      <c r="A11" s="179" t="str">
         <f>HYPERLINK("https://www.kb.cert.org/vuls/id/120541/","Renegotiation attack")</f>
         <v>Renegotiation attack</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="185" t="s">
+      <c r="A12" s="183" t="s">
         <v>594</v>
       </c>
-      <c r="D12" s="182"/>
+      <c r="D12" s="180"/>
     </row>
     <row r="13">
-      <c r="A13" s="185" t="s">
+      <c r="A13" s="183" t="s">
         <v>595</v>
       </c>
-      <c r="B13" s="182"/>
-      <c r="C13" s="182"/>
-      <c r="D13" s="182"/>
+      <c r="B13" s="180"/>
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
     </row>
     <row r="14">
-      <c r="A14" s="185" t="s">
+      <c r="A14" s="183" t="s">
         <v>596</v>
       </c>
-      <c r="D14" s="182"/>
+      <c r="D14" s="180"/>
     </row>
     <row r="15">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="183" t="s">
         <v>597</v>
       </c>
-      <c r="B15" s="182"/>
+      <c r="B15" s="180"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added mitigation for Certificate and CertificateExtensions
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -1046,7 +1046,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="605">
   <si>
     <t>NIST</t>
   </si>
@@ -2587,13 +2587,13 @@
     <t>X.509 version</t>
   </si>
   <si>
-    <t>VALUE Certificate X.509 version == 2</t>
+    <t>VALUE Certificate 2 == X.509 version and NOTE_FALSE In order for the certificate to be compliant it has to use X.509 version 2</t>
   </si>
   <si>
     <t>Issuer Distinguished Name</t>
   </si>
   <si>
-    <t>VALUE Certificate , not in [Issuer Distinguished Name][CN,O,OU,L,S]</t>
+    <t>VALUE Certificate , not in [Issuer Distinguished Name][CN,O,OU,L,S] and NOTE_FALSE The fields CN, O, OU, L, S of the Issuer Distinguished Name field should contain a single value [no "," character allowed]</t>
   </si>
   <si>
     <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason}, remember that BSI guidelines prohibit the usage of * in this field and VALUE Certificate * in [Issuer Distinguished Name][CN]</t>
@@ -2602,7 +2602,10 @@
     <t>validity</t>
   </si>
   <si>
-    <t>YEARS &lt;= 3</t>
+    <t>YEARS &lt;= 3 and NOTE_FALSE In order for the certificate to be compliant it should have a validity of 3 years or less</t>
+  </si>
+  <si>
+    <t>YEARS &lt;= 3 and NOTE_FALSE In order for the certificate to be compliant it must have a validity of 3 years or less</t>
   </si>
   <si>
     <t>Subject Distinguished Name</t>
@@ -2635,7 +2638,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>CertificateExtensions digitalSignature OR CertificateExtensions keyAgreement</t>
+    <t>(VALUE CertificateExtensions Digital Signature in keyUsage OR VALUE CertificateExtensions Key Agreement in keyUsage) and NOTE_FALSE Invalid keyUsage, allowed key usages are digital signature if using RSA certificate and key agreement if using ECDH or DH certificate</t>
   </si>
   <si>
     <t>extendedKeyUsage</t>
@@ -4373,7 +4376,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="142" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B1" s="143" t="s">
         <v>0</v>
@@ -4397,14 +4400,14 @@
       <c r="A2" s="144"/>
       <c r="B2" s="11"/>
       <c r="C2" s="145" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D2" s="147" t="s">
         <v>511</v>
       </c>
       <c r="E2" s="146"/>
       <c r="F2" s="145" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="G2" s="145" t="s">
         <v>511</v>
@@ -4417,14 +4420,14 @@
     </row>
     <row r="3">
       <c r="A3" s="145" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="153" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>15</v>
@@ -4441,14 +4444,14 @@
     </row>
     <row r="4">
       <c r="A4" s="145" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="154"/>
       <c r="D4" s="153" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>15</v>
@@ -4463,22 +4466,22 @@
     </row>
     <row r="5">
       <c r="A5" s="145" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D5" s="153" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="145" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G5" s="144"/>
       <c r="H5" s="11" t="s">
@@ -4491,14 +4494,14 @@
     </row>
     <row r="6">
       <c r="A6" s="145" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="154"/>
       <c r="D6" s="157" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>18</v>
@@ -4515,14 +4518,14 @@
     </row>
     <row r="7">
       <c r="A7" s="145" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="154"/>
       <c r="D7" s="153" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>15</v>
@@ -4537,7 +4540,7 @@
     </row>
     <row r="8">
       <c r="A8" s="145" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>23</v>
@@ -4559,21 +4562,21 @@
     </row>
     <row r="9">
       <c r="A9" s="145" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="152"/>
       <c r="D9" s="159" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="154"/>
       <c r="G9" s="151" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
@@ -4585,27 +4588,27 @@
     </row>
     <row r="10">
       <c r="A10" s="145" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="152"/>
       <c r="D10" s="160" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="154"/>
       <c r="G10" s="145" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="161" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>15</v>
@@ -4613,14 +4616,14 @@
     </row>
     <row r="11">
       <c r="A11" s="145" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="154"/>
       <c r="D11" s="160" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E11" s="162"/>
       <c r="F11" s="154"/>
@@ -4633,27 +4636,27 @@
     </row>
     <row r="12">
       <c r="A12" s="145" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="154"/>
       <c r="D12" s="153" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="154"/>
       <c r="G12" s="145" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="161" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>15</v>
@@ -4661,14 +4664,14 @@
     </row>
     <row r="13">
       <c r="A13" s="145" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="154"/>
       <c r="D13" s="153" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E13" s="164"/>
       <c r="F13" s="154"/>
@@ -4681,7 +4684,7 @@
     </row>
     <row r="14">
       <c r="A14" s="145" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>23</v>
@@ -4701,7 +4704,7 @@
     </row>
     <row r="15">
       <c r="A15" s="145" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>23</v>
@@ -4787,12 +4790,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B2" s="120"/>
       <c r="C2" s="120"/>
@@ -4800,7 +4803,7 @@
     </row>
     <row r="3">
       <c r="A3" s="145" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>13</v>
@@ -4815,7 +4818,7 @@
     </row>
     <row r="4">
       <c r="A4" s="145" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="165"/>
@@ -4905,7 +4908,7 @@
       </c>
       <c r="G1" s="172"/>
       <c r="H1" s="172" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="2">
@@ -4930,21 +4933,21 @@
     </row>
     <row r="4">
       <c r="A4" s="172" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B4" s="174" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C4" s="173"/>
       <c r="D4" s="174" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E4" s="173"/>
       <c r="F4" s="174" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="G4" s="174" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="H4" s="175"/>
     </row>
@@ -4961,20 +4964,20 @@
     <row r="6">
       <c r="A6" s="172"/>
       <c r="B6" s="176" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C6" s="174" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D6" s="174" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E6" s="173"/>
       <c r="F6" s="176" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="G6" s="174" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H6" s="175"/>
     </row>
@@ -4983,7 +4986,7 @@
       <c r="B7" s="172"/>
       <c r="C7" s="172"/>
       <c r="D7" s="174" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E7" s="173"/>
       <c r="F7" s="173"/>
@@ -4994,13 +4997,13 @@
       <c r="A8" s="172"/>
       <c r="B8" s="172"/>
       <c r="C8" s="172" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D8" s="173"/>
       <c r="E8" s="173"/>
       <c r="F8" s="173"/>
       <c r="G8" s="172" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H8" s="172" t="s">
         <v>420</v>
@@ -5010,7 +5013,7 @@
       <c r="A9" s="172"/>
       <c r="B9" s="172"/>
       <c r="C9" s="177" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D9" s="173"/>
       <c r="E9" s="173"/>
@@ -5021,18 +5024,18 @@
     <row r="10">
       <c r="A10" s="172"/>
       <c r="B10" s="174" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C10" s="174" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D10" s="173"/>
       <c r="E10" s="174" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F10" s="173"/>
       <c r="G10" s="174" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H10" s="175"/>
     </row>
@@ -5042,7 +5045,7 @@
       <c r="C11" s="172"/>
       <c r="D11" s="173"/>
       <c r="E11" s="174" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F11" s="173"/>
       <c r="G11" s="172"/>
@@ -5054,7 +5057,7 @@
       <c r="C12" s="172"/>
       <c r="D12" s="173"/>
       <c r="E12" s="174" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F12" s="173"/>
       <c r="G12" s="172"/>
@@ -5065,7 +5068,7 @@
       <c r="B13" s="172"/>
       <c r="C13" s="172"/>
       <c r="D13" s="174" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E13" s="172"/>
       <c r="F13" s="173"/>
@@ -5076,11 +5079,11 @@
       <c r="A14" s="172"/>
       <c r="B14" s="172"/>
       <c r="C14" s="174" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D14" s="173"/>
       <c r="E14" s="174" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="F14" s="173"/>
       <c r="G14" s="173"/>
@@ -5092,7 +5095,7 @@
       <c r="C15" s="172"/>
       <c r="D15" s="173"/>
       <c r="E15" s="174" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F15" s="173"/>
       <c r="G15" s="173"/>
@@ -5102,31 +5105,31 @@
       <c r="A16" s="172"/>
       <c r="B16" s="172"/>
       <c r="C16" s="176" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D16" s="173"/>
       <c r="E16" s="172"/>
       <c r="F16" s="173"/>
       <c r="G16" s="176" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="H16" s="179"/>
     </row>
     <row r="17">
       <c r="A17" s="172"/>
       <c r="B17" s="174" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C17" s="174" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D17" s="173"/>
       <c r="E17" s="174" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="F17" s="173"/>
       <c r="G17" s="174" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="H17" s="175"/>
     </row>
@@ -5136,7 +5139,7 @@
       <c r="C18" s="172"/>
       <c r="D18" s="173"/>
       <c r="E18" s="174" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F18" s="173"/>
       <c r="G18" s="172"/>
@@ -5148,7 +5151,7 @@
       <c r="C19" s="172"/>
       <c r="D19" s="173"/>
       <c r="E19" s="174" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F19" s="173"/>
       <c r="G19" s="173"/>
@@ -5158,11 +5161,11 @@
       <c r="A20" s="172"/>
       <c r="B20" s="172"/>
       <c r="C20" s="174" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D20" s="173"/>
       <c r="E20" s="174" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F20" s="172"/>
       <c r="G20" s="172"/>
@@ -5172,11 +5175,11 @@
       <c r="A21" s="172"/>
       <c r="B21" s="172"/>
       <c r="C21" s="174" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D21" s="173"/>
       <c r="E21" s="174" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F21" s="173"/>
       <c r="G21" s="173"/>
@@ -5185,14 +5188,14 @@
     <row r="22">
       <c r="A22" s="172"/>
       <c r="B22" s="177" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C22" s="177" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D22" s="173"/>
       <c r="E22" s="177" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F22" s="173"/>
       <c r="G22" s="173"/>
@@ -5202,7 +5205,7 @@
       <c r="A23" s="172"/>
       <c r="B23" s="172"/>
       <c r="C23" s="177" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D23" s="173"/>
       <c r="E23" s="172"/>
@@ -5214,7 +5217,7 @@
       <c r="A24" s="172"/>
       <c r="B24" s="172"/>
       <c r="C24" s="177" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D24" s="173"/>
       <c r="E24" s="173"/>
@@ -5226,7 +5229,7 @@
       <c r="A25" s="172"/>
       <c r="B25" s="172"/>
       <c r="C25" s="177" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D25" s="173"/>
       <c r="E25" s="173"/>
@@ -5237,16 +5240,16 @@
     <row r="26">
       <c r="A26" s="172"/>
       <c r="B26" s="172" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C26" s="173"/>
       <c r="D26" s="173"/>
       <c r="E26" s="172" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="F26" s="173"/>
       <c r="G26" s="172" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="H26" s="172" t="s">
         <v>420</v>
@@ -5255,25 +5258,25 @@
     <row r="27">
       <c r="A27" s="172"/>
       <c r="B27" s="174" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C27" s="173"/>
       <c r="D27" s="173"/>
       <c r="E27" s="173"/>
       <c r="F27" s="173"/>
       <c r="G27" s="176" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="H27" s="175"/>
     </row>
     <row r="28">
       <c r="A28" s="172"/>
       <c r="B28" s="177" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C28" s="173"/>
       <c r="D28" s="172" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E28" s="173"/>
       <c r="F28" s="173"/>
@@ -5292,7 +5295,7 @@
     </row>
     <row r="30">
       <c r="A30" s="172" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B30" s="172"/>
       <c r="C30" s="173"/>
@@ -5357,7 +5360,7 @@
     </row>
     <row r="5">
       <c r="A5" s="184" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B5" s="182"/>
       <c r="C5" s="182"/>
@@ -5409,13 +5412,13 @@
     </row>
     <row r="12">
       <c r="A12" s="185" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D12" s="182"/>
     </row>
     <row r="13">
       <c r="A13" s="185" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B13" s="182"/>
       <c r="C13" s="182"/>
@@ -5423,13 +5426,13 @@
     </row>
     <row r="14">
       <c r="A14" s="185" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D14" s="182"/>
     </row>
     <row r="15">
       <c r="A15" s="185" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B15" s="182"/>
     </row>
@@ -28739,7 +28742,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="151" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
@@ -28751,7 +28754,7 @@
     </row>
     <row r="6">
       <c r="A6" s="145" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -28763,7 +28766,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="151" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Improved mitigations for Certificates and added new function to check DN validity according to NIST
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -1046,7 +1046,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="606">
   <si>
     <t>NIST</t>
   </si>
@@ -2593,7 +2593,7 @@
     <t>Issuer Distinguished Name</t>
   </si>
   <si>
-    <t>VALUE Certificate , not in [Issuer Distinguished Name][CN,O,OU,L,S] and NOTE_FALSE The fields CN, O, OU, L, S of the Issuer Distinguished Name field should contain a single value [no "," character allowed]</t>
+    <t>CHECK_DN Issuer Distinguished Name - der</t>
   </si>
   <si>
     <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason}, remember that BSI guidelines prohibit the usage of * in this field and VALUE Certificate * in [Issuer Distinguished Name][CN]</t>
@@ -2611,6 +2611,9 @@
     <t>Subject Distinguished Name</t>
   </si>
   <si>
+    <t>CHECK_DN Subject Distinguished Name - der</t>
+  </si>
+  <si>
     <t>NOTE_TRUE the check failed in certificate {cert} for reason {reason}, remember that BSI guidelines prohibit the usage of * in this field and VALUE Certificate * in [Subject Distinguished Name][CN]</t>
   </si>
   <si>
@@ -2665,13 +2668,13 @@
     <t>authorityInfoAccess</t>
   </si>
   <si>
-    <t>VALUE CertificateExtensions OCSP - URI in subjectAltName</t>
+    <t>VALUE CertificateExtensions OCSP - URI in authorityInfoAccess and NOTE_FALSE the authorityInfoAccess extension must have a field CA Issuers containing HTTP URL for certificates issued to issuing CA</t>
   </si>
   <si>
     <t>THIS or CertificateExtensions CRL Distribution Points</t>
   </si>
   <si>
-    <t>VALUE CertificateExtensions CA ISSUERS - URI in subjectAltName</t>
+    <t>VALUE CertificateExtensions CA ISSUERS - URI in authorityInfoAccess and NOTE_FALSE the authorityInfoAccess extension must have the Online Certificate Status Protocol and it must contain HTTP URL for the issuing CA OCSP responder</t>
   </si>
   <si>
     <t>crlDistributionPoints</t>
@@ -4376,7 +4379,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="142" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B1" s="143" t="s">
         <v>0</v>
@@ -4400,14 +4403,14 @@
       <c r="A2" s="144"/>
       <c r="B2" s="11"/>
       <c r="C2" s="145" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D2" s="147" t="s">
         <v>511</v>
       </c>
       <c r="E2" s="146"/>
       <c r="F2" s="145" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G2" s="145" t="s">
         <v>511</v>
@@ -4420,14 +4423,14 @@
     </row>
     <row r="3">
       <c r="A3" s="145" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="153" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>15</v>
@@ -4444,14 +4447,14 @@
     </row>
     <row r="4">
       <c r="A4" s="145" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="154"/>
       <c r="D4" s="153" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>15</v>
@@ -4466,22 +4469,22 @@
     </row>
     <row r="5">
       <c r="A5" s="145" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D5" s="153" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="145" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G5" s="144"/>
       <c r="H5" s="11" t="s">
@@ -4494,14 +4497,14 @@
     </row>
     <row r="6">
       <c r="A6" s="145" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="154"/>
       <c r="D6" s="157" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>18</v>
@@ -4518,14 +4521,14 @@
     </row>
     <row r="7">
       <c r="A7" s="145" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="154"/>
       <c r="D7" s="153" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>15</v>
@@ -4540,7 +4543,7 @@
     </row>
     <row r="8">
       <c r="A8" s="145" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>23</v>
@@ -4562,21 +4565,21 @@
     </row>
     <row r="9">
       <c r="A9" s="145" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="152"/>
       <c r="D9" s="159" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="154"/>
       <c r="G9" s="151" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
@@ -4588,27 +4591,27 @@
     </row>
     <row r="10">
       <c r="A10" s="145" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="152"/>
       <c r="D10" s="160" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="154"/>
       <c r="G10" s="145" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="161" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>15</v>
@@ -4616,14 +4619,14 @@
     </row>
     <row r="11">
       <c r="A11" s="145" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="154"/>
       <c r="D11" s="160" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E11" s="162"/>
       <c r="F11" s="154"/>
@@ -4636,27 +4639,27 @@
     </row>
     <row r="12">
       <c r="A12" s="145" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="154"/>
       <c r="D12" s="153" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="154"/>
       <c r="G12" s="145" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="161" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>15</v>
@@ -4664,14 +4667,14 @@
     </row>
     <row r="13">
       <c r="A13" s="145" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="154"/>
       <c r="D13" s="153" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E13" s="164"/>
       <c r="F13" s="154"/>
@@ -4684,7 +4687,7 @@
     </row>
     <row r="14">
       <c r="A14" s="145" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>23</v>
@@ -4704,7 +4707,7 @@
     </row>
     <row r="15">
       <c r="A15" s="145" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>23</v>
@@ -4790,12 +4793,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B2" s="120"/>
       <c r="C2" s="120"/>
@@ -4803,7 +4806,7 @@
     </row>
     <row r="3">
       <c r="A3" s="145" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>13</v>
@@ -4818,7 +4821,7 @@
     </row>
     <row r="4">
       <c r="A4" s="145" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="165"/>
@@ -4908,7 +4911,7 @@
       </c>
       <c r="G1" s="172"/>
       <c r="H1" s="172" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2">
@@ -4933,21 +4936,21 @@
     </row>
     <row r="4">
       <c r="A4" s="172" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B4" s="174" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C4" s="173"/>
       <c r="D4" s="174" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E4" s="173"/>
       <c r="F4" s="174" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="G4" s="174" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="H4" s="175"/>
     </row>
@@ -4964,20 +4967,20 @@
     <row r="6">
       <c r="A6" s="172"/>
       <c r="B6" s="176" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C6" s="174" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D6" s="174" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E6" s="173"/>
       <c r="F6" s="176" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="G6" s="174" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="H6" s="175"/>
     </row>
@@ -4986,7 +4989,7 @@
       <c r="B7" s="172"/>
       <c r="C7" s="172"/>
       <c r="D7" s="174" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E7" s="173"/>
       <c r="F7" s="173"/>
@@ -4997,13 +5000,13 @@
       <c r="A8" s="172"/>
       <c r="B8" s="172"/>
       <c r="C8" s="172" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D8" s="173"/>
       <c r="E8" s="173"/>
       <c r="F8" s="173"/>
       <c r="G8" s="172" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="H8" s="172" t="s">
         <v>420</v>
@@ -5013,7 +5016,7 @@
       <c r="A9" s="172"/>
       <c r="B9" s="172"/>
       <c r="C9" s="177" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D9" s="173"/>
       <c r="E9" s="173"/>
@@ -5024,18 +5027,18 @@
     <row r="10">
       <c r="A10" s="172"/>
       <c r="B10" s="174" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C10" s="174" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D10" s="173"/>
       <c r="E10" s="174" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F10" s="173"/>
       <c r="G10" s="174" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="H10" s="175"/>
     </row>
@@ -5045,7 +5048,7 @@
       <c r="C11" s="172"/>
       <c r="D11" s="173"/>
       <c r="E11" s="174" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F11" s="173"/>
       <c r="G11" s="172"/>
@@ -5057,7 +5060,7 @@
       <c r="C12" s="172"/>
       <c r="D12" s="173"/>
       <c r="E12" s="174" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F12" s="173"/>
       <c r="G12" s="172"/>
@@ -5068,7 +5071,7 @@
       <c r="B13" s="172"/>
       <c r="C13" s="172"/>
       <c r="D13" s="174" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E13" s="172"/>
       <c r="F13" s="173"/>
@@ -5079,11 +5082,11 @@
       <c r="A14" s="172"/>
       <c r="B14" s="172"/>
       <c r="C14" s="174" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D14" s="173"/>
       <c r="E14" s="174" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F14" s="173"/>
       <c r="G14" s="173"/>
@@ -5095,7 +5098,7 @@
       <c r="C15" s="172"/>
       <c r="D15" s="173"/>
       <c r="E15" s="174" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F15" s="173"/>
       <c r="G15" s="173"/>
@@ -5105,31 +5108,31 @@
       <c r="A16" s="172"/>
       <c r="B16" s="172"/>
       <c r="C16" s="176" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D16" s="173"/>
       <c r="E16" s="172"/>
       <c r="F16" s="173"/>
       <c r="G16" s="176" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H16" s="179"/>
     </row>
     <row r="17">
       <c r="A17" s="172"/>
       <c r="B17" s="174" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C17" s="174" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D17" s="173"/>
       <c r="E17" s="174" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F17" s="173"/>
       <c r="G17" s="174" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H17" s="175"/>
     </row>
@@ -5139,7 +5142,7 @@
       <c r="C18" s="172"/>
       <c r="D18" s="173"/>
       <c r="E18" s="174" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F18" s="173"/>
       <c r="G18" s="172"/>
@@ -5151,7 +5154,7 @@
       <c r="C19" s="172"/>
       <c r="D19" s="173"/>
       <c r="E19" s="174" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F19" s="173"/>
       <c r="G19" s="173"/>
@@ -5161,11 +5164,11 @@
       <c r="A20" s="172"/>
       <c r="B20" s="172"/>
       <c r="C20" s="174" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D20" s="173"/>
       <c r="E20" s="174" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F20" s="172"/>
       <c r="G20" s="172"/>
@@ -5175,11 +5178,11 @@
       <c r="A21" s="172"/>
       <c r="B21" s="172"/>
       <c r="C21" s="174" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D21" s="173"/>
       <c r="E21" s="174" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="F21" s="173"/>
       <c r="G21" s="173"/>
@@ -5188,14 +5191,14 @@
     <row r="22">
       <c r="A22" s="172"/>
       <c r="B22" s="177" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C22" s="177" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D22" s="173"/>
       <c r="E22" s="177" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F22" s="173"/>
       <c r="G22" s="173"/>
@@ -5205,7 +5208,7 @@
       <c r="A23" s="172"/>
       <c r="B23" s="172"/>
       <c r="C23" s="177" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D23" s="173"/>
       <c r="E23" s="172"/>
@@ -5217,7 +5220,7 @@
       <c r="A24" s="172"/>
       <c r="B24" s="172"/>
       <c r="C24" s="177" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D24" s="173"/>
       <c r="E24" s="173"/>
@@ -5229,7 +5232,7 @@
       <c r="A25" s="172"/>
       <c r="B25" s="172"/>
       <c r="C25" s="177" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D25" s="173"/>
       <c r="E25" s="173"/>
@@ -5240,16 +5243,16 @@
     <row r="26">
       <c r="A26" s="172"/>
       <c r="B26" s="172" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C26" s="173"/>
       <c r="D26" s="173"/>
       <c r="E26" s="172" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="F26" s="173"/>
       <c r="G26" s="172" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H26" s="172" t="s">
         <v>420</v>
@@ -5258,25 +5261,25 @@
     <row r="27">
       <c r="A27" s="172"/>
       <c r="B27" s="174" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C27" s="173"/>
       <c r="D27" s="173"/>
       <c r="E27" s="173"/>
       <c r="F27" s="173"/>
       <c r="G27" s="176" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H27" s="175"/>
     </row>
     <row r="28">
       <c r="A28" s="172"/>
       <c r="B28" s="177" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C28" s="173"/>
       <c r="D28" s="172" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="E28" s="173"/>
       <c r="F28" s="173"/>
@@ -5295,7 +5298,7 @@
     </row>
     <row r="30">
       <c r="A30" s="172" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B30" s="172"/>
       <c r="C30" s="173"/>
@@ -5360,7 +5363,7 @@
     </row>
     <row r="5">
       <c r="A5" s="184" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B5" s="182"/>
       <c r="C5" s="182"/>
@@ -5412,13 +5415,13 @@
     </row>
     <row r="12">
       <c r="A12" s="185" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D12" s="182"/>
     </row>
     <row r="13">
       <c r="A13" s="185" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B13" s="182"/>
       <c r="C13" s="182"/>
@@ -5426,13 +5429,13 @@
     </row>
     <row r="14">
       <c r="A14" s="185" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D14" s="182"/>
     </row>
     <row r="15">
       <c r="A15" s="185" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B15" s="182"/>
     </row>
@@ -28760,13 +28763,13 @@
         <v>18</v>
       </c>
       <c r="C6" s="151" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="151" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Improved report for compliance module
</commit_message>
<xml_diff>
--- a/DatabaseFiller/guidelines.xlsx
+++ b/DatabaseFiller/guidelines.xlsx
@@ -1023,7 +1023,10 @@
     </comment>
     <comment authorId="0" ref="C4">
       <text>
-        <t xml:space="preserve">A single value should be encoded in each Relative Distinguished Name (RDN) (the single values that compose the DN). All attributes that are of DirectoryString type should be encoded as a PrintableString.</t>
+        <t xml:space="preserve">A single value should be encoded in each Relative Distinguished Name (RDN) (the single values that compose the DN). All attributes that are of DirectoryString type should be encoded as a PrintableString.
+----
+ho aggiunto un controllo molto specifico su questa cosa perché richiesto dal NIST e indovina un po' manco loro lo rispettano
+	-Riccardo Germenia</t>
       </text>
     </comment>
     <comment authorId="0" ref="E4">
@@ -3150,7 +3153,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="187">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3490,6 +3493,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -4378,20 +4384,20 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="144" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="110"/>
       <c r="D1" s="110"/>
-      <c r="E1" s="143" t="s">
+      <c r="E1" s="144" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="110"/>
       <c r="G1" s="110"/>
-      <c r="H1" s="143" t="s">
+      <c r="H1" s="144" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="110"/>
@@ -4400,217 +4406,217 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="144"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="145" t="s">
+      <c r="C2" s="146" t="s">
         <v>524</v>
       </c>
-      <c r="D2" s="147" t="s">
+      <c r="D2" s="148" t="s">
         <v>511</v>
       </c>
-      <c r="E2" s="146"/>
-      <c r="F2" s="145" t="s">
+      <c r="E2" s="147"/>
+      <c r="F2" s="146" t="s">
         <v>524</v>
       </c>
-      <c r="G2" s="145" t="s">
+      <c r="G2" s="146" t="s">
         <v>511</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="147" t="s">
+      <c r="I2" s="148" t="s">
         <v>511</v>
       </c>
-      <c r="J2" s="148"/>
+      <c r="J2" s="149"/>
     </row>
     <row r="3">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="146" t="s">
         <v>525</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="153" t="s">
+      <c r="C3" s="153"/>
+      <c r="D3" s="154" t="s">
         <v>526</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="154"/>
-      <c r="G3" s="144"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="145"/>
       <c r="H3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="128"/>
+      <c r="I3" s="129"/>
       <c r="J3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="146" t="s">
         <v>527</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="153" t="s">
+      <c r="C4" s="155"/>
+      <c r="D4" s="154" t="s">
         <v>528</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="154"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="156"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="156"/>
+      <c r="I4" s="157"/>
       <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="146" t="s">
         <v>529</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="146" t="s">
         <v>530</v>
       </c>
-      <c r="D5" s="153" t="s">
+      <c r="D5" s="154" t="s">
         <v>531</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="145" t="s">
+      <c r="F5" s="146" t="s">
         <v>530</v>
       </c>
-      <c r="G5" s="144"/>
+      <c r="G5" s="145"/>
       <c r="H5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="128"/>
+      <c r="I5" s="129"/>
       <c r="J5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="145" t="s">
+      <c r="A6" s="146" t="s">
         <v>532</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="154"/>
-      <c r="D6" s="157" t="s">
+      <c r="C6" s="155"/>
+      <c r="D6" s="158" t="s">
         <v>533</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="154"/>
-      <c r="G6" s="144"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="145"/>
       <c r="H6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="128"/>
+      <c r="I6" s="129"/>
       <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="145" t="s">
+      <c r="A7" s="146" t="s">
         <v>532</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="154"/>
-      <c r="D7" s="153" t="s">
+      <c r="C7" s="155"/>
+      <c r="D7" s="154" t="s">
         <v>534</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="154"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="156"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="157"/>
       <c r="J7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="145" t="s">
+      <c r="A8" s="146" t="s">
         <v>535</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="152"/>
-      <c r="D8" s="158"/>
+      <c r="C8" s="153"/>
+      <c r="D8" s="159"/>
       <c r="E8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="154"/>
-      <c r="G8" s="144"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="145"/>
       <c r="H8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="128"/>
+      <c r="I8" s="129"/>
       <c r="J8" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="145" t="s">
+      <c r="A9" s="146" t="s">
         <v>536</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="159" t="s">
+      <c r="C9" s="153"/>
+      <c r="D9" s="160" t="s">
         <v>537</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="154"/>
-      <c r="G9" s="151" t="s">
+      <c r="F9" s="155"/>
+      <c r="G9" s="152" t="s">
         <v>538</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="128"/>
+      <c r="I9" s="129"/>
       <c r="J9" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="145" t="s">
+      <c r="A10" s="146" t="s">
         <v>539</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="152"/>
-      <c r="D10" s="160" t="s">
+      <c r="C10" s="153"/>
+      <c r="D10" s="161" t="s">
         <v>540</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="154"/>
-      <c r="G10" s="145" t="s">
+      <c r="F10" s="155"/>
+      <c r="G10" s="146" t="s">
         <v>541</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="161" t="s">
+      <c r="I10" s="162" t="s">
         <v>541</v>
       </c>
       <c r="J10" s="12" t="s">
@@ -4618,47 +4624,47 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="145" t="s">
+      <c r="A11" s="146" t="s">
         <v>539</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="154"/>
-      <c r="D11" s="160" t="s">
+      <c r="C11" s="155"/>
+      <c r="D11" s="161" t="s">
         <v>542</v>
       </c>
-      <c r="E11" s="162"/>
-      <c r="F11" s="154"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="155"/>
-      <c r="I11" s="163"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="155"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="164"/>
       <c r="J11" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="145" t="s">
+      <c r="A12" s="146" t="s">
         <v>543</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="154"/>
-      <c r="D12" s="153" t="s">
+      <c r="C12" s="155"/>
+      <c r="D12" s="154" t="s">
         <v>544</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="154"/>
-      <c r="G12" s="145" t="s">
+      <c r="F12" s="155"/>
+      <c r="G12" s="146" t="s">
         <v>545</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="161" t="s">
+      <c r="I12" s="162" t="s">
         <v>545</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -4666,61 +4672,61 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="145" t="s">
+      <c r="A13" s="146" t="s">
         <v>543</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="154"/>
-      <c r="D13" s="153" t="s">
+      <c r="C13" s="155"/>
+      <c r="D13" s="154" t="s">
         <v>546</v>
       </c>
-      <c r="E13" s="164"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="166"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="155"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="167"/>
       <c r="J13" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="145" t="s">
+      <c r="A14" s="146" t="s">
         <v>547</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="154"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="164"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
+      <c r="C14" s="155"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="155"/>
       <c r="H14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="149"/>
+      <c r="I14" s="150"/>
       <c r="J14" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="145" t="s">
+      <c r="A15" s="146" t="s">
         <v>548</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="154"/>
-      <c r="D15" s="147"/>
-      <c r="E15" s="168"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="152"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="148"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="153"/>
+      <c r="G15" s="153"/>
       <c r="H15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="149"/>
+      <c r="I15" s="150"/>
       <c r="J15" s="12" t="s">
         <v>15</v>
       </c>
@@ -4782,14 +4788,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="169"/>
+      <c r="A1" s="170"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="170" t="s">
+      <c r="D1" s="171" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -4800,33 +4806,33 @@
       <c r="A2" s="9" t="s">
         <v>550</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
       <c r="D2" s="113"/>
     </row>
     <row r="3">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="146" t="s">
         <v>551</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="172" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="172" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="146" t="s">
         <v>552</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="165"/>
+      <c r="C4" s="166"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="171" t="s">
+      <c r="E4" s="172" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4899,414 +4905,414 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="172" t="s">
+      <c r="D1" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172" t="s">
+      <c r="E1" s="173"/>
+      <c r="F1" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172" t="s">
+      <c r="G1" s="173"/>
+      <c r="H1" s="173" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="172"/>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
+      <c r="A2" s="173"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="3">
-      <c r="A3" s="172"/>
-      <c r="B3" s="172"/>
-      <c r="C3" s="173"/>
-      <c r="D3" s="173"/>
-      <c r="E3" s="173"/>
-      <c r="F3" s="173"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="173"/>
+      <c r="A3" s="173"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
     </row>
     <row r="4">
-      <c r="A4" s="172" t="s">
+      <c r="A4" s="173" t="s">
         <v>554</v>
       </c>
-      <c r="B4" s="174" t="s">
+      <c r="B4" s="175" t="s">
         <v>555</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="174" t="s">
+      <c r="C4" s="174"/>
+      <c r="D4" s="175" t="s">
         <v>556</v>
       </c>
-      <c r="E4" s="173"/>
-      <c r="F4" s="174" t="s">
+      <c r="E4" s="174"/>
+      <c r="F4" s="175" t="s">
         <v>557</v>
       </c>
-      <c r="G4" s="174" t="s">
+      <c r="G4" s="175" t="s">
         <v>558</v>
       </c>
-      <c r="H4" s="175"/>
+      <c r="H4" s="176"/>
     </row>
     <row r="5">
-      <c r="A5" s="172"/>
-      <c r="B5" s="172"/>
-      <c r="C5" s="173"/>
-      <c r="D5" s="173"/>
-      <c r="E5" s="173"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="172"/>
-      <c r="H5" s="175"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="174"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="174"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="173"/>
+      <c r="H5" s="176"/>
     </row>
     <row r="6">
-      <c r="A6" s="172"/>
-      <c r="B6" s="176" t="s">
+      <c r="A6" s="173"/>
+      <c r="B6" s="177" t="s">
         <v>559</v>
       </c>
-      <c r="C6" s="174" t="s">
+      <c r="C6" s="175" t="s">
         <v>560</v>
       </c>
-      <c r="D6" s="174" t="s">
+      <c r="D6" s="175" t="s">
         <v>561</v>
       </c>
-      <c r="E6" s="173"/>
-      <c r="F6" s="176" t="s">
+      <c r="E6" s="174"/>
+      <c r="F6" s="177" t="s">
         <v>562</v>
       </c>
-      <c r="G6" s="174" t="s">
+      <c r="G6" s="175" t="s">
         <v>563</v>
       </c>
-      <c r="H6" s="175"/>
+      <c r="H6" s="176"/>
     </row>
     <row r="7">
-      <c r="A7" s="172"/>
-      <c r="B7" s="172"/>
-      <c r="C7" s="172"/>
-      <c r="D7" s="174" t="s">
+      <c r="A7" s="173"/>
+      <c r="B7" s="173"/>
+      <c r="C7" s="173"/>
+      <c r="D7" s="175" t="s">
         <v>564</v>
       </c>
-      <c r="E7" s="173"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="172"/>
-      <c r="H7" s="172"/>
+      <c r="E7" s="174"/>
+      <c r="F7" s="174"/>
+      <c r="G7" s="173"/>
+      <c r="H7" s="173"/>
     </row>
     <row r="8">
-      <c r="A8" s="172"/>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172" t="s">
+      <c r="A8" s="173"/>
+      <c r="B8" s="173"/>
+      <c r="C8" s="173" t="s">
         <v>565</v>
       </c>
-      <c r="D8" s="173"/>
-      <c r="E8" s="173"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="172" t="s">
+      <c r="D8" s="174"/>
+      <c r="E8" s="174"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="173" t="s">
         <v>566</v>
       </c>
-      <c r="H8" s="172" t="s">
+      <c r="H8" s="173" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="172"/>
-      <c r="B9" s="172"/>
-      <c r="C9" s="177" t="s">
+      <c r="A9" s="173"/>
+      <c r="B9" s="173"/>
+      <c r="C9" s="178" t="s">
         <v>567</v>
       </c>
-      <c r="D9" s="173"/>
-      <c r="E9" s="173"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="173"/>
-      <c r="H9" s="178"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="174"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="179"/>
     </row>
     <row r="10">
-      <c r="A10" s="172"/>
-      <c r="B10" s="174" t="s">
+      <c r="A10" s="173"/>
+      <c r="B10" s="175" t="s">
         <v>568</v>
       </c>
-      <c r="C10" s="174" t="s">
+      <c r="C10" s="175" t="s">
         <v>569</v>
       </c>
-      <c r="D10" s="173"/>
-      <c r="E10" s="174" t="s">
+      <c r="D10" s="174"/>
+      <c r="E10" s="175" t="s">
         <v>570</v>
       </c>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174" t="s">
+      <c r="F10" s="174"/>
+      <c r="G10" s="175" t="s">
         <v>571</v>
       </c>
-      <c r="H10" s="175"/>
+      <c r="H10" s="176"/>
     </row>
     <row r="11">
-      <c r="A11" s="172"/>
-      <c r="B11" s="172"/>
-      <c r="C11" s="172"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="174" t="s">
+      <c r="A11" s="173"/>
+      <c r="B11" s="173"/>
+      <c r="C11" s="173"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175" t="s">
         <v>572</v>
       </c>
-      <c r="F11" s="173"/>
-      <c r="G11" s="172"/>
-      <c r="H11" s="175"/>
+      <c r="F11" s="174"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="176"/>
     </row>
     <row r="12">
-      <c r="A12" s="172"/>
-      <c r="B12" s="172"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="174" t="s">
+      <c r="A12" s="173"/>
+      <c r="B12" s="173"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="174"/>
+      <c r="E12" s="175" t="s">
         <v>573</v>
       </c>
-      <c r="F12" s="173"/>
-      <c r="G12" s="172"/>
-      <c r="H12" s="175"/>
+      <c r="F12" s="174"/>
+      <c r="G12" s="173"/>
+      <c r="H12" s="176"/>
     </row>
     <row r="13">
-      <c r="A13" s="172"/>
-      <c r="B13" s="172"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="174" t="s">
+      <c r="A13" s="173"/>
+      <c r="B13" s="173"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="175" t="s">
         <v>564</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="172"/>
-      <c r="H13" s="175"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="174"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="176"/>
     </row>
     <row r="14">
-      <c r="A14" s="172"/>
-      <c r="B14" s="172"/>
-      <c r="C14" s="174" t="s">
+      <c r="A14" s="173"/>
+      <c r="B14" s="173"/>
+      <c r="C14" s="175" t="s">
         <v>574</v>
       </c>
-      <c r="D14" s="173"/>
-      <c r="E14" s="174" t="s">
+      <c r="D14" s="174"/>
+      <c r="E14" s="175" t="s">
         <v>575</v>
       </c>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="175"/>
+      <c r="F14" s="174"/>
+      <c r="G14" s="174"/>
+      <c r="H14" s="176"/>
     </row>
     <row r="15">
-      <c r="A15" s="172"/>
-      <c r="B15" s="172"/>
-      <c r="C15" s="172"/>
-      <c r="D15" s="173"/>
-      <c r="E15" s="174" t="s">
+      <c r="A15" s="173"/>
+      <c r="B15" s="173"/>
+      <c r="C15" s="173"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="175" t="s">
         <v>576</v>
       </c>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="175"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="176"/>
     </row>
     <row r="16">
-      <c r="A16" s="172"/>
-      <c r="B16" s="172"/>
-      <c r="C16" s="176" t="s">
+      <c r="A16" s="173"/>
+      <c r="B16" s="173"/>
+      <c r="C16" s="177" t="s">
         <v>577</v>
       </c>
-      <c r="D16" s="173"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="176" t="s">
+      <c r="D16" s="174"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="174"/>
+      <c r="G16" s="177" t="s">
         <v>578</v>
       </c>
-      <c r="H16" s="179"/>
+      <c r="H16" s="180"/>
     </row>
     <row r="17">
-      <c r="A17" s="172"/>
-      <c r="B17" s="174" t="s">
+      <c r="A17" s="173"/>
+      <c r="B17" s="175" t="s">
         <v>579</v>
       </c>
-      <c r="C17" s="174" t="s">
+      <c r="C17" s="175" t="s">
         <v>580</v>
       </c>
-      <c r="D17" s="173"/>
-      <c r="E17" s="174" t="s">
+      <c r="D17" s="174"/>
+      <c r="E17" s="175" t="s">
         <v>581</v>
       </c>
-      <c r="F17" s="173"/>
-      <c r="G17" s="174" t="s">
+      <c r="F17" s="174"/>
+      <c r="G17" s="175" t="s">
         <v>582</v>
       </c>
-      <c r="H17" s="175"/>
+      <c r="H17" s="176"/>
     </row>
     <row r="18">
-      <c r="A18" s="172"/>
-      <c r="B18" s="172"/>
-      <c r="C18" s="172"/>
-      <c r="D18" s="173"/>
-      <c r="E18" s="174" t="s">
+      <c r="A18" s="173"/>
+      <c r="B18" s="173"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="174"/>
+      <c r="E18" s="175" t="s">
         <v>583</v>
       </c>
-      <c r="F18" s="173"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="175"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="173"/>
+      <c r="H18" s="176"/>
     </row>
     <row r="19">
-      <c r="A19" s="172"/>
-      <c r="B19" s="172"/>
-      <c r="C19" s="172"/>
-      <c r="D19" s="173"/>
-      <c r="E19" s="174" t="s">
+      <c r="A19" s="173"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="175" t="s">
         <v>584</v>
       </c>
-      <c r="F19" s="173"/>
-      <c r="G19" s="173"/>
-      <c r="H19" s="175"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="174"/>
+      <c r="H19" s="176"/>
     </row>
     <row r="20">
-      <c r="A20" s="172"/>
-      <c r="B20" s="172"/>
-      <c r="C20" s="174" t="s">
+      <c r="A20" s="173"/>
+      <c r="B20" s="173"/>
+      <c r="C20" s="175" t="s">
         <v>585</v>
       </c>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174" t="s">
+      <c r="D20" s="174"/>
+      <c r="E20" s="175" t="s">
         <v>586</v>
       </c>
-      <c r="F20" s="172"/>
-      <c r="G20" s="172"/>
-      <c r="H20" s="175"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="173"/>
+      <c r="H20" s="176"/>
     </row>
     <row r="21">
-      <c r="A21" s="172"/>
-      <c r="B21" s="172"/>
-      <c r="C21" s="174" t="s">
+      <c r="A21" s="173"/>
+      <c r="B21" s="173"/>
+      <c r="C21" s="175" t="s">
         <v>587</v>
       </c>
-      <c r="D21" s="173"/>
-      <c r="E21" s="174" t="s">
+      <c r="D21" s="174"/>
+      <c r="E21" s="175" t="s">
         <v>588</v>
       </c>
-      <c r="F21" s="173"/>
-      <c r="G21" s="173"/>
-      <c r="H21" s="175"/>
+      <c r="F21" s="174"/>
+      <c r="G21" s="174"/>
+      <c r="H21" s="176"/>
     </row>
     <row r="22">
-      <c r="A22" s="172"/>
-      <c r="B22" s="177" t="s">
+      <c r="A22" s="173"/>
+      <c r="B22" s="178" t="s">
         <v>589</v>
       </c>
-      <c r="C22" s="177" t="s">
+      <c r="C22" s="178" t="s">
         <v>590</v>
       </c>
-      <c r="D22" s="173"/>
-      <c r="E22" s="177" t="s">
+      <c r="D22" s="174"/>
+      <c r="E22" s="178" t="s">
         <v>591</v>
       </c>
-      <c r="F22" s="173"/>
-      <c r="G22" s="173"/>
-      <c r="H22" s="178"/>
+      <c r="F22" s="174"/>
+      <c r="G22" s="174"/>
+      <c r="H22" s="179"/>
     </row>
     <row r="23">
-      <c r="A23" s="172"/>
-      <c r="B23" s="172"/>
-      <c r="C23" s="177" t="s">
+      <c r="A23" s="173"/>
+      <c r="B23" s="173"/>
+      <c r="C23" s="178" t="s">
         <v>592</v>
       </c>
-      <c r="D23" s="173"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="173"/>
-      <c r="H23" s="178"/>
+      <c r="D23" s="174"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="174"/>
+      <c r="G23" s="174"/>
+      <c r="H23" s="179"/>
     </row>
     <row r="24">
-      <c r="A24" s="172"/>
-      <c r="B24" s="172"/>
-      <c r="C24" s="177" t="s">
+      <c r="A24" s="173"/>
+      <c r="B24" s="173"/>
+      <c r="C24" s="178" t="s">
         <v>593</v>
       </c>
-      <c r="D24" s="173"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="178"/>
+      <c r="D24" s="174"/>
+      <c r="E24" s="174"/>
+      <c r="F24" s="174"/>
+      <c r="G24" s="174"/>
+      <c r="H24" s="179"/>
     </row>
     <row r="25">
-      <c r="A25" s="172"/>
-      <c r="B25" s="172"/>
-      <c r="C25" s="177" t="s">
+      <c r="A25" s="173"/>
+      <c r="B25" s="173"/>
+      <c r="C25" s="178" t="s">
         <v>594</v>
       </c>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="173"/>
-      <c r="H25" s="178"/>
+      <c r="D25" s="174"/>
+      <c r="E25" s="174"/>
+      <c r="F25" s="174"/>
+      <c r="G25" s="174"/>
+      <c r="H25" s="179"/>
     </row>
     <row r="26">
-      <c r="A26" s="172"/>
-      <c r="B26" s="172" t="s">
+      <c r="A26" s="173"/>
+      <c r="B26" s="173" t="s">
         <v>595</v>
       </c>
-      <c r="C26" s="173"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="172" t="s">
+      <c r="C26" s="174"/>
+      <c r="D26" s="174"/>
+      <c r="E26" s="173" t="s">
         <v>596</v>
       </c>
-      <c r="F26" s="173"/>
-      <c r="G26" s="172" t="s">
+      <c r="F26" s="174"/>
+      <c r="G26" s="173" t="s">
         <v>578</v>
       </c>
-      <c r="H26" s="172" t="s">
+      <c r="H26" s="173" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="172"/>
-      <c r="B27" s="174" t="s">
+      <c r="A27" s="173"/>
+      <c r="B27" s="175" t="s">
         <v>597</v>
       </c>
-      <c r="C27" s="173"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="176" t="s">
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="177" t="s">
         <v>578</v>
       </c>
-      <c r="H27" s="175"/>
+      <c r="H27" s="176"/>
     </row>
     <row r="28">
-      <c r="A28" s="172"/>
-      <c r="B28" s="177" t="s">
+      <c r="A28" s="173"/>
+      <c r="B28" s="178" t="s">
         <v>598</v>
       </c>
-      <c r="C28" s="173"/>
-      <c r="D28" s="172" t="s">
+      <c r="C28" s="174"/>
+      <c r="D28" s="173" t="s">
         <v>599</v>
       </c>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="180"/>
-      <c r="H28" s="178"/>
+      <c r="E28" s="174"/>
+      <c r="F28" s="174"/>
+      <c r="G28" s="181"/>
+      <c r="H28" s="179"/>
     </row>
     <row r="29">
-      <c r="A29" s="172"/>
-      <c r="B29" s="172"/>
-      <c r="C29" s="172"/>
-      <c r="D29" s="172"/>
-      <c r="E29" s="173"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="180"/>
-      <c r="H29" s="178"/>
+      <c r="A29" s="173"/>
+      <c r="B29" s="173"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="174"/>
+      <c r="F29" s="174"/>
+      <c r="G29" s="181"/>
+      <c r="H29" s="179"/>
     </row>
     <row r="30">
-      <c r="A30" s="172" t="s">
+      <c r="A30" s="173" t="s">
         <v>600</v>
       </c>
-      <c r="B30" s="172"/>
-      <c r="C30" s="173"/>
-      <c r="D30" s="173"/>
-      <c r="E30" s="173"/>
-      <c r="F30" s="173"/>
-      <c r="G30" s="173"/>
-      <c r="H30" s="178"/>
+      <c r="B30" s="173"/>
+      <c r="C30" s="174"/>
+      <c r="D30" s="174"/>
+      <c r="E30" s="174"/>
+      <c r="F30" s="174"/>
+      <c r="G30" s="174"/>
+      <c r="H30" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5339,105 +5345,105 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="181" t="str">
+      <c r="A2" s="182" t="str">
         <f>HYPERLINK("http://www.isg.rhul.ac.uk/tls/Lucky13.html","Lucky 13")</f>
         <v>Lucky 13</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
     </row>
     <row r="3">
-      <c r="A3" s="183" t="str">
+      <c r="A3" s="184" t="str">
         <f>HYPERLINK("https://nerdoholic.org/uploads/dergln/beast_part2/ssl_jun21.pdf","BEAST")</f>
         <v>BEAST</v>
       </c>
-      <c r="B3" s="182"/>
+      <c r="B3" s="183"/>
     </row>
     <row r="4">
-      <c r="A4" s="181" t="str">
+      <c r="A4" s="182" t="str">
         <f>HYPERLINK("https://sweet32.info/","Sweet32")</f>
         <v>Sweet32</v>
       </c>
-      <c r="D4" s="182"/>
+      <c r="D4" s="183"/>
     </row>
     <row r="5">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="185" t="s">
         <v>601</v>
       </c>
-      <c r="B5" s="182"/>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
+      <c r="B5" s="183"/>
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
     </row>
     <row r="6">
-      <c r="A6" s="181" t="str">
+      <c r="A6" s="182" t="str">
         <f>HYPERLINK("http://breachattack.com/","BREACH")</f>
         <v>BREACH</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="181" t="str">
+      <c r="A7" s="182" t="str">
         <f>HYPERLINK("https://security.googleblog.com/2014/10/this-poodle-bites-exploiting-ssl-30.html","POODLE")</f>
         <v>POODLE</v>
       </c>
-      <c r="B7" s="182"/>
-      <c r="D7" s="182"/>
+      <c r="B7" s="183"/>
+      <c r="D7" s="183"/>
     </row>
     <row r="8">
-      <c r="A8" s="181" t="str">
+      <c r="A8" s="182" t="str">
         <f>HYPERLINK("https://mitls.org/pages/attacks/3SHAKE","3SHAKE")</f>
         <v>3SHAKE</v>
       </c>
-      <c r="B8" s="182"/>
-      <c r="C8" s="182"/>
-      <c r="D8" s="182"/>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="183"/>
     </row>
     <row r="9">
-      <c r="A9" s="181" t="str">
+      <c r="A9" s="182" t="str">
         <f>HYPERLINK("https://drownattack.com/","DROWN")</f>
         <v>DROWN</v>
       </c>
-      <c r="D9" s="182"/>
+      <c r="D9" s="183"/>
     </row>
     <row r="10">
-      <c r="A10" s="181" t="str">
+      <c r="A10" s="182" t="str">
         <f>HYPERLINK("https://robotattack.org/","ROBOT ")</f>
         <v>ROBOT </v>
       </c>
-      <c r="B10" s="182"/>
-      <c r="D10" s="182"/>
+      <c r="B10" s="183"/>
+      <c r="D10" s="183"/>
     </row>
     <row r="11">
-      <c r="A11" s="181" t="str">
+      <c r="A11" s="182" t="str">
         <f>HYPERLINK("https://www.kb.cert.org/vuls/id/120541/","Renegotiation attack")</f>
         <v>Renegotiation attack</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="185" t="s">
+      <c r="A12" s="186" t="s">
         <v>602</v>
       </c>
-      <c r="D12" s="182"/>
+      <c r="D12" s="183"/>
     </row>
     <row r="13">
-      <c r="A13" s="185" t="s">
+      <c r="A13" s="186" t="s">
         <v>603</v>
       </c>
-      <c r="B13" s="182"/>
-      <c r="C13" s="182"/>
-      <c r="D13" s="182"/>
+      <c r="B13" s="183"/>
+      <c r="C13" s="183"/>
+      <c r="D13" s="183"/>
     </row>
     <row r="14">
-      <c r="A14" s="185" t="s">
+      <c r="A14" s="186" t="s">
         <v>604</v>
       </c>
-      <c r="D14" s="182"/>
+      <c r="D14" s="183"/>
     </row>
     <row r="15">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="186" t="s">
         <v>605</v>
       </c>
-      <c r="B15" s="182"/>
+      <c r="B15" s="183"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -27539,15 +27545,15 @@
       <c r="B2" s="110"/>
       <c r="C2" s="110"/>
       <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
+      <c r="E2" s="121"/>
       <c r="F2" s="113"/>
-      <c r="G2" s="121" t="s">
+      <c r="G2" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="121" t="s">
+      <c r="H2" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="122" t="s">
         <v>11</v>
       </c>
     </row>
@@ -27567,16 +27573,16 @@
       <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="123" t="s">
+      <c r="F3" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="124" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27596,16 +27602,16 @@
       <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="123" t="s">
+      <c r="F4" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="124" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27625,16 +27631,16 @@
       <c r="E5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="123" t="s">
+      <c r="F5" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="124" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27654,16 +27660,16 @@
       <c r="E6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="123" t="s">
+      <c r="F6" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="124" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27683,16 +27689,16 @@
       <c r="E7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="123" t="s">
+      <c r="F7" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="124" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27712,16 +27718,16 @@
       <c r="E8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="123" t="s">
+      <c r="F8" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="124" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27741,25 +27747,24 @@
       <c r="E9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="122" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="123" t="s">
+      <c r="F9" s="123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="124" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:I1"/>
@@ -27823,7 +27828,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>485</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -27850,22 +27855,22 @@
       <c r="A2" s="110"/>
       <c r="B2" s="110"/>
       <c r="C2" s="110"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126" t="s">
+      <c r="D2" s="126"/>
+      <c r="E2" s="127" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="125"/>
-      <c r="G2" s="127" t="s">
+      <c r="F2" s="126"/>
+      <c r="G2" s="128" t="s">
         <v>35</v>
       </c>
       <c r="H2" s="110"/>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="121" t="s">
+      <c r="J2" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="121" t="s">
+      <c r="K2" s="122" t="s">
         <v>11</v>
       </c>
     </row>
@@ -27886,7 +27891,7 @@
       <c r="F3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="128"/>
+      <c r="G3" s="129"/>
       <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
@@ -27919,7 +27924,7 @@
       <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="128" t="s">
+      <c r="G4" s="129" t="s">
         <v>489</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -27954,7 +27959,7 @@
       <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="128" t="s">
+      <c r="G5" s="129" t="s">
         <v>492</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -27989,7 +27994,7 @@
       <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="128" t="s">
+      <c r="G6" s="129" t="s">
         <v>495</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -28065,69 +28070,69 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>496</v>
       </c>
-      <c r="B1" s="129" t="s">
+      <c r="B1" s="130" t="s">
         <v>497</v>
       </c>
       <c r="C1" s="87" t="s">
         <v>498</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="132" t="s">
+      <c r="E1" s="132"/>
+      <c r="F1" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="131"/>
-      <c r="H1" s="132" t="s">
+      <c r="G1" s="132"/>
+      <c r="H1" s="133" t="s">
         <v>499</v>
       </c>
-      <c r="I1" s="131"/>
-      <c r="J1" s="132" t="s">
+      <c r="I1" s="132"/>
+      <c r="J1" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="133"/>
-      <c r="L1" s="134" t="s">
+      <c r="K1" s="134"/>
+      <c r="L1" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
     </row>
     <row r="2">
       <c r="A2" s="110"/>
       <c r="B2" s="110"/>
       <c r="C2" s="110"/>
       <c r="D2" s="113"/>
-      <c r="E2" s="131" t="s">
+      <c r="E2" s="132" t="s">
         <v>500</v>
       </c>
       <c r="F2" s="113"/>
-      <c r="G2" s="131" t="s">
+      <c r="G2" s="132" t="s">
         <v>500</v>
       </c>
       <c r="H2" s="113"/>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="132" t="s">
         <v>500</v>
       </c>
       <c r="J2" s="113"/>
-      <c r="K2" s="131" t="s">
+      <c r="K2" s="132" t="s">
         <v>500</v>
       </c>
-      <c r="L2" s="136" t="s">
+      <c r="L2" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="136" t="s">
+      <c r="M2" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="136" t="s">
+      <c r="N2" s="137" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="138" t="s">
         <v>501</v>
       </c>
       <c r="B3" s="100" t="s">
@@ -28139,17 +28144,17 @@
       <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="138" t="s">
+      <c r="E3" s="139" t="s">
         <v>502</v>
       </c>
-      <c r="F3" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="140"/>
-      <c r="H3" s="141" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="140"/>
+      <c r="F3" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="141"/>
+      <c r="H3" s="142" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="141"/>
       <c r="J3" s="23" t="s">
         <v>15</v>
       </c>
@@ -28171,19 +28176,19 @@
       <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="138" t="s">
+      <c r="E4" s="139" t="s">
         <v>503</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="140" t="s">
+      <c r="G4" s="141" t="s">
         <v>504</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="140" t="s">
+      <c r="I4" s="141" t="s">
         <v>504</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -28209,29 +28214,29 @@
       <c r="C5" s="25">
         <v>-1.0</v>
       </c>
-      <c r="D5" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="138"/>
-      <c r="F5" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="140"/>
-      <c r="H5" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="140"/>
-      <c r="J5" s="139" t="s">
+      <c r="D5" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="139"/>
+      <c r="F5" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="141"/>
+      <c r="H5" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="141"/>
+      <c r="J5" s="140" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="83"/>
-      <c r="L5" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="139" t="s">
+      <c r="L5" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="140" t="s">
         <v>15</v>
       </c>
     </row>
@@ -28245,17 +28250,17 @@
       <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="138" t="s">
+      <c r="E6" s="139" t="s">
         <v>502</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="140"/>
+      <c r="G6" s="141"/>
       <c r="H6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="140"/>
+      <c r="I6" s="141"/>
       <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
@@ -28277,19 +28282,19 @@
       <c r="D7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="138" t="s">
+      <c r="E7" s="139" t="s">
         <v>503</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="140" t="s">
+      <c r="G7" s="141" t="s">
         <v>504</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="140" t="s">
+      <c r="I7" s="141" t="s">
         <v>504</v>
       </c>
       <c r="J7" s="23" t="s">
@@ -28316,19 +28321,19 @@
       <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="138" t="s">
+      <c r="E8" s="139" t="s">
         <v>502</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="140" t="s">
+      <c r="G8" s="141" t="s">
         <v>442</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="140"/>
+      <c r="I8" s="141"/>
       <c r="J8" s="11" t="s">
         <v>18</v>
       </c>
@@ -28352,19 +28357,19 @@
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="138" t="s">
+      <c r="E9" s="139" t="s">
         <v>503</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="140" t="s">
+      <c r="G9" s="141" t="s">
         <v>504</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="140" t="s">
+      <c r="I9" s="141" t="s">
         <v>504</v>
       </c>
       <c r="J9" s="23" t="s">
@@ -28385,18 +28390,18 @@
       <c r="C10" s="25">
         <v>1024.0</v>
       </c>
-      <c r="D10" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="140"/>
-      <c r="F10" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="140"/>
-      <c r="H10" s="141" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="140"/>
+      <c r="D10" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="141"/>
+      <c r="F10" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="141"/>
+      <c r="H10" s="142" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="141"/>
       <c r="J10" s="23" t="s">
         <v>15</v>
       </c>
@@ -28412,7 +28417,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="138" t="s">
         <v>506</v>
       </c>
       <c r="B11" s="100" t="s">
@@ -28421,18 +28426,18 @@
       <c r="C11" s="25">
         <v>224.0</v>
       </c>
-      <c r="D11" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="140"/>
-      <c r="F11" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="140"/>
-      <c r="H11" s="141" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="140"/>
+      <c r="D11" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="141"/>
+      <c r="F11" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="141"/>
+      <c r="H11" s="142" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="141"/>
       <c r="J11" s="23" t="s">
         <v>15</v>
       </c>
@@ -28451,20 +28456,20 @@
       <c r="C12" s="25">
         <v>256.0</v>
       </c>
-      <c r="D12" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="140"/>
+      <c r="D12" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="141"/>
       <c r="F12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="140" t="s">
+      <c r="G12" s="141" t="s">
         <v>504</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="140" t="s">
+      <c r="I12" s="141" t="s">
         <v>504</v>
       </c>
       <c r="J12" s="23" t="s">
@@ -28488,26 +28493,26 @@
       <c r="C13" s="25">
         <v>1024.0</v>
       </c>
-      <c r="D13" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="140"/>
-      <c r="F13" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="140"/>
-      <c r="H13" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="140"/>
-      <c r="J13" s="139" t="s">
+      <c r="D13" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="141"/>
+      <c r="F13" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="141"/>
+      <c r="H13" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="141"/>
+      <c r="J13" s="140" t="s">
         <v>15</v>
       </c>
       <c r="K13" s="23"/>
-      <c r="L13" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" s="139" t="s">
+      <c r="L13" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="140" t="s">
         <v>15</v>
       </c>
       <c r="N13" s="7" t="s">
@@ -28518,18 +28523,18 @@
       <c r="C14" s="25">
         <v>2048.0</v>
       </c>
-      <c r="D14" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="140"/>
+      <c r="D14" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="141"/>
       <c r="F14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="140"/>
+      <c r="G14" s="141"/>
       <c r="H14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="140"/>
+      <c r="I14" s="141"/>
       <c r="J14" s="23" t="s">
         <v>15</v>
       </c>
@@ -28548,20 +28553,20 @@
       <c r="C15" s="25">
         <v>3076.0</v>
       </c>
-      <c r="D15" s="139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="140"/>
+      <c r="D15" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="141"/>
       <c r="F15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="140" t="s">
+      <c r="G15" s="141" t="s">
         <v>504</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="140" t="s">
+      <c r="I15" s="141" t="s">
         <v>504</v>
       </c>
       <c r="J15" s="23" t="s">
@@ -28650,18 +28655,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>509</v>
       </c>
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="144" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="110"/>
-      <c r="D1" s="143" t="s">
+      <c r="D1" s="144" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="110"/>
-      <c r="F1" s="143" t="s">
+      <c r="F1" s="144" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="110"/>
@@ -28670,111 +28675,111 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="144"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="145" t="s">
+      <c r="C2" s="146" t="s">
         <v>511</v>
       </c>
-      <c r="D2" s="146"/>
-      <c r="E2" s="145" t="s">
+      <c r="D2" s="147"/>
+      <c r="E2" s="146" t="s">
         <v>511</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="147" t="s">
+      <c r="G2" s="148" t="s">
         <v>511</v>
       </c>
-      <c r="H2" s="148"/>
+      <c r="H2" s="149"/>
     </row>
     <row r="3">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="146" t="s">
         <v>512</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="146" t="s">
         <v>513</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="144"/>
+      <c r="E3" s="145"/>
       <c r="F3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="149"/>
+      <c r="G3" s="150"/>
       <c r="H3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="150" t="s">
+      <c r="A4" s="151" t="s">
         <v>514</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="152" t="s">
         <v>515</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="151" t="s">
+      <c r="E4" s="152" t="s">
         <v>516</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="149"/>
+      <c r="G4" s="150"/>
       <c r="H4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="146" t="s">
         <v>517</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="152" t="s">
         <v>518</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="151" t="s">
+      <c r="E5" s="152" t="s">
         <v>519</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="149"/>
+      <c r="G5" s="150"/>
       <c r="H5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="145" t="s">
+      <c r="A6" s="146" t="s">
         <v>520</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="152" t="s">
         <v>521</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="151" t="s">
+      <c r="E6" s="152" t="s">
         <v>522</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="149"/>
+      <c r="G6" s="150"/>
       <c r="H6" s="12" t="s">
         <v>15</v>
       </c>

</xml_diff>